<commit_message>
A few more data points
git-svn-id: svn+ssh://software-srn.sandia.gov/svn/mapreduce/trunk@607 3fc257bb-8550-0410-81b3-a5c103da83f7
</commit_message>
<xml_diff>
--- a/paper/results.xlsx
+++ b/paper/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-160" yWindow="200" windowWidth="34400" windowHeight="21100" tabRatio="500"/>
+    <workbookView xWindow="6400" yWindow="-420" windowWidth="21600" windowHeight="13380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
     <definedName name="jj_1" localSheetId="0">Sheet1!$G$41:$H$64</definedName>
     <definedName name="jjj" localSheetId="0">Sheet1!$M$15:$N$84</definedName>
   </definedNames>
-  <calcPr calcId="130407" concurrentCalc="0"/>
+  <calcPr calcId="130406" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
@@ -45,74 +45,74 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="17">
   <si>
     <t>RMAT Generation</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>All runs on odin, pernode mode</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Number of Processors</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>R-MAT 20</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>R-MAT 24</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>R-MAT 28</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>R-MAT 32</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>PageRank</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve"> </t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve"> </t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve"> </t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve"> </t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>SSSP</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve"> </t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve"> </t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>BOLD VALUES are updated to include only edge generation time.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>BOLD TIMES have 0.002 tolerance</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -125,8 +125,18 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="5">
     <font>
+      <sz val="10"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <i/>
       <sz val="10"/>
       <name val="Verdana"/>
     </font>
@@ -160,9 +170,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -178,11 +190,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="jj_1" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="jj" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="jj" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="jj_1" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -505,10 +517,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:Q84"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="Q55" sqref="Q55"/>
+    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -593,13 +606,13 @@
       <c r="A5">
         <v>1</v>
       </c>
-      <c r="B5" s="1">
-        <f>AVERAGE(B15:B17)</f>
-        <v>117.78133333333334</v>
-      </c>
-      <c r="C5" s="1">
-        <f>AVERAGE(C15:C17)</f>
-        <v>3413.29</v>
+      <c r="B5" s="3">
+        <f>AVERAGE(B45:B49)</f>
+        <v>77.772759999999991</v>
+      </c>
+      <c r="C5" s="3">
+        <f>AVERAGE(C45:C49)</f>
+        <v>1721.3100000000002</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
@@ -638,13 +651,13 @@
       <c r="A6">
         <v>2</v>
       </c>
-      <c r="B6" s="1">
-        <f>AVERAGE(B18:B20)</f>
-        <v>65.872466666666668</v>
-      </c>
-      <c r="C6" s="1">
-        <f>AVERAGE(C18:C20)</f>
-        <v>1544.175</v>
+      <c r="B6" s="3">
+        <f>AVERAGE(B50:B54)</f>
+        <v>31.010299999999994</v>
+      </c>
+      <c r="C6" s="3">
+        <f>AVERAGE(C50:C54)</f>
+        <v>648.01340000000005</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -691,8 +704,9 @@
         <f>AVERAGE(C21:C23)</f>
         <v>614.31700000000001</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>9</v>
+      <c r="D7" s="1">
+        <f>AVERAGE(D21:D23)</f>
+        <v>15524.5</v>
       </c>
       <c r="E7" s="1"/>
       <c r="G7">
@@ -829,7 +843,7 @@
       </c>
       <c r="D10" s="1">
         <f>AVERAGE(D30:D32)</f>
-        <v>3600.81</v>
+        <v>2970.46</v>
       </c>
       <c r="E10" s="1"/>
       <c r="G10">
@@ -876,7 +890,7 @@
       </c>
       <c r="D11" s="1">
         <f>AVERAGE(D33:D35)</f>
-        <v>1199.0533333333333</v>
+        <v>1296.2333333333333</v>
       </c>
       <c r="E11" s="1"/>
       <c r="G11">
@@ -884,15 +898,15 @@
       </c>
       <c r="H11" s="1">
         <f>AVERAGE(H33:H35)</f>
-        <v>0.17804277777777777</v>
+        <v>0.16751722222222223</v>
       </c>
       <c r="I11" s="1">
         <f>AVERAGE(I33:I35)</f>
-        <v>5.7829435897435895</v>
+        <v>4.9898277777777782</v>
       </c>
       <c r="J11" s="1">
         <f>AVERAGE(J33:J35)</f>
-        <v>982.71857142857152</v>
+        <v>963.14857142857147</v>
       </c>
       <c r="K11" s="1"/>
       <c r="M11">
@@ -1129,6 +1143,9 @@
       <c r="C21">
         <v>571.48199999999997</v>
       </c>
+      <c r="D21" s="4">
+        <v>15524.5</v>
+      </c>
       <c r="G21">
         <v>4</v>
       </c>
@@ -1317,6 +1334,10 @@
         <f t="shared" si="0"/>
         <v>48.247769230769229</v>
       </c>
+      <c r="J27">
+        <f>J53/5</f>
+        <v>2005.94</v>
+      </c>
       <c r="M27">
         <v>2</v>
       </c>
@@ -1399,8 +1420,8 @@
       <c r="C30">
         <v>111.245</v>
       </c>
-      <c r="D30">
-        <v>3600.81</v>
+      <c r="D30" s="4">
+        <v>2970.46</v>
       </c>
       <c r="G30">
         <v>32</v>
@@ -1510,12 +1531,12 @@
         <v>64</v>
       </c>
       <c r="H33">
-        <f t="shared" si="1"/>
-        <v>0.17129166666666665</v>
+        <f>H59/6</f>
+        <v>0.16703666666666669</v>
       </c>
       <c r="I33">
-        <f t="shared" si="0"/>
-        <v>5.6947538461538461</v>
+        <f>I59/6</f>
+        <v>5.7520500000000006</v>
       </c>
       <c r="J33">
         <f>J59/14</f>
@@ -1548,16 +1569,16 @@
         <v>64</v>
       </c>
       <c r="H34">
-        <f t="shared" si="1"/>
-        <v>0.19192500000000001</v>
+        <f>H60/6</f>
+        <v>0.16784333333333334</v>
       </c>
       <c r="I34">
-        <f t="shared" si="0"/>
-        <v>5.9638538461538468</v>
+        <f>I60/6</f>
+        <v>4.4872833333333331</v>
       </c>
       <c r="J34">
-        <f>J60/14</f>
-        <v>1000.6999999999999</v>
+        <f>J60/5</f>
+        <v>941.99</v>
       </c>
       <c r="M34">
         <v>2</v>
@@ -1579,19 +1600,19 @@
       <c r="C35" s="2">
         <v>22.258600000000001</v>
       </c>
-      <c r="D35">
-        <v>947.87</v>
+      <c r="D35" s="4">
+        <v>1239.4100000000001</v>
       </c>
       <c r="G35">
         <v>64</v>
       </c>
       <c r="H35">
-        <f t="shared" si="1"/>
-        <v>0.17091166666666668</v>
+        <f>H61/6</f>
+        <v>0.16767166666666666</v>
       </c>
       <c r="I35">
-        <f t="shared" si="0"/>
-        <v>5.6902230769230764</v>
+        <f>I61/6</f>
+        <v>4.7301500000000001</v>
       </c>
       <c r="J35">
         <f>J61/5</f>
@@ -1712,6 +1733,9 @@
       </c>
     </row>
     <row r="40" spans="1:15">
+      <c r="B40" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="M40">
         <v>4</v>
       </c>
@@ -1766,9 +1790,6 @@
       <c r="A43" t="s">
         <v>8</v>
       </c>
-      <c r="B43" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="G43">
         <v>1</v>
       </c>
@@ -1809,6 +1830,15 @@
       </c>
     </row>
     <row r="45" spans="1:15">
+      <c r="A45">
+        <v>1</v>
+      </c>
+      <c r="B45">
+        <v>79.586600000000004</v>
+      </c>
+      <c r="C45">
+        <v>1663.96</v>
+      </c>
       <c r="G45">
         <v>2</v>
       </c>
@@ -1829,6 +1859,15 @@
       </c>
     </row>
     <row r="46" spans="1:15">
+      <c r="A46">
+        <v>1</v>
+      </c>
+      <c r="B46">
+        <v>79.441599999999994</v>
+      </c>
+      <c r="C46">
+        <v>1605.35</v>
+      </c>
       <c r="G46">
         <v>2</v>
       </c>
@@ -1849,6 +1888,15 @@
       </c>
     </row>
     <row r="47" spans="1:15">
+      <c r="A47">
+        <v>1</v>
+      </c>
+      <c r="B47">
+        <v>81.992699999999999</v>
+      </c>
+      <c r="C47">
+        <v>1894.62</v>
+      </c>
       <c r="G47">
         <v>4</v>
       </c>
@@ -1869,6 +1917,12 @@
       </c>
     </row>
     <row r="48" spans="1:15">
+      <c r="A48">
+        <v>1</v>
+      </c>
+      <c r="B48">
+        <v>67.202399999999997</v>
+      </c>
       <c r="G48">
         <v>4</v>
       </c>
@@ -1888,7 +1942,13 @@
         <v>416.49299999999999</v>
       </c>
     </row>
-    <row r="49" spans="7:15">
+    <row r="49" spans="1:15">
+      <c r="A49">
+        <v>1</v>
+      </c>
+      <c r="B49">
+        <v>80.640500000000003</v>
+      </c>
       <c r="G49">
         <v>4</v>
       </c>
@@ -1908,7 +1968,16 @@
         <v>414.233</v>
       </c>
     </row>
-    <row r="50" spans="7:15">
+    <row r="50" spans="1:15">
+      <c r="A50">
+        <v>2</v>
+      </c>
+      <c r="B50">
+        <v>33.642000000000003</v>
+      </c>
+      <c r="C50">
+        <v>649.19600000000003</v>
+      </c>
       <c r="G50">
         <v>8</v>
       </c>
@@ -1928,7 +1997,16 @@
         <v>404.476</v>
       </c>
     </row>
-    <row r="51" spans="7:15">
+    <row r="51" spans="1:15">
+      <c r="A51">
+        <v>2</v>
+      </c>
+      <c r="B51">
+        <v>34.658299999999997</v>
+      </c>
+      <c r="C51">
+        <v>623.91</v>
+      </c>
       <c r="G51">
         <v>8</v>
       </c>
@@ -1948,7 +2026,16 @@
         <v>402.28399999999999</v>
       </c>
     </row>
-    <row r="52" spans="7:15">
+    <row r="52" spans="1:15">
+      <c r="A52">
+        <v>2</v>
+      </c>
+      <c r="B52">
+        <v>28.674499999999998</v>
+      </c>
+      <c r="C52">
+        <v>618.76800000000003</v>
+      </c>
       <c r="G52">
         <v>8</v>
       </c>
@@ -1968,7 +2055,16 @@
         <v>401.87599999999998</v>
       </c>
     </row>
-    <row r="53" spans="7:15">
+    <row r="53" spans="1:15">
+      <c r="A53">
+        <v>2</v>
+      </c>
+      <c r="B53">
+        <v>28.255500000000001</v>
+      </c>
+      <c r="C53">
+        <v>712.03899999999999</v>
+      </c>
       <c r="G53">
         <v>16</v>
       </c>
@@ -1978,8 +2074,8 @@
       <c r="I53">
         <v>627.221</v>
       </c>
-      <c r="J53" t="s">
-        <v>8</v>
+      <c r="J53" s="4">
+        <v>10029.700000000001</v>
       </c>
       <c r="M53">
         <v>8</v>
@@ -1991,7 +2087,16 @@
         <v>382.67399999999998</v>
       </c>
     </row>
-    <row r="54" spans="7:15">
+    <row r="54" spans="1:15">
+      <c r="A54">
+        <v>2</v>
+      </c>
+      <c r="B54">
+        <v>29.821200000000001</v>
+      </c>
+      <c r="C54">
+        <v>636.154</v>
+      </c>
       <c r="G54">
         <v>16</v>
       </c>
@@ -2011,7 +2116,7 @@
         <v>439.31099999999998</v>
       </c>
     </row>
-    <row r="55" spans="7:15">
+    <row r="55" spans="1:15">
       <c r="G55">
         <v>16</v>
       </c>
@@ -2031,7 +2136,7 @@
         <v>443.43700000000001</v>
       </c>
     </row>
-    <row r="56" spans="7:15">
+    <row r="56" spans="1:15">
       <c r="G56">
         <v>32</v>
       </c>
@@ -2054,7 +2159,7 @@
         <v>394.49599999999998</v>
       </c>
     </row>
-    <row r="57" spans="7:15">
+    <row r="57" spans="1:15">
       <c r="G57">
         <v>32</v>
       </c>
@@ -2080,7 +2185,7 @@
         <v>379.82600000000002</v>
       </c>
     </row>
-    <row r="58" spans="7:15">
+    <row r="58" spans="1:15">
       <c r="G58">
         <v>32</v>
       </c>
@@ -2100,15 +2205,15 @@
         <v>472.43400000000003</v>
       </c>
     </row>
-    <row r="59" spans="7:15">
+    <row r="59" spans="1:15">
       <c r="G59">
         <v>64</v>
       </c>
-      <c r="H59">
-        <v>2.0554999999999999</v>
-      </c>
-      <c r="I59">
-        <v>74.031800000000004</v>
+      <c r="H59" s="4">
+        <v>1.0022200000000001</v>
+      </c>
+      <c r="I59" s="4">
+        <v>34.512300000000003</v>
       </c>
       <c r="J59">
         <v>13892.7</v>
@@ -2123,18 +2228,18 @@
         <v>426.74599999999998</v>
       </c>
     </row>
-    <row r="60" spans="7:15">
+    <row r="60" spans="1:15">
       <c r="G60">
         <v>64</v>
       </c>
-      <c r="H60">
-        <v>2.3031000000000001</v>
-      </c>
-      <c r="I60">
-        <v>77.530100000000004</v>
-      </c>
-      <c r="J60">
-        <v>14009.8</v>
+      <c r="H60" s="4">
+        <v>1.0070600000000001</v>
+      </c>
+      <c r="I60" s="4">
+        <v>26.9237</v>
+      </c>
+      <c r="J60" s="4">
+        <v>4709.95</v>
       </c>
       <c r="M60">
         <v>16</v>
@@ -2146,15 +2251,15 @@
         <v>427.02199999999999</v>
       </c>
     </row>
-    <row r="61" spans="7:15">
+    <row r="61" spans="1:15">
       <c r="G61">
         <v>64</v>
       </c>
-      <c r="H61">
-        <v>2.0509400000000002</v>
-      </c>
-      <c r="I61">
-        <v>73.972899999999996</v>
+      <c r="H61" s="4">
+        <v>1.00603</v>
+      </c>
+      <c r="I61" s="4">
+        <v>28.3809</v>
       </c>
       <c r="J61" s="2">
         <v>4775.6000000000004</v>
@@ -2169,7 +2274,7 @@
         <v>353.012</v>
       </c>
     </row>
-    <row r="62" spans="7:15">
+    <row r="62" spans="1:15">
       <c r="G62">
         <v>124</v>
       </c>
@@ -2189,7 +2294,7 @@
         <v>459.416</v>
       </c>
     </row>
-    <row r="63" spans="7:15">
+    <row r="63" spans="1:15">
       <c r="G63">
         <v>124</v>
       </c>
@@ -2209,7 +2314,7 @@
         <v>463.56299999999999</v>
       </c>
     </row>
-    <row r="64" spans="7:15">
+    <row r="64" spans="1:15">
       <c r="G64">
         <v>124</v>
       </c>
@@ -2450,7 +2555,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>

<commit_message>
Minor changes to paper.  Some new results.
git-svn-id: svn+ssh://software-srn.sandia.gov/svn/mapreduce/trunk@608 3fc257bb-8550-0410-81b3-a5c103da83f7
</commit_message>
<xml_diff>
--- a/paper/results.xlsx
+++ b/paper/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6400" yWindow="-420" windowWidth="21600" windowHeight="13380" tabRatio="500"/>
+    <workbookView xWindow="360" yWindow="-420" windowWidth="23240" windowHeight="21660" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
     <definedName name="jj_1" localSheetId="0">Sheet1!$G$41:$H$64</definedName>
     <definedName name="jjj" localSheetId="0">Sheet1!$M$15:$N$84</definedName>
   </definedNames>
-  <calcPr calcId="130406" concurrentCalc="0"/>
+  <calcPr calcId="130407" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
@@ -45,88 +45,103 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="18">
   <si>
     <t>RMAT Generation</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>All runs on odin, pernode mode</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>Number of Processors</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>R-MAT 20</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>R-MAT 24</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>R-MAT 28</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>R-MAT 32</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>PageRank</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve"> </t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve"> </t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve"> </t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve"> </t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>SSSP</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>BOLD VALUES are updated to include only edge generation time.</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>BOLD TIMES have 0.002 tolerance</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>ORIG ALG</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>R-MAT 24</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Times per iteration</t>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="0.00"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
+      <sz val="10"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <i/>
       <sz val="10"/>
       <name val="Verdana"/>
     </font>
@@ -170,11 +185,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -190,11 +208,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="jj" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="jj_1" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="jj_1" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="jj" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -517,11 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:Q84"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -551,8 +568,16 @@
       <c r="G2" t="s">
         <v>1</v>
       </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
       <c r="M2" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="F3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -571,6 +596,9 @@
       <c r="E4" t="s">
         <v>6</v>
       </c>
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
       <c r="G4" t="s">
         <v>2</v>
       </c>
@@ -606,18 +634,23 @@
       <c r="A5">
         <v>1</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="4">
         <f>AVERAGE(B45:B49)</f>
         <v>77.772759999999991</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="4">
         <f>AVERAGE(C45:C49)</f>
-        <v>1721.3100000000002</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="1"/>
+        <v>1665.6020000000001</v>
+      </c>
+      <c r="D5" s="4" t="e">
+        <f>AVERAGE(D45:D49)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E5" s="5"/>
+      <c r="F5" s="4">
+        <f>AVERAGE(F45:F49)</f>
+        <v>1726.4380000000001</v>
+      </c>
       <c r="G5">
         <v>1</v>
       </c>
@@ -651,18 +684,23 @@
       <c r="A6">
         <v>2</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="4">
         <f>AVERAGE(B50:B54)</f>
         <v>31.010299999999994</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="6">
         <f>AVERAGE(C50:C54)</f>
         <v>648.01340000000005</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="1"/>
+      <c r="D6" s="6">
+        <f>AVERAGE(D50:D54)</f>
+        <v>17422.400000000001</v>
+      </c>
+      <c r="E6" s="5"/>
+      <c r="F6" s="6">
+        <f>AVERAGE(F50:F54)</f>
+        <v>680.96640000000002</v>
+      </c>
       <c r="G6">
         <v>2</v>
       </c>
@@ -696,19 +734,23 @@
       <c r="A7">
         <v>4</v>
       </c>
-      <c r="B7" s="1">
-        <f>AVERAGE(B21:B23)</f>
-        <v>26.420766666666669</v>
-      </c>
-      <c r="C7" s="1">
-        <f>AVERAGE(C21:C23)</f>
-        <v>614.31700000000001</v>
-      </c>
-      <c r="D7" s="1">
-        <f>AVERAGE(D21:D23)</f>
-        <v>15524.5</v>
-      </c>
-      <c r="E7" s="1"/>
+      <c r="B7" s="6">
+        <f>AVERAGE(B55:B59)</f>
+        <v>12.74222</v>
+      </c>
+      <c r="C7" s="6">
+        <f>AVERAGE(C55:C59)</f>
+        <v>333.67740000000003</v>
+      </c>
+      <c r="D7" s="6">
+        <f>AVERAGE(D55:D59)</f>
+        <v>8961.0066666666662</v>
+      </c>
+      <c r="E7" s="5"/>
+      <c r="F7" s="6">
+        <f>AVERAGE(F55:F59)</f>
+        <v>368.64599999999996</v>
+      </c>
       <c r="G7">
         <v>4</v>
       </c>
@@ -742,18 +784,23 @@
       <c r="A8">
         <v>8</v>
       </c>
-      <c r="B8" s="1">
-        <f>AVERAGE(B24:B26)</f>
-        <v>10.275106666666666</v>
-      </c>
-      <c r="C8" s="1">
-        <f>AVERAGE(C24:C26)</f>
-        <v>326.91433333333333</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="1"/>
+      <c r="B8" s="6">
+        <f>AVERAGE(B60:B64)</f>
+        <v>5.5719900000000004</v>
+      </c>
+      <c r="C8" s="6">
+        <f>AVERAGE(C60:C64)</f>
+        <v>290.37060000000008</v>
+      </c>
+      <c r="D8" s="6">
+        <f>AVERAGE(D60:D64)</f>
+        <v>10185.300000000001</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="6">
+        <f>AVERAGE(F60:F64)</f>
+        <v>194.54080000000002</v>
+      </c>
       <c r="G8">
         <v>8</v>
       </c>
@@ -787,19 +834,23 @@
       <c r="A9">
         <v>16</v>
       </c>
-      <c r="B9" s="1">
-        <f>AVERAGE(B27:B29)</f>
-        <v>5.9819866666666668</v>
-      </c>
-      <c r="C9" s="1">
-        <f>AVERAGE(C27:C29)</f>
-        <v>165.17966666666666</v>
-      </c>
-      <c r="D9" s="1">
-        <f>AVERAGE(D27:D29)</f>
-        <v>3818.05</v>
-      </c>
-      <c r="E9" s="1"/>
+      <c r="B9" s="6">
+        <f>AVERAGE(B65:B69)</f>
+        <v>3.1590979999999997</v>
+      </c>
+      <c r="C9" s="6">
+        <f>AVERAGE(C65:C69)</f>
+        <v>180.2516</v>
+      </c>
+      <c r="D9" s="6">
+        <f>AVERAGE(D65:D69)</f>
+        <v>4896.6550000000007</v>
+      </c>
+      <c r="E9" s="5"/>
+      <c r="F9" s="6">
+        <f>AVERAGE(F65:F69)</f>
+        <v>199.28340000000003</v>
+      </c>
       <c r="G9">
         <v>16</v>
       </c>
@@ -811,8 +862,9 @@
         <f>AVERAGE(I27:I29)</f>
         <v>45.144256410256411</v>
       </c>
-      <c r="J9" s="1" t="s">
-        <v>14</v>
+      <c r="J9" s="1">
+        <f>AVERAGE(J27:J29)</f>
+        <v>2005.3</v>
       </c>
       <c r="K9" s="1"/>
       <c r="M9">
@@ -833,25 +885,29 @@
       <c r="A10">
         <v>32</v>
       </c>
-      <c r="B10" s="1">
-        <f>AVERAGE(B30:B32)</f>
-        <v>5.0002333333333331</v>
-      </c>
-      <c r="C10" s="1">
-        <f>AVERAGE(C30:C32)</f>
-        <v>126.13833333333332</v>
-      </c>
-      <c r="D10" s="1">
-        <f>AVERAGE(D30:D32)</f>
-        <v>2970.46</v>
-      </c>
-      <c r="E10" s="1"/>
+      <c r="B10" s="6">
+        <f>AVERAGE(B70:B74)</f>
+        <v>2.1852</v>
+      </c>
+      <c r="C10" s="6">
+        <f>AVERAGE(C70:C74)</f>
+        <v>72.055959999999999</v>
+      </c>
+      <c r="D10" s="6">
+        <f>AVERAGE(D70:D74)</f>
+        <v>1843.2800000000002</v>
+      </c>
+      <c r="E10" s="5"/>
+      <c r="F10" s="6">
+        <f>AVERAGE(F70:F74)</f>
+        <v>90.752319999999997</v>
+      </c>
       <c r="G10">
         <v>32</v>
       </c>
       <c r="H10" s="1">
         <f>AVERAGE(H30:H32)</f>
-        <v>0.52386361111111113</v>
+        <v>0.33328555555555556</v>
       </c>
       <c r="I10" s="1">
         <f>AVERAGE(I30:I32)</f>
@@ -859,7 +915,7 @@
       </c>
       <c r="J10" s="1">
         <f>AVERAGE(J30:J32)</f>
-        <v>2159.2357142857145</v>
+        <v>2006.79</v>
       </c>
       <c r="K10" s="1"/>
       <c r="M10">
@@ -880,19 +936,23 @@
       <c r="A11">
         <v>64</v>
       </c>
-      <c r="B11" s="1">
-        <f>AVERAGE(B33:B35)</f>
-        <v>2.1078266666666665</v>
-      </c>
-      <c r="C11" s="1">
-        <f>AVERAGE(C33:C35)</f>
-        <v>25.374666666666666</v>
-      </c>
-      <c r="D11" s="1">
-        <f>AVERAGE(D33:D35)</f>
-        <v>1296.2333333333333</v>
-      </c>
-      <c r="E11" s="1"/>
+      <c r="B11" s="6">
+        <f>AVERAGE(B75:B79)</f>
+        <v>1.7162280000000003</v>
+      </c>
+      <c r="C11" s="6">
+        <f>AVERAGE(C75:C79)</f>
+        <v>15.513859999999999</v>
+      </c>
+      <c r="D11" s="6">
+        <f>AVERAGE(D75:D79)</f>
+        <v>808.01980000000003</v>
+      </c>
+      <c r="E11" s="5"/>
+      <c r="F11" s="6">
+        <f>AVERAGE(F75:F79)</f>
+        <v>14.404679999999999</v>
+      </c>
       <c r="G11">
         <v>64</v>
       </c>
@@ -906,7 +966,7 @@
       </c>
       <c r="J11" s="1">
         <f>AVERAGE(J33:J35)</f>
-        <v>963.14857142857147</v>
+        <v>942.84133333333341</v>
       </c>
       <c r="K11" s="1"/>
       <c r="M11">
@@ -927,18 +987,19 @@
       <c r="A12">
         <v>124</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="5">
         <f>AVERAGE(B36:B38)</f>
         <v>3.230116666666667</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="5">
         <f>AVERAGE(C36:C38)</f>
         <v>14.657500000000001</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="1"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
       <c r="G12">
         <v>124</v>
       </c>
@@ -1143,7 +1204,7 @@
       <c r="C21">
         <v>571.48199999999997</v>
       </c>
-      <c r="D21" s="4">
+      <c r="D21" s="3">
         <v>15524.5</v>
       </c>
       <c r="G21">
@@ -1369,6 +1430,10 @@
         <f t="shared" si="0"/>
         <v>44.930384615384618</v>
       </c>
+      <c r="J28">
+        <f>J54/5</f>
+        <v>2004.6599999999999</v>
+      </c>
       <c r="M28">
         <v>2</v>
       </c>
@@ -1420,23 +1485,23 @@
       <c r="C30">
         <v>111.245</v>
       </c>
-      <c r="D30" s="4">
+      <c r="D30" s="3">
         <v>2970.46</v>
       </c>
       <c r="G30">
         <v>32</v>
       </c>
       <c r="H30">
-        <f t="shared" si="1"/>
-        <v>0.55256749999999999</v>
+        <f>H56/6</f>
+        <v>0.33262666666666668</v>
       </c>
       <c r="I30">
         <f t="shared" si="0"/>
         <v>38.402846153846156</v>
       </c>
       <c r="J30">
-        <f>J56/14</f>
-        <v>2304.1214285714286</v>
+        <f>J56/5</f>
+        <v>2004.1</v>
       </c>
       <c r="M30">
         <v>2</v>
@@ -1462,16 +1527,16 @@
         <v>32</v>
       </c>
       <c r="H31">
-        <f t="shared" si="1"/>
-        <v>0.51017499999999993</v>
+        <f>H57/6</f>
+        <v>0.33597000000000005</v>
       </c>
       <c r="I31">
         <f t="shared" si="0"/>
         <v>35.460615384615387</v>
       </c>
       <c r="J31">
-        <f>J57/14</f>
-        <v>2014.3500000000001</v>
+        <f>J57/5</f>
+        <v>2009.48</v>
       </c>
       <c r="M31">
         <v>2</v>
@@ -1497,8 +1562,8 @@
         <v>32</v>
       </c>
       <c r="H32">
-        <f t="shared" si="1"/>
-        <v>0.50884833333333335</v>
+        <f>H58/6</f>
+        <v>0.33126</v>
       </c>
       <c r="I32">
         <f t="shared" si="0"/>
@@ -1531,16 +1596,16 @@
         <v>64</v>
       </c>
       <c r="H33">
-        <f>H59/6</f>
+        <f t="shared" ref="H33:I35" si="2">H59/6</f>
         <v>0.16703666666666669</v>
       </c>
       <c r="I33">
-        <f>I59/6</f>
+        <f t="shared" si="2"/>
         <v>5.7520500000000006</v>
       </c>
       <c r="J33">
-        <f>J59/14</f>
-        <v>992.33571428571429</v>
+        <f>J59/5</f>
+        <v>931.41399999999999</v>
       </c>
       <c r="M33">
         <v>2</v>
@@ -1569,11 +1634,11 @@
         <v>64</v>
       </c>
       <c r="H34">
-        <f>H60/6</f>
+        <f t="shared" si="2"/>
         <v>0.16784333333333334</v>
       </c>
       <c r="I34">
-        <f>I60/6</f>
+        <f t="shared" si="2"/>
         <v>4.4872833333333331</v>
       </c>
       <c r="J34">
@@ -1600,18 +1665,18 @@
       <c r="C35" s="2">
         <v>22.258600000000001</v>
       </c>
-      <c r="D35" s="4">
+      <c r="D35" s="3">
         <v>1239.4100000000001</v>
       </c>
       <c r="G35">
         <v>64</v>
       </c>
       <c r="H35">
-        <f>H61/6</f>
+        <f t="shared" si="2"/>
         <v>0.16767166666666666</v>
       </c>
       <c r="I35">
-        <f>I61/6</f>
+        <f t="shared" si="2"/>
         <v>4.7301500000000001</v>
       </c>
       <c r="J35">
@@ -1734,7 +1799,7 @@
     </row>
     <row r="40" spans="1:15">
       <c r="B40" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="M40">
         <v>4</v>
@@ -1839,6 +1904,9 @@
       <c r="C45">
         <v>1663.96</v>
       </c>
+      <c r="F45">
+        <v>1689.5</v>
+      </c>
       <c r="G45">
         <v>2</v>
       </c>
@@ -1868,6 +1936,9 @@
       <c r="C46">
         <v>1605.35</v>
       </c>
+      <c r="F46">
+        <v>1662.66</v>
+      </c>
       <c r="G46">
         <v>2</v>
       </c>
@@ -1897,6 +1968,9 @@
       <c r="C47">
         <v>1894.62</v>
       </c>
+      <c r="F47">
+        <v>1976.78</v>
+      </c>
       <c r="G47">
         <v>4</v>
       </c>
@@ -1923,6 +1997,12 @@
       <c r="B48">
         <v>67.202399999999997</v>
       </c>
+      <c r="C48">
+        <v>1582.4</v>
+      </c>
+      <c r="F48">
+        <v>1664.84</v>
+      </c>
       <c r="G48">
         <v>4</v>
       </c>
@@ -1949,6 +2029,12 @@
       <c r="B49">
         <v>80.640500000000003</v>
       </c>
+      <c r="C49">
+        <v>1581.68</v>
+      </c>
+      <c r="F49">
+        <v>1638.41</v>
+      </c>
       <c r="G49">
         <v>4</v>
       </c>
@@ -1978,6 +2064,12 @@
       <c r="C50">
         <v>649.19600000000003</v>
       </c>
+      <c r="D50">
+        <v>17422.400000000001</v>
+      </c>
+      <c r="F50">
+        <v>662.99</v>
+      </c>
       <c r="G50">
         <v>8</v>
       </c>
@@ -2007,6 +2099,9 @@
       <c r="C51">
         <v>623.91</v>
       </c>
+      <c r="F51">
+        <v>644.30899999999997</v>
+      </c>
       <c r="G51">
         <v>8</v>
       </c>
@@ -2036,6 +2131,9 @@
       <c r="C52">
         <v>618.76800000000003</v>
       </c>
+      <c r="F52">
+        <v>649.74800000000005</v>
+      </c>
       <c r="G52">
         <v>8</v>
       </c>
@@ -2065,6 +2163,9 @@
       <c r="C53">
         <v>712.03899999999999</v>
       </c>
+      <c r="F53">
+        <v>787.46799999999996</v>
+      </c>
       <c r="G53">
         <v>16</v>
       </c>
@@ -2074,7 +2175,7 @@
       <c r="I53">
         <v>627.221</v>
       </c>
-      <c r="J53" s="4">
+      <c r="J53" s="3">
         <v>10029.700000000001</v>
       </c>
       <c r="M53">
@@ -2097,6 +2198,9 @@
       <c r="C54">
         <v>636.154</v>
       </c>
+      <c r="F54">
+        <v>660.31700000000001</v>
+      </c>
       <c r="G54">
         <v>16</v>
       </c>
@@ -2106,6 +2210,9 @@
       <c r="I54">
         <v>584.09500000000003</v>
       </c>
+      <c r="J54" s="7">
+        <v>10023.299999999999</v>
+      </c>
       <c r="M54">
         <v>8</v>
       </c>
@@ -2117,6 +2224,21 @@
       </c>
     </row>
     <row r="55" spans="1:15">
+      <c r="A55">
+        <v>4</v>
+      </c>
+      <c r="B55">
+        <v>14.0671</v>
+      </c>
+      <c r="C55">
+        <v>319.83499999999998</v>
+      </c>
+      <c r="D55">
+        <v>9021.7900000000009</v>
+      </c>
+      <c r="F55">
+        <v>362.3</v>
+      </c>
       <c r="G55">
         <v>16</v>
       </c>
@@ -2137,17 +2259,32 @@
       </c>
     </row>
     <row r="56" spans="1:15">
+      <c r="A56">
+        <v>4</v>
+      </c>
+      <c r="B56">
+        <v>12.7728</v>
+      </c>
+      <c r="C56">
+        <v>323.94099999999997</v>
+      </c>
+      <c r="D56">
+        <v>8920.1</v>
+      </c>
+      <c r="F56">
+        <v>346.88499999999999</v>
+      </c>
       <c r="G56">
         <v>32</v>
       </c>
-      <c r="H56">
-        <v>6.6308100000000003</v>
+      <c r="H56" s="7">
+        <v>1.99576</v>
       </c>
       <c r="I56">
         <v>499.23700000000002</v>
       </c>
-      <c r="J56">
-        <v>32257.7</v>
+      <c r="J56" s="7">
+        <v>10020.5</v>
       </c>
       <c r="M56">
         <v>16</v>
@@ -2160,20 +2297,35 @@
       </c>
     </row>
     <row r="57" spans="1:15">
+      <c r="A57">
+        <v>4</v>
+      </c>
+      <c r="B57">
+        <v>14.036899999999999</v>
+      </c>
+      <c r="C57">
+        <v>387.06099999999998</v>
+      </c>
+      <c r="D57">
+        <v>8941.1299999999992</v>
+      </c>
+      <c r="F57">
+        <v>429.25099999999998</v>
+      </c>
       <c r="G57">
         <v>32</v>
       </c>
-      <c r="H57">
-        <v>6.1220999999999997</v>
+      <c r="H57" s="7">
+        <v>2.0158200000000002</v>
       </c>
       <c r="I57">
         <v>460.988</v>
       </c>
-      <c r="J57">
-        <v>28200.9</v>
+      <c r="J57" s="7">
+        <v>10047.4</v>
       </c>
       <c r="K57" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="M57">
         <v>16</v>
@@ -2186,11 +2338,23 @@
       </c>
     </row>
     <row r="58" spans="1:15">
+      <c r="A58">
+        <v>4</v>
+      </c>
+      <c r="B58">
+        <v>12.254799999999999</v>
+      </c>
+      <c r="C58">
+        <v>318.97899999999998</v>
+      </c>
+      <c r="F58">
+        <v>351.52199999999999</v>
+      </c>
       <c r="G58">
         <v>32</v>
       </c>
-      <c r="H58">
-        <v>6.1061800000000002</v>
+      <c r="H58" s="7">
+        <v>1.98756</v>
       </c>
       <c r="I58">
         <v>452.202</v>
@@ -2206,17 +2370,29 @@
       </c>
     </row>
     <row r="59" spans="1:15">
+      <c r="A59">
+        <v>4</v>
+      </c>
+      <c r="B59">
+        <v>10.579499999999999</v>
+      </c>
+      <c r="C59">
+        <v>318.57100000000003</v>
+      </c>
+      <c r="F59">
+        <v>353.27199999999999</v>
+      </c>
       <c r="G59">
         <v>64</v>
       </c>
-      <c r="H59" s="4">
+      <c r="H59" s="3">
         <v>1.0022200000000001</v>
       </c>
-      <c r="I59" s="4">
+      <c r="I59" s="3">
         <v>34.512300000000003</v>
       </c>
-      <c r="J59">
-        <v>13892.7</v>
+      <c r="J59" s="7">
+        <v>4657.07</v>
       </c>
       <c r="M59">
         <v>16</v>
@@ -2229,16 +2405,31 @@
       </c>
     </row>
     <row r="60" spans="1:15">
+      <c r="A60">
+        <v>8</v>
+      </c>
+      <c r="B60">
+        <v>5.58392</v>
+      </c>
+      <c r="C60">
+        <v>338.029</v>
+      </c>
+      <c r="D60">
+        <v>10201.5</v>
+      </c>
+      <c r="F60">
+        <v>210.07900000000001</v>
+      </c>
       <c r="G60">
         <v>64</v>
       </c>
-      <c r="H60" s="4">
+      <c r="H60" s="3">
         <v>1.0070600000000001</v>
       </c>
-      <c r="I60" s="4">
+      <c r="I60" s="3">
         <v>26.9237</v>
       </c>
-      <c r="J60" s="4">
+      <c r="J60" s="3">
         <v>4709.95</v>
       </c>
       <c r="M60">
@@ -2252,13 +2443,28 @@
       </c>
     </row>
     <row r="61" spans="1:15">
+      <c r="A61">
+        <v>8</v>
+      </c>
+      <c r="B61">
+        <v>5.5550499999999996</v>
+      </c>
+      <c r="C61">
+        <v>247.834</v>
+      </c>
+      <c r="D61">
+        <v>10205.700000000001</v>
+      </c>
+      <c r="F61">
+        <v>183.90899999999999</v>
+      </c>
       <c r="G61">
         <v>64</v>
       </c>
-      <c r="H61" s="4">
+      <c r="H61" s="3">
         <v>1.00603</v>
       </c>
-      <c r="I61" s="4">
+      <c r="I61" s="3">
         <v>28.3809</v>
       </c>
       <c r="J61" s="2">
@@ -2275,6 +2481,21 @@
       </c>
     </row>
     <row r="62" spans="1:15">
+      <c r="A62">
+        <v>8</v>
+      </c>
+      <c r="B62">
+        <v>5.5539100000000001</v>
+      </c>
+      <c r="C62">
+        <v>265.44</v>
+      </c>
+      <c r="D62">
+        <v>10148.700000000001</v>
+      </c>
+      <c r="F62">
+        <v>193.48099999999999</v>
+      </c>
       <c r="G62">
         <v>124</v>
       </c>
@@ -2295,6 +2516,18 @@
       </c>
     </row>
     <row r="63" spans="1:15">
+      <c r="A63">
+        <v>8</v>
+      </c>
+      <c r="B63">
+        <v>5.5922700000000001</v>
+      </c>
+      <c r="C63">
+        <v>292.64</v>
+      </c>
+      <c r="F63">
+        <v>194.22900000000001</v>
+      </c>
       <c r="G63">
         <v>124</v>
       </c>
@@ -2315,6 +2548,18 @@
       </c>
     </row>
     <row r="64" spans="1:15">
+      <c r="A64">
+        <v>8</v>
+      </c>
+      <c r="B64">
+        <v>5.5747999999999998</v>
+      </c>
+      <c r="C64">
+        <v>307.91000000000003</v>
+      </c>
+      <c r="F64">
+        <v>191.006</v>
+      </c>
       <c r="G64">
         <v>124</v>
       </c>
@@ -2334,7 +2579,22 @@
         <v>416.21899999999999</v>
       </c>
     </row>
-    <row r="65" spans="13:15">
+    <row r="65" spans="1:15">
+      <c r="A65">
+        <v>16</v>
+      </c>
+      <c r="B65">
+        <v>2.9831099999999999</v>
+      </c>
+      <c r="C65">
+        <v>185.36</v>
+      </c>
+      <c r="D65">
+        <v>4940.72</v>
+      </c>
+      <c r="F65">
+        <v>196.43600000000001</v>
+      </c>
       <c r="M65">
         <v>32</v>
       </c>
@@ -2345,7 +2605,22 @@
         <v>191.916</v>
       </c>
     </row>
-    <row r="66" spans="13:15">
+    <row r="66" spans="1:15">
+      <c r="A66">
+        <v>16</v>
+      </c>
+      <c r="B66">
+        <v>3.0395599999999998</v>
+      </c>
+      <c r="C66">
+        <v>173.58099999999999</v>
+      </c>
+      <c r="D66">
+        <v>4852.59</v>
+      </c>
+      <c r="F66">
+        <v>176.88800000000001</v>
+      </c>
       <c r="M66">
         <v>32</v>
       </c>
@@ -2356,7 +2631,19 @@
         <v>202.07400000000001</v>
       </c>
     </row>
-    <row r="67" spans="13:15">
+    <row r="67" spans="1:15">
+      <c r="A67">
+        <v>16</v>
+      </c>
+      <c r="B67">
+        <v>3.2753299999999999</v>
+      </c>
+      <c r="C67">
+        <v>170.404</v>
+      </c>
+      <c r="F67">
+        <v>186.203</v>
+      </c>
       <c r="M67">
         <v>32</v>
       </c>
@@ -2367,7 +2654,19 @@
         <v>214.15100000000001</v>
       </c>
     </row>
-    <row r="68" spans="13:15">
+    <row r="68" spans="1:15">
+      <c r="A68">
+        <v>16</v>
+      </c>
+      <c r="B68">
+        <v>3.2482899999999999</v>
+      </c>
+      <c r="C68">
+        <v>164.99299999999999</v>
+      </c>
+      <c r="F68">
+        <v>200.07400000000001</v>
+      </c>
       <c r="M68">
         <v>32</v>
       </c>
@@ -2378,7 +2677,19 @@
         <v>250.226</v>
       </c>
     </row>
-    <row r="69" spans="13:15">
+    <row r="69" spans="1:15">
+      <c r="A69">
+        <v>16</v>
+      </c>
+      <c r="B69">
+        <v>3.2492000000000001</v>
+      </c>
+      <c r="C69">
+        <v>206.92</v>
+      </c>
+      <c r="F69">
+        <v>236.816</v>
+      </c>
       <c r="M69">
         <v>32</v>
       </c>
@@ -2389,7 +2700,22 @@
         <v>193.43</v>
       </c>
     </row>
-    <row r="70" spans="13:15">
+    <row r="70" spans="1:15">
+      <c r="A70">
+        <v>32</v>
+      </c>
+      <c r="B70">
+        <v>2.10717</v>
+      </c>
+      <c r="C70">
+        <v>69.868300000000005</v>
+      </c>
+      <c r="D70">
+        <v>1680.33</v>
+      </c>
+      <c r="F70">
+        <v>81.354500000000002</v>
+      </c>
       <c r="M70">
         <v>32</v>
       </c>
@@ -2400,7 +2726,22 @@
         <v>239.16900000000001</v>
       </c>
     </row>
-    <row r="71" spans="13:15">
+    <row r="71" spans="1:15">
+      <c r="A71">
+        <v>32</v>
+      </c>
+      <c r="B71">
+        <v>2.2664800000000001</v>
+      </c>
+      <c r="C71">
+        <v>74.1892</v>
+      </c>
+      <c r="D71">
+        <v>1831.94</v>
+      </c>
+      <c r="F71">
+        <v>102.149</v>
+      </c>
       <c r="M71">
         <v>32</v>
       </c>
@@ -2411,7 +2752,22 @@
         <v>199.828</v>
       </c>
     </row>
-    <row r="72" spans="13:15">
+    <row r="72" spans="1:15">
+      <c r="A72">
+        <v>32</v>
+      </c>
+      <c r="B72">
+        <v>2.1227999999999998</v>
+      </c>
+      <c r="C72">
+        <v>72.215299999999999</v>
+      </c>
+      <c r="D72">
+        <v>2169.2600000000002</v>
+      </c>
+      <c r="F72">
+        <v>82.326700000000002</v>
+      </c>
       <c r="M72">
         <v>32</v>
       </c>
@@ -2422,7 +2778,22 @@
         <v>203.13200000000001</v>
       </c>
     </row>
-    <row r="73" spans="13:15">
+    <row r="73" spans="1:15">
+      <c r="A73">
+        <v>32</v>
+      </c>
+      <c r="B73">
+        <v>2.2177899999999999</v>
+      </c>
+      <c r="C73">
+        <v>86.012699999999995</v>
+      </c>
+      <c r="D73">
+        <v>1750.51</v>
+      </c>
+      <c r="F73">
+        <v>106.52200000000001</v>
+      </c>
       <c r="M73">
         <v>32</v>
       </c>
@@ -2433,7 +2804,22 @@
         <v>238.333</v>
       </c>
     </row>
-    <row r="74" spans="13:15">
+    <row r="74" spans="1:15">
+      <c r="A74">
+        <v>32</v>
+      </c>
+      <c r="B74">
+        <v>2.2117599999999999</v>
+      </c>
+      <c r="C74">
+        <v>57.994300000000003</v>
+      </c>
+      <c r="D74">
+        <v>1784.36</v>
+      </c>
+      <c r="F74">
+        <v>81.409400000000005</v>
+      </c>
       <c r="M74">
         <v>32</v>
       </c>
@@ -2444,7 +2830,22 @@
         <v>195.01900000000001</v>
       </c>
     </row>
-    <row r="75" spans="13:15">
+    <row r="75" spans="1:15">
+      <c r="A75">
+        <v>64</v>
+      </c>
+      <c r="B75">
+        <v>1.72241</v>
+      </c>
+      <c r="C75">
+        <v>16.153300000000002</v>
+      </c>
+      <c r="D75">
+        <v>862.94899999999996</v>
+      </c>
+      <c r="F75">
+        <v>12.8367</v>
+      </c>
       <c r="M75">
         <v>64</v>
       </c>
@@ -2455,7 +2856,22 @@
         <v>31.647099999999998</v>
       </c>
     </row>
-    <row r="76" spans="13:15">
+    <row r="76" spans="1:15">
+      <c r="A76">
+        <v>64</v>
+      </c>
+      <c r="B76">
+        <v>1.7247699999999999</v>
+      </c>
+      <c r="C76">
+        <v>12.231400000000001</v>
+      </c>
+      <c r="D76">
+        <v>735.04100000000005</v>
+      </c>
+      <c r="F76">
+        <v>13.389099999999999</v>
+      </c>
       <c r="M76">
         <v>64</v>
       </c>
@@ -2466,7 +2882,22 @@
         <v>53.1434</v>
       </c>
     </row>
-    <row r="77" spans="13:15">
+    <row r="77" spans="1:15">
+      <c r="A77">
+        <v>64</v>
+      </c>
+      <c r="B77">
+        <v>1.74777</v>
+      </c>
+      <c r="C77">
+        <v>16.022600000000001</v>
+      </c>
+      <c r="D77">
+        <v>721.71299999999997</v>
+      </c>
+      <c r="F77">
+        <v>16.428100000000001</v>
+      </c>
       <c r="M77">
         <v>64</v>
       </c>
@@ -2477,7 +2908,22 @@
         <v>47.1267</v>
       </c>
     </row>
-    <row r="78" spans="13:15">
+    <row r="78" spans="1:15">
+      <c r="A78">
+        <v>64</v>
+      </c>
+      <c r="B78">
+        <v>1.6972799999999999</v>
+      </c>
+      <c r="C78">
+        <v>16.2988</v>
+      </c>
+      <c r="D78">
+        <v>862.24599999999998</v>
+      </c>
+      <c r="F78">
+        <v>16.513400000000001</v>
+      </c>
       <c r="M78">
         <v>64</v>
       </c>
@@ -2488,7 +2934,22 @@
         <v>43.902099999999997</v>
       </c>
     </row>
-    <row r="79" spans="13:15">
+    <row r="79" spans="1:15">
+      <c r="A79">
+        <v>64</v>
+      </c>
+      <c r="B79">
+        <v>1.6889099999999999</v>
+      </c>
+      <c r="C79">
+        <v>16.863199999999999</v>
+      </c>
+      <c r="D79">
+        <v>858.15</v>
+      </c>
+      <c r="F79">
+        <v>12.8561</v>
+      </c>
       <c r="M79">
         <v>64</v>
       </c>
@@ -2499,7 +2960,7 @@
         <v>39.096699999999998</v>
       </c>
     </row>
-    <row r="80" spans="13:15">
+    <row r="80" spans="1:15">
       <c r="M80">
         <v>64</v>
       </c>
@@ -2555,7 +3016,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>

<commit_message>
Added CC, TRI, LUBY, updated PAGERANK results.
git-svn-id: svn+ssh://software-srn.sandia.gov/svn/mapreduce/trunk@611 3fc257bb-8550-0410-81b3-a5c103da83f7
</commit_message>
<xml_diff>
--- a/paper/results.xlsx
+++ b/paper/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3220" yWindow="60" windowWidth="23240" windowHeight="21660" tabRatio="500"/>
+    <workbookView xWindow="1140" yWindow="2100" windowWidth="34400" windowHeight="21160" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="jj" localSheetId="0">Sheet1!$A$15:$B$38</definedName>
     <definedName name="jj_1" localSheetId="0">Sheet1!$H$41:$I$64</definedName>
-    <definedName name="jjj" localSheetId="0">Sheet1!$N$15:$O$84</definedName>
+    <definedName name="jjj" localSheetId="0">Sheet1!$AL$15:$AM$84</definedName>
   </definedNames>
   <calcPr calcId="130407" concurrentCalc="0"/>
   <extLst>
@@ -45,11 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="20">
-  <si>
-    <t>RMAT Generation</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="29">
   <si>
     <t>All runs on odin, pernode mode</t>
     <phoneticPr fontId="6" type="noConversion"/>
@@ -95,15 +91,7 @@
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>SSSP</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
     <t>BOLD VALUES are updated to include only edge generation time.</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>BOLD TIMES have 0.002 tolerance</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
@@ -126,6 +114,54 @@
     <t>RMAT-28</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
+  <si>
+    <t>ORIG ALG</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>RMAT-28</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Trilinos</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>RMAT-20</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Trilinos</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>RMAT-24</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Luby</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>CC</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tri</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>SSSP:  Not run yet without bad nodes</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>RMAT Generation:  Not run yet without bad nodes</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pagerank</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -143,7 +179,6 @@
       <name val="Verdana"/>
     </font>
     <font>
-      <b/>
       <sz val="10"/>
       <name val="Verdana"/>
     </font>
@@ -215,11 +250,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="jj_1" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="jj" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="jj" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="jj_1" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -542,108 +577,189 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:R84"/>
+  <dimension ref="A1:AP85"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8:G9"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="AE10" sqref="AE10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="9.5703125" customWidth="1"/>
     <col min="2" max="2" width="8" customWidth="1"/>
     <col min="8" max="8" width="16.5703125" customWidth="1"/>
-    <col min="14" max="14" width="16.140625" customWidth="1"/>
-    <col min="15" max="15" width="8" customWidth="1"/>
+    <col min="38" max="38" width="16.140625" customWidth="1"/>
+    <col min="39" max="39" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:42">
       <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1" t="s">
+        <v>28</v>
+      </c>
+      <c r="T1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:42">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="N1" t="s">
+      <c r="H2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:42">
+      <c r="F3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:18">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="G3" t="s">
+        <v>15</v>
+      </c>
+      <c r="M3" t="s">
         <v>17</v>
       </c>
-      <c r="N2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18">
-      <c r="F3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="O3" t="s">
+        <v>19</v>
+      </c>
+      <c r="P3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:42">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" t="s">
+        <v>4</v>
+      </c>
+      <c r="L4" t="s">
+        <v>5</v>
+      </c>
+      <c r="M4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:18">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="O4" t="s">
+        <v>20</v>
+      </c>
+      <c r="P4" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>18</v>
+      </c>
+      <c r="T4" t="s">
+        <v>1</v>
+      </c>
+      <c r="U4" t="s">
+        <v>2</v>
+      </c>
+      <c r="V4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="W4" t="s">
+        <v>4</v>
+      </c>
+      <c r="X4" t="s">
         <v>5</v>
       </c>
-      <c r="E4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I4" t="s">
+      <c r="Z4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB4" t="s">
         <v>3</v>
       </c>
-      <c r="J4" t="s">
-        <v>4</v>
-      </c>
-      <c r="K4" t="s">
+      <c r="AC4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD4" t="s">
         <v>5</v>
       </c>
-      <c r="L4" t="s">
-        <v>6</v>
-      </c>
-      <c r="N4" t="s">
-        <v>2</v>
-      </c>
-      <c r="O4" t="s">
+      <c r="AF4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH4" t="s">
         <v>3</v>
       </c>
-      <c r="P4" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q4" t="s">
+      <c r="AI4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AJ4" t="s">
         <v>5</v>
       </c>
-      <c r="R4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18">
+      <c r="AL4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AM4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AN4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AO4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AP4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:42">
       <c r="A5">
         <v>1</v>
       </c>
@@ -670,31 +786,64 @@
       </c>
       <c r="I5" s="1">
         <f>AVERAGE(I15:I17)</f>
-        <v>29.667527777777778</v>
+        <v>28.531333333333333</v>
       </c>
       <c r="J5" s="1">
         <f>AVERAGE(J15:J17)</f>
-        <v>1523.9025641025644</v>
+        <v>1529.4561111111113</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L5" s="1"/>
-      <c r="N5">
-        <v>1</v>
-      </c>
-      <c r="O5" s="1">
-        <f>AVERAGE(O15:O24)</f>
+      <c r="O5">
+        <f>AVERAGE(O15:O19)</f>
+        <v>0.30378166666666673</v>
+      </c>
+      <c r="T5">
+        <v>1</v>
+      </c>
+      <c r="U5">
+        <f>AVERAGE(U15:U19)</f>
+        <v>150.76600000000002</v>
+      </c>
+      <c r="V5">
+        <f>AVERAGE(V15:V19)</f>
+        <v>8259.74</v>
+      </c>
+      <c r="Z5">
+        <v>1</v>
+      </c>
+      <c r="AA5">
+        <f>AVERAGE(AA15:AA19)</f>
+        <v>410.38033333333328</v>
+      </c>
+      <c r="AB5">
+        <f>AVERAGE(AB15:AB19)</f>
+        <v>20011.2</v>
+      </c>
+      <c r="AF5">
+        <v>1</v>
+      </c>
+      <c r="AG5">
+        <f>AVERAGE(AG15:AG19)</f>
+        <v>1960.7150000000001</v>
+      </c>
+      <c r="AL5">
+        <v>1</v>
+      </c>
+      <c r="AM5" s="1">
+        <f>AVERAGE(AM15:AM24)</f>
         <v>98.959870000000024</v>
       </c>
-      <c r="P5" s="1">
-        <f>AVERAGE(P15:P24)</f>
+      <c r="AN5" s="1">
+        <f>AVERAGE(AN15:AN24)</f>
         <v>5763.19</v>
       </c>
-      <c r="Q5" s="1"/>
-      <c r="R5" s="1"/>
-    </row>
-    <row r="6" spans="1:18">
+      <c r="AO5" s="1"/>
+      <c r="AP5" s="1"/>
+    </row>
+    <row r="6" spans="1:42">
       <c r="A6">
         <v>2</v>
       </c>
@@ -721,31 +870,68 @@
       </c>
       <c r="I6" s="1">
         <f>AVERAGE(I18:I20)</f>
-        <v>16.621694444444444</v>
+        <v>16.147544444444446</v>
       </c>
       <c r="J6" s="1">
         <f>AVERAGE(J18:J20)</f>
-        <v>792.54615384615374</v>
+        <v>819.26111111111106</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L6" s="1"/>
-      <c r="N6">
-        <v>2</v>
-      </c>
-      <c r="O6" s="1">
-        <f>AVERAGE(O25:O34)</f>
+      <c r="O6">
+        <f>AVERAGE(O20:O24)</f>
+        <v>0.12164140000000001</v>
+      </c>
+      <c r="P6">
+        <f>AVERAGE(P20:P24)</f>
+        <v>3.6764899999999998</v>
+      </c>
+      <c r="T6">
+        <v>2</v>
+      </c>
+      <c r="U6">
+        <f>AVERAGE(U20:U24)</f>
+        <v>106.48399999999999</v>
+      </c>
+      <c r="V6">
+        <f>AVERAGE(V20:V24)</f>
+        <v>4943.416666666667</v>
+      </c>
+      <c r="Z6">
+        <v>2</v>
+      </c>
+      <c r="AA6">
+        <f>AVERAGE(AA20:AA24)</f>
+        <v>266.76033333333334</v>
+      </c>
+      <c r="AB6">
+        <f>AVERAGE(AB20:AB24)</f>
+        <v>12141.8</v>
+      </c>
+      <c r="AF6">
+        <v>2</v>
+      </c>
+      <c r="AG6">
+        <f>AVERAGE(AG20:AG24)</f>
+        <v>1225.6000000000001</v>
+      </c>
+      <c r="AL6">
+        <v>2</v>
+      </c>
+      <c r="AM6" s="1">
+        <f>AVERAGE(AM25:AM34)</f>
         <v>56.68085</v>
       </c>
-      <c r="P6" s="1">
-        <f>AVERAGE(P25:P34)</f>
+      <c r="AN6" s="1">
+        <f>AVERAGE(AN25:AN34)</f>
         <v>2426.3740000000003</v>
       </c>
-      <c r="Q6" s="1"/>
-      <c r="R6" s="1"/>
-    </row>
-    <row r="7" spans="1:18">
+      <c r="AO6" s="1"/>
+      <c r="AP6" s="1"/>
+    </row>
+    <row r="7" spans="1:42">
       <c r="A7">
         <v>4</v>
       </c>
@@ -772,31 +958,72 @@
       </c>
       <c r="I7" s="1">
         <f>AVERAGE(I21:I23)</f>
-        <v>4.1770749999999994</v>
+        <v>4.2492722222222232</v>
       </c>
       <c r="J7" s="1">
         <f>AVERAGE(J21:J23)</f>
-        <v>359.25871794871796</v>
+        <v>326.47944444444443</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L7" s="1"/>
-      <c r="N7">
-        <v>4</v>
-      </c>
-      <c r="O7" s="1">
-        <f>AVERAGE(O35:O44)</f>
+      <c r="O7">
+        <f>AVERAGE(O25:O29)</f>
+        <v>7.039419999999999E-2</v>
+      </c>
+      <c r="P7">
+        <f>AVERAGE(P25:P29)</f>
+        <v>2.0148600000000001</v>
+      </c>
+      <c r="T7">
+        <v>4</v>
+      </c>
+      <c r="U7">
+        <f>AVERAGE(U25:U29)</f>
+        <v>53.930299999999995</v>
+      </c>
+      <c r="V7">
+        <f>AVERAGE(V25:V29)</f>
+        <v>1943.665</v>
+      </c>
+      <c r="Z7">
+        <v>4</v>
+      </c>
+      <c r="AA7">
+        <f>AVERAGE(AA25:AA29)</f>
+        <v>146.07225</v>
+      </c>
+      <c r="AB7">
+        <f>AVERAGE(AB25:AB29)</f>
+        <v>5206.5774999999994</v>
+      </c>
+      <c r="AF7">
+        <v>4</v>
+      </c>
+      <c r="AG7">
+        <f>AVERAGE(AG25:AG29)</f>
+        <v>572.35</v>
+      </c>
+      <c r="AH7">
+        <f>AVERAGE(AH25:AH29)</f>
+        <v>26946.7</v>
+      </c>
+      <c r="AL7">
+        <v>4</v>
+      </c>
+      <c r="AM7" s="1">
+        <f>AVERAGE(AM35:AM44)</f>
         <v>13.016690000000001</v>
       </c>
-      <c r="P7" s="1">
-        <f>AVERAGE(P35:P44)</f>
+      <c r="AN7" s="1">
+        <f>AVERAGE(AN35:AN44)</f>
         <v>924.60090000000002</v>
       </c>
-      <c r="Q7" s="1"/>
-      <c r="R7" s="1"/>
-    </row>
-    <row r="8" spans="1:18">
+      <c r="AO7" s="1"/>
+      <c r="AP7" s="1"/>
+    </row>
+    <row r="8" spans="1:42">
       <c r="A8">
         <v>8</v>
       </c>
@@ -826,31 +1053,77 @@
       </c>
       <c r="I8" s="1">
         <f>AVERAGE(I24:I26)</f>
-        <v>1.4050277777777778</v>
+        <v>1.4770972222222223</v>
       </c>
       <c r="J8" s="1">
         <f>AVERAGE(J24:J26)</f>
-        <v>120.5551282051282</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>10</v>
+        <v>117.80883333333334</v>
+      </c>
+      <c r="K8" s="1">
+        <f>AVERAGE(K24:K26)</f>
+        <v>3873.4800000000005</v>
       </c>
       <c r="L8" s="1"/>
-      <c r="N8">
-        <v>8</v>
-      </c>
-      <c r="O8" s="1">
-        <f>AVERAGE(O45:O54)</f>
+      <c r="O8">
+        <f>AVERAGE(O30:O34)</f>
+        <v>3.57513E-2</v>
+      </c>
+      <c r="P8">
+        <f>AVERAGE(P30:P34)</f>
+        <v>1.0679209999999999</v>
+      </c>
+      <c r="T8">
+        <v>8</v>
+      </c>
+      <c r="U8">
+        <f>AVERAGE(U30:U34)</f>
+        <v>18.299700000000001</v>
+      </c>
+      <c r="V8">
+        <f>AVERAGE(V30:V34)</f>
+        <v>629.30225000000007</v>
+      </c>
+      <c r="W8">
+        <f>AVERAGE(W30:W34)</f>
+        <v>23233</v>
+      </c>
+      <c r="Z8">
+        <v>8</v>
+      </c>
+      <c r="AA8">
+        <f>AVERAGE(AA30:AA34)</f>
+        <v>48.778424999999999</v>
+      </c>
+      <c r="AB8">
+        <f>AVERAGE(AB30:AB34)</f>
+        <v>1648.6624999999999</v>
+      </c>
+      <c r="AF8">
+        <v>8</v>
+      </c>
+      <c r="AG8">
+        <f>AVERAGE(AG30:AG34)</f>
+        <v>215.30549999999999</v>
+      </c>
+      <c r="AH8">
+        <f>AVERAGE(AH30:AH34)</f>
+        <v>11218.55</v>
+      </c>
+      <c r="AL8">
+        <v>8</v>
+      </c>
+      <c r="AM8" s="1">
+        <f>AVERAGE(AM45:AM54)</f>
         <v>4.0994849999999996</v>
       </c>
-      <c r="P8" s="1">
-        <f>AVERAGE(P45:P54)</f>
+      <c r="AN8" s="1">
+        <f>AVERAGE(AN45:AN54)</f>
         <v>409.97899999999998</v>
       </c>
-      <c r="Q8" s="1"/>
-      <c r="R8" s="1"/>
-    </row>
-    <row r="9" spans="1:18">
+      <c r="AO8" s="1"/>
+      <c r="AP8" s="1"/>
+    </row>
+    <row r="9" spans="1:42">
       <c r="A9">
         <v>16</v>
       </c>
@@ -880,32 +1153,81 @@
       </c>
       <c r="I9" s="1">
         <f>AVERAGE(I27:I29)</f>
-        <v>0.67409111111111109</v>
+        <v>0.68704777777777781</v>
       </c>
       <c r="J9" s="1">
         <f>AVERAGE(J27:J29)</f>
-        <v>45.144256410256411</v>
+        <v>43.852944444444439</v>
       </c>
       <c r="K9" s="1">
         <f>AVERAGE(K27:K29)</f>
-        <v>2005.3</v>
+        <v>2041.6799999999998</v>
       </c>
       <c r="L9" s="1"/>
-      <c r="N9">
-        <v>16</v>
-      </c>
-      <c r="O9" s="1">
-        <f>AVERAGE(O55:O64)</f>
+      <c r="O9">
+        <f>AVERAGE(O35:O39)</f>
+        <v>1.8425733333333333E-2</v>
+      </c>
+      <c r="P9">
+        <f>AVERAGE(P35:P39)</f>
+        <v>0.57296500000000006</v>
+      </c>
+      <c r="T9">
+        <v>16</v>
+      </c>
+      <c r="U9">
+        <f>AVERAGE(U35:U39)</f>
+        <v>4.1263419999999993</v>
+      </c>
+      <c r="V9">
+        <f>AVERAGE(V35:V39)</f>
+        <v>251.50020000000004</v>
+      </c>
+      <c r="W9">
+        <f>AVERAGE(W35:W39)</f>
+        <v>11092.400000000001</v>
+      </c>
+      <c r="Z9">
+        <v>16</v>
+      </c>
+      <c r="AA9">
+        <f>AVERAGE(AA35:AA39)</f>
+        <v>12.126520000000001</v>
+      </c>
+      <c r="AB9">
+        <f>AVERAGE(AB35:AB39)</f>
+        <v>718.85839999999996</v>
+      </c>
+      <c r="AC9">
+        <f>AVERAGE(AC35:AC39)</f>
+        <v>28453</v>
+      </c>
+      <c r="AF9">
+        <v>16</v>
+      </c>
+      <c r="AG9">
+        <f>AVERAGE(AG35:AG39)</f>
+        <v>85.118840000000006</v>
+      </c>
+      <c r="AH9">
+        <f>AVERAGE(AH35:AH39)</f>
+        <v>7944.1559999999999</v>
+      </c>
+      <c r="AL9">
+        <v>16</v>
+      </c>
+      <c r="AM9" s="1">
+        <f>AVERAGE(AM55:AM64)</f>
         <v>2.3383849999999997</v>
       </c>
-      <c r="P9" s="1">
-        <f>AVERAGE(P55:P64)</f>
+      <c r="AN9" s="1">
+        <f>AVERAGE(AN55:AN64)</f>
         <v>423.61710000000005</v>
       </c>
-      <c r="Q9" s="1"/>
-      <c r="R9" s="1"/>
-    </row>
-    <row r="10" spans="1:18">
+      <c r="AO9" s="1"/>
+      <c r="AP9" s="1"/>
+    </row>
+    <row r="10" spans="1:42">
       <c r="A10">
         <v>32</v>
       </c>
@@ -935,32 +1257,81 @@
       </c>
       <c r="I10" s="1">
         <f>AVERAGE(I30:I32)</f>
-        <v>0.33328555555555556</v>
+        <v>0.36834888888888889</v>
       </c>
       <c r="J10" s="1">
         <f>AVERAGE(J30:J32)</f>
-        <v>36.216076923076919</v>
+        <v>23.622333333333334</v>
       </c>
       <c r="K10" s="1">
         <f>AVERAGE(K30:K32)</f>
-        <v>2006.79</v>
+        <v>955.64066666666668</v>
       </c>
       <c r="L10" s="1"/>
-      <c r="N10">
-        <v>32</v>
-      </c>
-      <c r="O10" s="1">
-        <f>AVERAGE(O65:O74)</f>
+      <c r="O10">
+        <f>AVERAGE(O40:O44)</f>
+        <v>9.3230400000000012E-3</v>
+      </c>
+      <c r="P10">
+        <f>AVERAGE(P40:P44)</f>
+        <v>0.29707600000000001</v>
+      </c>
+      <c r="T10">
+        <v>32</v>
+      </c>
+      <c r="U10">
+        <f>AVERAGE(U40:U44)</f>
+        <v>2.1167399999999996</v>
+      </c>
+      <c r="V10">
+        <f>AVERAGE(V40:V44)</f>
+        <v>141.94760000000002</v>
+      </c>
+      <c r="W10">
+        <f>AVERAGE(W40:W44)</f>
+        <v>5725.9760000000006</v>
+      </c>
+      <c r="Z10">
+        <v>32</v>
+      </c>
+      <c r="AA10">
+        <f>AVERAGE(AA40:AA44)</f>
+        <v>6.9125460000000007</v>
+      </c>
+      <c r="AB10">
+        <f>AVERAGE(AB40:AB44)</f>
+        <v>415.79740000000004</v>
+      </c>
+      <c r="AC10">
+        <f>AVERAGE(AC40:AC44)</f>
+        <v>14250.8</v>
+      </c>
+      <c r="AF10">
+        <v>32</v>
+      </c>
+      <c r="AG10">
+        <f>AVERAGE(AG40:AG44)</f>
+        <v>65.111239999999995</v>
+      </c>
+      <c r="AH10">
+        <f>AVERAGE(AH40:AH44)</f>
+        <v>6511.4820000000009</v>
+      </c>
+      <c r="AL10">
+        <v>32</v>
+      </c>
+      <c r="AM10" s="1">
+        <f>AVERAGE(AM65:AM74)</f>
         <v>1.509998</v>
       </c>
-      <c r="P10" s="1">
-        <f>AVERAGE(P65:P74)</f>
+      <c r="AN10" s="1">
+        <f>AVERAGE(AN65:AN74)</f>
         <v>212.72780000000003</v>
       </c>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="1"/>
-    </row>
-    <row r="11" spans="1:18">
+      <c r="AO10" s="1"/>
+      <c r="AP10" s="1"/>
+    </row>
+    <row r="11" spans="1:42">
       <c r="A11">
         <v>64</v>
       </c>
@@ -990,32 +1361,81 @@
       </c>
       <c r="I11" s="1">
         <f>AVERAGE(I33:I35)</f>
-        <v>0.16751722222222223</v>
+        <v>0.18439222222222221</v>
       </c>
       <c r="J11" s="1">
         <f>AVERAGE(J33:J35)</f>
-        <v>4.9898277777777782</v>
+        <v>5.0188166666666669</v>
       </c>
       <c r="K11" s="1">
         <f>AVERAGE(K33:K35)</f>
-        <v>942.84133333333341</v>
+        <v>391.39933333333329</v>
       </c>
       <c r="L11" s="1"/>
-      <c r="N11">
-        <v>64</v>
-      </c>
-      <c r="O11" s="1">
-        <f>AVERAGE(O75:O84)</f>
+      <c r="O11">
+        <f>AVERAGE(O45:O49)</f>
+        <v>4.9461666666666673E-3</v>
+      </c>
+      <c r="P11">
+        <f>AVERAGE(P45:P49)</f>
+        <v>0.14927593333333333</v>
+      </c>
+      <c r="T11">
+        <v>64</v>
+      </c>
+      <c r="U11">
+        <f>AVERAGE(U45:U49)</f>
+        <v>1.1083940000000001</v>
+      </c>
+      <c r="V11">
+        <f>AVERAGE(V45:V49)</f>
+        <v>137.27640000000002</v>
+      </c>
+      <c r="W11">
+        <f>AVERAGE(W45:W49)</f>
+        <v>5975.0120000000006</v>
+      </c>
+      <c r="Z11">
+        <v>64</v>
+      </c>
+      <c r="AA11">
+        <f>AVERAGE(AA45:AA49)</f>
+        <v>6.227036</v>
+      </c>
+      <c r="AB11">
+        <f>AVERAGE(AB45:AB49)</f>
+        <v>470.88020000000006</v>
+      </c>
+      <c r="AC11">
+        <f>AVERAGE(AC45:AC49)</f>
+        <v>15864.05</v>
+      </c>
+      <c r="AF11">
+        <v>64</v>
+      </c>
+      <c r="AG11">
+        <f>AVERAGE(AG45:AG49)</f>
+        <v>37.333460000000002</v>
+      </c>
+      <c r="AH11">
+        <f>AVERAGE(AH45:AH49)</f>
+        <v>3370.9660000000003</v>
+      </c>
+      <c r="AL11">
+        <v>64</v>
+      </c>
+      <c r="AM11" s="1">
+        <f>AVERAGE(AM75:AM84)</f>
         <v>1.3839149999999996</v>
       </c>
-      <c r="P11" s="1">
-        <f>AVERAGE(P75:P84)</f>
+      <c r="AN11" s="1">
+        <f>AVERAGE(AN75:AN84)</f>
         <v>43.537410000000001</v>
       </c>
-      <c r="Q11" s="1"/>
-      <c r="R11" s="1"/>
-    </row>
-    <row r="12" spans="1:18">
+      <c r="AO11" s="1"/>
+      <c r="AP11" s="1"/>
+    </row>
+    <row r="12" spans="1:42">
       <c r="A12">
         <v>124</v>
       </c>
@@ -1028,7 +1448,7 @@
         <v>14.657500000000001</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
@@ -1038,25 +1458,25 @@
       </c>
       <c r="I12" s="1">
         <f>AVERAGE(I36:I38)</f>
-        <v>0.15289361111111111</v>
+        <v>0</v>
       </c>
       <c r="J12" s="1">
         <f>AVERAGE(J36:J38)</f>
-        <v>3.1249666666666669</v>
+        <v>0</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L12" s="1"/>
-      <c r="N12">
+      <c r="AL12">
         <v>124</v>
       </c>
-      <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
-      <c r="Q12" s="1"/>
-      <c r="R12" s="1"/>
-    </row>
-    <row r="15" spans="1:18">
+      <c r="AM12" s="1"/>
+      <c r="AN12" s="1"/>
+      <c r="AO12" s="1"/>
+      <c r="AP12" s="1"/>
+    </row>
+    <row r="15" spans="1:42">
       <c r="A15">
         <v>1</v>
       </c>
@@ -1070,24 +1490,55 @@
         <v>1</v>
       </c>
       <c r="I15">
-        <f>I41/12</f>
-        <v>29.925416666666667</v>
+        <f>I41/6</f>
+        <v>29.257333333333335</v>
       </c>
       <c r="J15">
-        <f t="shared" ref="J15:J38" si="0">J41/13</f>
-        <v>1533.5769230769231</v>
+        <f t="shared" ref="J15:J35" si="0">J41/6</f>
+        <v>1525.6366666666665</v>
       </c>
       <c r="N15">
         <v>1</v>
       </c>
       <c r="O15">
+        <f>O51/6</f>
+        <v>0.30490166666666668</v>
+      </c>
+      <c r="T15">
+        <v>1</v>
+      </c>
+      <c r="U15">
+        <v>148.828</v>
+      </c>
+      <c r="V15">
+        <v>8259.74</v>
+      </c>
+      <c r="Z15">
+        <v>1</v>
+      </c>
+      <c r="AA15">
+        <v>360.00599999999997</v>
+      </c>
+      <c r="AB15">
+        <v>20011.2</v>
+      </c>
+      <c r="AF15">
+        <v>1</v>
+      </c>
+      <c r="AG15">
+        <v>1955.19</v>
+      </c>
+      <c r="AL15">
+        <v>1</v>
+      </c>
+      <c r="AM15">
         <v>101.836</v>
       </c>
-      <c r="P15">
+      <c r="AN15">
         <v>5763.19</v>
       </c>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:42">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1095,27 +1546,52 @@
         <v>115.398</v>
       </c>
       <c r="C16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H16">
         <v>1</v>
       </c>
       <c r="I16">
-        <f t="shared" ref="I16:I38" si="1">I42/12</f>
-        <v>29.40625</v>
+        <f t="shared" ref="I16:I35" si="1">I42/6</f>
+        <v>28.227666666666668</v>
       </c>
       <c r="J16">
         <f t="shared" si="0"/>
-        <v>1499.5923076923077</v>
+        <v>1534.99</v>
       </c>
       <c r="N16">
         <v>1</v>
       </c>
       <c r="O16">
+        <f t="shared" ref="O16:P49" si="2">O52/6</f>
+        <v>0.30325666666666667</v>
+      </c>
+      <c r="T16">
+        <v>1</v>
+      </c>
+      <c r="U16">
+        <v>152.70400000000001</v>
+      </c>
+      <c r="Z16">
+        <v>1</v>
+      </c>
+      <c r="AA16">
+        <v>420.54599999999999</v>
+      </c>
+      <c r="AF16">
+        <v>1</v>
+      </c>
+      <c r="AG16">
+        <v>1966.24</v>
+      </c>
+      <c r="AL16">
+        <v>1</v>
+      </c>
+      <c r="AM16">
         <v>97.226200000000006</v>
       </c>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:40">
       <c r="A17">
         <v>1</v>
       </c>
@@ -1123,27 +1599,46 @@
         <v>110.443</v>
       </c>
       <c r="C17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H17">
         <v>1</v>
       </c>
       <c r="I17">
         <f t="shared" si="1"/>
-        <v>29.670916666666667</v>
+        <v>28.108999999999998</v>
       </c>
       <c r="J17">
         <f t="shared" si="0"/>
-        <v>1538.5384615384614</v>
+        <v>1527.7416666666668</v>
       </c>
       <c r="N17">
         <v>1</v>
       </c>
       <c r="O17">
+        <f t="shared" si="2"/>
+        <v>0.30329166666666668</v>
+      </c>
+      <c r="T17">
+        <v>1</v>
+      </c>
+      <c r="Z17">
+        <v>1</v>
+      </c>
+      <c r="AA17">
+        <v>450.589</v>
+      </c>
+      <c r="AF17">
+        <v>1</v>
+      </c>
+      <c r="AL17">
+        <v>1</v>
+      </c>
+      <c r="AM17">
         <v>99.859300000000005</v>
       </c>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:40">
       <c r="A18">
         <v>2</v>
       </c>
@@ -1158,20 +1653,36 @@
       </c>
       <c r="I18">
         <f t="shared" si="1"/>
-        <v>16.761583333333334</v>
+        <v>15.786033333333334</v>
       </c>
       <c r="J18">
         <f t="shared" si="0"/>
-        <v>799.93076923076922</v>
+        <v>822.11833333333334</v>
       </c>
       <c r="N18">
         <v>1</v>
       </c>
       <c r="O18">
+        <f t="shared" si="2"/>
+        <v>0.30324499999999999</v>
+      </c>
+      <c r="T18">
+        <v>1</v>
+      </c>
+      <c r="Z18">
+        <v>1</v>
+      </c>
+      <c r="AF18">
+        <v>1</v>
+      </c>
+      <c r="AL18">
+        <v>1</v>
+      </c>
+      <c r="AM18">
         <v>94.698499999999996</v>
       </c>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:40">
       <c r="A19">
         <v>2</v>
       </c>
@@ -1186,20 +1697,36 @@
       </c>
       <c r="I19">
         <f t="shared" si="1"/>
-        <v>16.135333333333332</v>
+        <v>15.785266666666667</v>
       </c>
       <c r="J19">
         <f t="shared" si="0"/>
-        <v>786.72307692307686</v>
+        <v>818.54333333333341</v>
       </c>
       <c r="N19">
         <v>1</v>
       </c>
       <c r="O19">
+        <f t="shared" si="2"/>
+        <v>0.30421333333333334</v>
+      </c>
+      <c r="T19">
+        <v>1</v>
+      </c>
+      <c r="Z19">
+        <v>1</v>
+      </c>
+      <c r="AF19">
+        <v>1</v>
+      </c>
+      <c r="AL19">
+        <v>1</v>
+      </c>
+      <c r="AM19">
         <v>100.968</v>
       </c>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:40">
       <c r="A20">
         <v>2</v>
       </c>
@@ -1207,27 +1734,62 @@
         <v>73.784400000000005</v>
       </c>
       <c r="C20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H20">
         <v>2</v>
       </c>
       <c r="I20">
         <f t="shared" si="1"/>
-        <v>16.968166666666665</v>
+        <v>16.871333333333332</v>
       </c>
       <c r="J20">
         <f t="shared" si="0"/>
-        <v>790.98461538461538</v>
+        <v>817.12166666666656</v>
       </c>
       <c r="N20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O20">
+        <f t="shared" si="2"/>
+        <v>0.12201433333333334</v>
+      </c>
+      <c r="P20">
+        <f t="shared" si="2"/>
+        <v>3.6693833333333337</v>
+      </c>
+      <c r="T20">
+        <v>2</v>
+      </c>
+      <c r="U20">
+        <v>106.054</v>
+      </c>
+      <c r="V20">
+        <v>4928.42</v>
+      </c>
+      <c r="Z20">
+        <v>2</v>
+      </c>
+      <c r="AA20">
+        <v>253.66300000000001</v>
+      </c>
+      <c r="AB20">
+        <v>12029.3</v>
+      </c>
+      <c r="AF20">
+        <v>2</v>
+      </c>
+      <c r="AG20">
+        <v>1237.76</v>
+      </c>
+      <c r="AL20">
+        <v>1</v>
+      </c>
+      <c r="AM20">
         <v>85.743200000000002</v>
       </c>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:40">
       <c r="A21">
         <v>4</v>
       </c>
@@ -1245,20 +1807,55 @@
       </c>
       <c r="I21">
         <f t="shared" si="1"/>
-        <v>3.5380916666666664</v>
+        <v>4.3326666666666664</v>
       </c>
       <c r="J21">
         <f t="shared" si="0"/>
-        <v>356.00076923076927</v>
+        <v>318.48833333333334</v>
       </c>
       <c r="N21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O21">
+        <f t="shared" si="2"/>
+        <v>0.12170983333333334</v>
+      </c>
+      <c r="P21">
+        <f t="shared" si="2"/>
+        <v>3.6611666666666665</v>
+      </c>
+      <c r="T21">
+        <v>2</v>
+      </c>
+      <c r="U21">
+        <v>104.238</v>
+      </c>
+      <c r="V21">
+        <v>4925.74</v>
+      </c>
+      <c r="Z21">
+        <v>2</v>
+      </c>
+      <c r="AA21">
+        <v>298.27999999999997</v>
+      </c>
+      <c r="AB21">
+        <v>12254.3</v>
+      </c>
+      <c r="AF21">
+        <v>2</v>
+      </c>
+      <c r="AG21">
+        <v>1222.57</v>
+      </c>
+      <c r="AL21">
+        <v>1</v>
+      </c>
+      <c r="AM21">
         <v>104.277</v>
       </c>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:40">
       <c r="A22">
         <v>4</v>
       </c>
@@ -1273,20 +1870,52 @@
       </c>
       <c r="I22">
         <f t="shared" si="1"/>
-        <v>4.1913999999999998</v>
+        <v>4.0477166666666671</v>
       </c>
       <c r="J22">
         <f t="shared" si="0"/>
-        <v>363.77692307692308</v>
+        <v>319.59499999999997</v>
       </c>
       <c r="N22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O22">
+        <f t="shared" si="2"/>
+        <v>0.12155266666666666</v>
+      </c>
+      <c r="P22">
+        <f t="shared" si="2"/>
+        <v>3.6710999999999996</v>
+      </c>
+      <c r="T22">
+        <v>2</v>
+      </c>
+      <c r="U22">
+        <v>109.16</v>
+      </c>
+      <c r="V22">
+        <v>4976.09</v>
+      </c>
+      <c r="Z22">
+        <v>2</v>
+      </c>
+      <c r="AA22">
+        <v>248.33799999999999</v>
+      </c>
+      <c r="AF22">
+        <v>2</v>
+      </c>
+      <c r="AG22">
+        <v>1216.47</v>
+      </c>
+      <c r="AL22">
+        <v>1</v>
+      </c>
+      <c r="AM22">
         <v>101.43600000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:16">
+    <row r="23" spans="1:40">
       <c r="A23">
         <v>4</v>
       </c>
@@ -1294,27 +1923,47 @@
         <v>24.4193</v>
       </c>
       <c r="C23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H23">
         <v>4</v>
       </c>
       <c r="I23">
         <f t="shared" si="1"/>
-        <v>4.8017333333333339</v>
+        <v>4.3674333333333335</v>
       </c>
       <c r="J23">
         <f t="shared" si="0"/>
-        <v>357.99846153846153</v>
+        <v>341.35500000000002</v>
       </c>
       <c r="N23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O23">
+        <f t="shared" si="2"/>
+        <v>0.1214755</v>
+      </c>
+      <c r="P23">
+        <f t="shared" si="2"/>
+        <v>3.6918666666666664</v>
+      </c>
+      <c r="T23">
+        <v>2</v>
+      </c>
+      <c r="Z23">
+        <v>2</v>
+      </c>
+      <c r="AF23">
+        <v>2</v>
+      </c>
+      <c r="AL23">
+        <v>1</v>
+      </c>
+      <c r="AM23">
         <v>99.882499999999993</v>
       </c>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:40">
       <c r="A24">
         <v>8</v>
       </c>
@@ -1329,20 +1978,44 @@
       </c>
       <c r="I24">
         <f t="shared" si="1"/>
-        <v>1.4049750000000001</v>
+        <v>1.4921433333333332</v>
       </c>
       <c r="J24">
         <f t="shared" si="0"/>
-        <v>124.16615384615385</v>
+        <v>118.63850000000001</v>
+      </c>
+      <c r="K24">
+        <f>K50/5</f>
+        <v>3873.4800000000005</v>
       </c>
       <c r="N24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O24">
+        <f t="shared" si="2"/>
+        <v>0.12145466666666667</v>
+      </c>
+      <c r="P24">
+        <f t="shared" si="2"/>
+        <v>3.6889333333333334</v>
+      </c>
+      <c r="T24">
+        <v>2</v>
+      </c>
+      <c r="Z24">
+        <v>2</v>
+      </c>
+      <c r="AF24">
+        <v>2</v>
+      </c>
+      <c r="AL24">
+        <v>1</v>
+      </c>
+      <c r="AM24">
         <v>103.672</v>
       </c>
     </row>
-    <row r="25" spans="1:16">
+    <row r="25" spans="1:40">
       <c r="A25">
         <v>8</v>
       </c>
@@ -1357,23 +2030,61 @@
       </c>
       <c r="I25">
         <f t="shared" si="1"/>
-        <v>1.4050083333333332</v>
+        <v>1.4532866666666668</v>
       </c>
       <c r="J25">
         <f t="shared" si="0"/>
-        <v>119.43538461538462</v>
+        <v>117.52050000000001</v>
       </c>
       <c r="N25">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="O25">
+        <f t="shared" si="2"/>
+        <v>7.0817333333333329E-2</v>
+      </c>
+      <c r="P25">
+        <f t="shared" si="2"/>
+        <v>2.0156166666666668</v>
+      </c>
+      <c r="T25">
+        <v>4</v>
+      </c>
+      <c r="U25">
+        <v>49.619799999999998</v>
+      </c>
+      <c r="V25">
+        <v>1978.99</v>
+      </c>
+      <c r="Z25">
+        <v>4</v>
+      </c>
+      <c r="AA25">
+        <v>165.45500000000001</v>
+      </c>
+      <c r="AB25">
+        <v>5535.62</v>
+      </c>
+      <c r="AF25">
+        <v>4</v>
+      </c>
+      <c r="AG25">
+        <v>575.56100000000004</v>
+      </c>
+      <c r="AH25">
+        <v>26727.5</v>
+      </c>
+      <c r="AL25">
+        <v>2</v>
+      </c>
+      <c r="AM25">
         <v>55.442999999999998</v>
       </c>
-      <c r="P25">
+      <c r="AN25">
         <v>2431.34</v>
       </c>
     </row>
-    <row r="26" spans="1:16">
+    <row r="26" spans="1:40">
       <c r="A26">
         <v>8</v>
       </c>
@@ -1388,23 +2099,61 @@
       </c>
       <c r="I26">
         <f t="shared" si="1"/>
-        <v>1.4051</v>
+        <v>1.4858616666666666</v>
       </c>
       <c r="J26">
         <f t="shared" si="0"/>
-        <v>118.06384615384614</v>
+        <v>117.2675</v>
       </c>
       <c r="N26">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="O26">
+        <f t="shared" si="2"/>
+        <v>7.0219999999999991E-2</v>
+      </c>
+      <c r="P26">
+        <f t="shared" si="2"/>
+        <v>2.0112833333333335</v>
+      </c>
+      <c r="T26">
+        <v>4</v>
+      </c>
+      <c r="U26">
+        <v>50.363100000000003</v>
+      </c>
+      <c r="V26">
+        <v>1914.89</v>
+      </c>
+      <c r="Z26">
+        <v>4</v>
+      </c>
+      <c r="AA26">
+        <v>137.345</v>
+      </c>
+      <c r="AB26">
+        <v>5091.75</v>
+      </c>
+      <c r="AF26">
+        <v>4</v>
+      </c>
+      <c r="AG26">
+        <v>567.447</v>
+      </c>
+      <c r="AH26">
+        <v>27165.9</v>
+      </c>
+      <c r="AL26">
+        <v>2</v>
+      </c>
+      <c r="AM26">
         <v>58.367600000000003</v>
       </c>
-      <c r="P26">
+      <c r="AN26">
         <v>2334.67</v>
       </c>
     </row>
-    <row r="27" spans="1:16">
+    <row r="27" spans="1:40">
       <c r="A27">
         <v>16</v>
       </c>
@@ -1422,27 +2171,62 @@
       </c>
       <c r="I27">
         <f t="shared" si="1"/>
-        <v>0.67512916666666667</v>
+        <v>0.68832833333333332</v>
       </c>
       <c r="J27">
         <f t="shared" si="0"/>
-        <v>48.247769230769229</v>
+        <v>48.26</v>
       </c>
       <c r="K27">
-        <f>K53/5</f>
-        <v>2005.94</v>
+        <f t="shared" ref="K25:K35" si="3">K53/5</f>
+        <v>2026.2</v>
       </c>
       <c r="N27">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="O27">
+        <f t="shared" si="2"/>
+        <v>7.0446500000000009E-2</v>
+      </c>
+      <c r="P27">
+        <f t="shared" si="2"/>
+        <v>2.0166999999999997</v>
+      </c>
+      <c r="T27">
+        <v>4</v>
+      </c>
+      <c r="U27">
+        <v>51.638300000000001</v>
+      </c>
+      <c r="V27">
+        <v>1947.83</v>
+      </c>
+      <c r="Z27">
+        <v>4</v>
+      </c>
+      <c r="AA27">
+        <v>139.84700000000001</v>
+      </c>
+      <c r="AB27">
+        <v>5106.9399999999996</v>
+      </c>
+      <c r="AF27">
+        <v>4</v>
+      </c>
+      <c r="AG27">
+        <v>574.04200000000003</v>
+      </c>
+      <c r="AL27">
+        <v>2</v>
+      </c>
+      <c r="AM27">
         <v>55.547199999999997</v>
       </c>
-      <c r="P27">
+      <c r="AN27">
         <v>2322.7600000000002</v>
       </c>
     </row>
-    <row r="28" spans="1:16">
+    <row r="28" spans="1:40">
       <c r="A28">
         <v>16</v>
       </c>
@@ -1457,27 +2241,59 @@
       </c>
       <c r="I28">
         <f t="shared" si="1"/>
-        <v>0.67334499999999997</v>
+        <v>0.70209500000000002</v>
       </c>
       <c r="J28">
         <f t="shared" si="0"/>
-        <v>44.930384615384618</v>
+        <v>40.335999999999999</v>
       </c>
       <c r="K28">
-        <f>K54/5</f>
-        <v>2004.6599999999999</v>
+        <f t="shared" si="3"/>
+        <v>2057.16</v>
       </c>
       <c r="N28">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="O28">
+        <f t="shared" si="2"/>
+        <v>7.0028833333333332E-2</v>
+      </c>
+      <c r="P28">
+        <f t="shared" si="2"/>
+        <v>2.0131333333333332</v>
+      </c>
+      <c r="T28">
+        <v>4</v>
+      </c>
+      <c r="U28">
+        <v>64.099999999999994</v>
+      </c>
+      <c r="V28">
+        <v>1932.95</v>
+      </c>
+      <c r="Z28">
+        <v>4</v>
+      </c>
+      <c r="AA28">
+        <v>141.642</v>
+      </c>
+      <c r="AB28">
+        <v>5092</v>
+      </c>
+      <c r="AF28">
+        <v>4</v>
+      </c>
+      <c r="AL28">
+        <v>2</v>
+      </c>
+      <c r="AM28">
         <v>52.131100000000004</v>
       </c>
-      <c r="P28">
+      <c r="AN28">
         <v>2568.0300000000002</v>
       </c>
     </row>
-    <row r="29" spans="1:16">
+    <row r="29" spans="1:40">
       <c r="A29">
         <v>16</v>
       </c>
@@ -1492,23 +2308,43 @@
       </c>
       <c r="I29">
         <f t="shared" si="1"/>
-        <v>0.67379916666666662</v>
+        <v>0.67072000000000009</v>
       </c>
       <c r="J29">
         <f t="shared" si="0"/>
-        <v>42.254615384615377</v>
+        <v>42.962833333333329</v>
       </c>
       <c r="N29">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="O29">
+        <f t="shared" si="2"/>
+        <v>7.0458333333333331E-2</v>
+      </c>
+      <c r="P29">
+        <f t="shared" si="2"/>
+        <v>2.0175666666666667</v>
+      </c>
+      <c r="T29">
+        <v>4</v>
+      </c>
+      <c r="Z29">
+        <v>4</v>
+      </c>
+      <c r="AF29">
+        <v>4</v>
+      </c>
+      <c r="AL29">
+        <v>2</v>
+      </c>
+      <c r="AM29">
         <v>59.497700000000002</v>
       </c>
-      <c r="P29">
+      <c r="AN29">
         <v>2313.0500000000002</v>
       </c>
     </row>
-    <row r="30" spans="1:16">
+    <row r="30" spans="1:40">
       <c r="A30">
         <v>32</v>
       </c>
@@ -1525,28 +2361,69 @@
         <v>32</v>
       </c>
       <c r="I30">
-        <f>I56/6</f>
-        <v>0.33262666666666668</v>
+        <f t="shared" si="1"/>
+        <v>0.36327333333333334</v>
       </c>
       <c r="J30">
         <f t="shared" si="0"/>
-        <v>38.402846153846156</v>
+        <v>23.622333333333334</v>
       </c>
       <c r="K30">
-        <f>K56/5</f>
-        <v>2004.1</v>
+        <f t="shared" si="3"/>
+        <v>1018.1420000000001</v>
       </c>
       <c r="N30">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="O30">
+        <f t="shared" si="2"/>
+        <v>3.5843E-2</v>
+      </c>
+      <c r="P30">
+        <f t="shared" si="2"/>
+        <v>1.0692066666666666</v>
+      </c>
+      <c r="T30">
+        <v>8</v>
+      </c>
+      <c r="U30">
+        <v>17.361499999999999</v>
+      </c>
+      <c r="V30">
+        <v>632.78899999999999</v>
+      </c>
+      <c r="W30">
+        <v>23233</v>
+      </c>
+      <c r="Z30">
+        <v>8</v>
+      </c>
+      <c r="AA30">
+        <v>42.23</v>
+      </c>
+      <c r="AB30">
+        <v>1640.08</v>
+      </c>
+      <c r="AF30">
+        <v>8</v>
+      </c>
+      <c r="AG30">
+        <v>214.79300000000001</v>
+      </c>
+      <c r="AH30">
+        <v>11377.8</v>
+      </c>
+      <c r="AL30">
+        <v>2</v>
+      </c>
+      <c r="AM30">
         <v>53.045299999999997</v>
       </c>
-      <c r="P30">
+      <c r="AN30">
         <v>2288.2399999999998</v>
       </c>
     </row>
-    <row r="31" spans="1:16">
+    <row r="31" spans="1:40">
       <c r="A31">
         <v>32</v>
       </c>
@@ -1560,28 +2437,62 @@
         <v>32</v>
       </c>
       <c r="I31">
-        <f>I57/6</f>
-        <v>0.33597000000000005</v>
-      </c>
-      <c r="J31">
-        <f t="shared" si="0"/>
-        <v>35.460615384615387</v>
+        <f t="shared" si="1"/>
+        <v>0.37943333333333334</v>
       </c>
       <c r="K31">
-        <f>K57/5</f>
-        <v>2009.48</v>
+        <f t="shared" si="3"/>
+        <v>921.78199999999993</v>
       </c>
       <c r="N31">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="O31">
+        <f t="shared" si="2"/>
+        <v>3.5554666666666665E-2</v>
+      </c>
+      <c r="P31">
+        <f t="shared" si="2"/>
+        <v>1.0697650000000001</v>
+      </c>
+      <c r="T31">
+        <v>8</v>
+      </c>
+      <c r="U31">
+        <v>19.6265</v>
+      </c>
+      <c r="V31">
+        <v>615.34100000000001</v>
+      </c>
+      <c r="Z31">
+        <v>8</v>
+      </c>
+      <c r="AA31">
+        <v>53.9011</v>
+      </c>
+      <c r="AB31">
+        <v>1654.56</v>
+      </c>
+      <c r="AF31">
+        <v>8</v>
+      </c>
+      <c r="AG31">
+        <v>217.55799999999999</v>
+      </c>
+      <c r="AH31">
+        <v>11059.3</v>
+      </c>
+      <c r="AL31">
+        <v>2</v>
+      </c>
+      <c r="AM31">
         <v>53.076799999999999</v>
       </c>
-      <c r="P31">
+      <c r="AN31">
         <v>2535.4699999999998</v>
       </c>
     </row>
-    <row r="32" spans="1:16">
+    <row r="32" spans="1:40">
       <c r="A32">
         <v>32</v>
       </c>
@@ -1595,24 +2506,59 @@
         <v>32</v>
       </c>
       <c r="I32">
-        <f>I58/6</f>
-        <v>0.33126</v>
-      </c>
-      <c r="J32">
-        <f t="shared" si="0"/>
-        <v>34.784769230769228</v>
+        <f t="shared" si="1"/>
+        <v>0.36234000000000005</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="3"/>
+        <v>926.99799999999993</v>
       </c>
       <c r="N32">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="O32">
+        <f t="shared" si="2"/>
+        <v>3.5790166666666665E-2</v>
+      </c>
+      <c r="P32">
+        <f t="shared" si="2"/>
+        <v>1.0616366666666666</v>
+      </c>
+      <c r="T32">
+        <v>8</v>
+      </c>
+      <c r="U32">
+        <v>18.945699999999999</v>
+      </c>
+      <c r="V32">
+        <v>648.80600000000004</v>
+      </c>
+      <c r="Z32">
+        <v>8</v>
+      </c>
+      <c r="AA32">
+        <v>44.323599999999999</v>
+      </c>
+      <c r="AB32">
+        <v>1649.74</v>
+      </c>
+      <c r="AF32">
+        <v>8</v>
+      </c>
+      <c r="AG32">
+        <v>207.96</v>
+      </c>
+      <c r="AL32">
+        <v>2</v>
+      </c>
+      <c r="AM32">
         <v>51.253300000000003</v>
       </c>
-      <c r="P32">
+      <c r="AN32">
         <v>2552.4699999999998</v>
       </c>
     </row>
-    <row r="33" spans="1:16">
+    <row r="33" spans="1:40">
       <c r="A33">
         <v>64</v>
       </c>
@@ -1629,28 +2575,63 @@
         <v>64</v>
       </c>
       <c r="I33">
-        <f t="shared" ref="I33:J35" si="2">I59/6</f>
-        <v>0.16703666666666669</v>
+        <f t="shared" si="1"/>
+        <v>0.17820499999999997</v>
       </c>
       <c r="J33">
-        <f t="shared" si="2"/>
-        <v>5.7520500000000006</v>
+        <f t="shared" si="0"/>
+        <v>5.1360166666666665</v>
       </c>
       <c r="K33">
-        <f>K59/5</f>
-        <v>931.41399999999999</v>
+        <f t="shared" si="3"/>
+        <v>391.11599999999999</v>
       </c>
       <c r="N33">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="O33">
+        <f t="shared" si="2"/>
+        <v>3.5815E-2</v>
+      </c>
+      <c r="P33">
+        <f t="shared" si="2"/>
+        <v>1.0692233333333332</v>
+      </c>
+      <c r="T33">
+        <v>8</v>
+      </c>
+      <c r="U33">
+        <v>17.2651</v>
+      </c>
+      <c r="V33">
+        <v>620.27300000000002</v>
+      </c>
+      <c r="Z33">
+        <v>8</v>
+      </c>
+      <c r="AA33">
+        <v>54.658999999999999</v>
+      </c>
+      <c r="AB33">
+        <v>1650.27</v>
+      </c>
+      <c r="AF33">
+        <v>8</v>
+      </c>
+      <c r="AG33">
+        <v>220.911</v>
+      </c>
+      <c r="AL33">
+        <v>2</v>
+      </c>
+      <c r="AM33">
         <v>62.247100000000003</v>
       </c>
-      <c r="P33">
+      <c r="AN33">
         <v>2568.02</v>
       </c>
     </row>
-    <row r="34" spans="1:16">
+    <row r="34" spans="1:40">
       <c r="A34">
         <v>64</v>
       </c>
@@ -1667,28 +2648,48 @@
         <v>64</v>
       </c>
       <c r="I34">
-        <f t="shared" si="2"/>
-        <v>0.16784333333333334</v>
+        <f t="shared" si="1"/>
+        <v>0.19303666666666666</v>
       </c>
       <c r="J34">
-        <f t="shared" si="2"/>
-        <v>4.4872833333333331</v>
+        <f t="shared" si="0"/>
+        <v>4.9707833333333333</v>
       </c>
       <c r="K34">
-        <f>K60/5</f>
-        <v>941.99</v>
+        <f t="shared" si="3"/>
+        <v>393.416</v>
       </c>
       <c r="N34">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="O34">
+        <f t="shared" si="2"/>
+        <v>3.5753666666666663E-2</v>
+      </c>
+      <c r="P34">
+        <f t="shared" si="2"/>
+        <v>1.0697733333333332</v>
+      </c>
+      <c r="T34">
+        <v>8</v>
+      </c>
+      <c r="Z34">
+        <v>8</v>
+      </c>
+      <c r="AF34">
+        <v>8</v>
+      </c>
+      <c r="AL34">
+        <v>2</v>
+      </c>
+      <c r="AM34">
         <v>66.199399999999997</v>
       </c>
-      <c r="P34">
+      <c r="AN34">
         <v>2349.69</v>
       </c>
     </row>
-    <row r="35" spans="1:16">
+    <row r="35" spans="1:40">
       <c r="A35">
         <v>64</v>
       </c>
@@ -1705,28 +2706,72 @@
         <v>64</v>
       </c>
       <c r="I35">
-        <f t="shared" si="2"/>
-        <v>0.16767166666666666</v>
+        <f t="shared" si="1"/>
+        <v>0.18193499999999999</v>
       </c>
       <c r="J35">
-        <f t="shared" si="2"/>
-        <v>4.7301500000000001</v>
+        <f t="shared" si="0"/>
+        <v>4.9496500000000001</v>
       </c>
       <c r="K35">
-        <f>K61/5</f>
-        <v>955.12000000000012</v>
+        <f t="shared" si="3"/>
+        <v>389.666</v>
       </c>
       <c r="N35">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="O35">
+        <f t="shared" si="2"/>
+        <v>1.8580333333333334E-2</v>
+      </c>
+      <c r="P35">
+        <f t="shared" si="2"/>
+        <v>0.57930166666666671</v>
+      </c>
+      <c r="T35">
+        <v>16</v>
+      </c>
+      <c r="U35">
+        <v>4.4084099999999999</v>
+      </c>
+      <c r="V35">
+        <v>256.834</v>
+      </c>
+      <c r="W35">
+        <v>11137.1</v>
+      </c>
+      <c r="Z35">
+        <v>16</v>
+      </c>
+      <c r="AA35">
+        <v>11.3919</v>
+      </c>
+      <c r="AB35">
+        <v>726.06</v>
+      </c>
+      <c r="AC35">
+        <v>28453</v>
+      </c>
+      <c r="AF35">
+        <v>16</v>
+      </c>
+      <c r="AG35">
+        <v>84.037300000000002</v>
+      </c>
+      <c r="AH35">
+        <v>5599.24</v>
+      </c>
+      <c r="AL35">
+        <v>4</v>
+      </c>
+      <c r="AM35">
         <v>14.6533</v>
       </c>
-      <c r="P35">
+      <c r="AN35">
         <v>979.43600000000004</v>
       </c>
     </row>
-    <row r="36" spans="1:16">
+    <row r="36" spans="1:40">
       <c r="A36">
         <v>124</v>
       </c>
@@ -1740,24 +2785,65 @@
         <v>124</v>
       </c>
       <c r="I36">
-        <f t="shared" si="1"/>
-        <v>0.15416166666666667</v>
+        <f t="shared" ref="I16:I38" si="4">I62/12</f>
+        <v>0</v>
       </c>
       <c r="J36">
-        <f t="shared" si="0"/>
-        <v>2.1879153846153847</v>
+        <f t="shared" ref="J15:J38" si="5">J62/13</f>
+        <v>0</v>
       </c>
       <c r="N36">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="O36">
+        <f t="shared" si="2"/>
+        <v>1.847E-2</v>
+      </c>
+      <c r="P36">
+        <f t="shared" si="2"/>
+        <v>0.57502500000000001</v>
+      </c>
+      <c r="T36">
+        <v>16</v>
+      </c>
+      <c r="U36">
+        <v>4.0432499999999996</v>
+      </c>
+      <c r="V36">
+        <v>247.46799999999999</v>
+      </c>
+      <c r="W36">
+        <v>11047.7</v>
+      </c>
+      <c r="Z36">
+        <v>16</v>
+      </c>
+      <c r="AA36">
+        <v>13.485099999999999</v>
+      </c>
+      <c r="AB36">
+        <v>733.28899999999999</v>
+      </c>
+      <c r="AF36">
+        <v>16</v>
+      </c>
+      <c r="AG36">
+        <v>83.993799999999993</v>
+      </c>
+      <c r="AH36">
+        <v>5615.84</v>
+      </c>
+      <c r="AL36">
+        <v>4</v>
+      </c>
+      <c r="AM36">
         <v>13.579599999999999</v>
       </c>
-      <c r="P36">
+      <c r="AN36">
         <v>915.13</v>
       </c>
     </row>
-    <row r="37" spans="1:16">
+    <row r="37" spans="1:40">
       <c r="A37">
         <v>124</v>
       </c>
@@ -1771,24 +2857,62 @@
         <v>124</v>
       </c>
       <c r="I37">
-        <f t="shared" si="1"/>
-        <v>0.15224750000000001</v>
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
       <c r="J37">
-        <f t="shared" si="0"/>
-        <v>4.9603307692307697</v>
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
       <c r="N37">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="O37">
+        <f t="shared" si="2"/>
+        <v>1.8494E-2</v>
+      </c>
+      <c r="P37">
+        <f t="shared" si="2"/>
+        <v>0.57332666666666665</v>
+      </c>
+      <c r="T37">
+        <v>16</v>
+      </c>
+      <c r="U37">
+        <v>4.0551399999999997</v>
+      </c>
+      <c r="V37">
+        <v>244.07900000000001</v>
+      </c>
+      <c r="Z37">
+        <v>16</v>
+      </c>
+      <c r="AA37">
+        <v>12.716699999999999</v>
+      </c>
+      <c r="AB37">
+        <v>704.52599999999995</v>
+      </c>
+      <c r="AF37">
+        <v>16</v>
+      </c>
+      <c r="AG37">
+        <v>88.934600000000003</v>
+      </c>
+      <c r="AH37">
+        <v>5816.1</v>
+      </c>
+      <c r="AL37">
+        <v>4</v>
+      </c>
+      <c r="AM37">
         <v>13.036099999999999</v>
       </c>
-      <c r="P37">
+      <c r="AN37">
         <v>952.69600000000003</v>
       </c>
     </row>
-    <row r="38" spans="1:16">
+    <row r="38" spans="1:40">
       <c r="A38">
         <v>124</v>
       </c>
@@ -1802,132 +2926,423 @@
         <v>124</v>
       </c>
       <c r="I38">
-        <f t="shared" si="1"/>
-        <v>0.15227166666666667</v>
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
       <c r="J38">
-        <f t="shared" si="0"/>
-        <v>2.2266538461538463</v>
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
       <c r="N38">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="O38">
+        <f t="shared" si="2"/>
+        <v>1.8281666666666665E-2</v>
+      </c>
+      <c r="P38">
+        <f t="shared" si="2"/>
+        <v>0.56794</v>
+      </c>
+      <c r="T38">
+        <v>16</v>
+      </c>
+      <c r="U38">
+        <v>4.0430299999999999</v>
+      </c>
+      <c r="V38">
+        <v>249.995</v>
+      </c>
+      <c r="Z38">
+        <v>16</v>
+      </c>
+      <c r="AA38">
+        <v>11.480399999999999</v>
+      </c>
+      <c r="AB38">
+        <v>721.29200000000003</v>
+      </c>
+      <c r="AF38">
+        <v>16</v>
+      </c>
+      <c r="AG38">
+        <v>85.170299999999997</v>
+      </c>
+      <c r="AH38">
+        <v>11366.1</v>
+      </c>
+      <c r="AL38">
+        <v>4</v>
+      </c>
+      <c r="AM38">
         <v>12.4773</v>
       </c>
-      <c r="P38">
+      <c r="AN38">
         <v>921.92700000000002</v>
       </c>
     </row>
-    <row r="39" spans="1:16">
+    <row r="39" spans="1:40">
       <c r="N39">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="O39">
+        <f t="shared" si="2"/>
+        <v>1.8302666666666665E-2</v>
+      </c>
+      <c r="P39">
+        <f t="shared" si="2"/>
+        <v>0.56923166666666669</v>
+      </c>
+      <c r="T39">
+        <v>16</v>
+      </c>
+      <c r="U39">
+        <v>4.08188</v>
+      </c>
+      <c r="V39">
+        <v>259.125</v>
+      </c>
+      <c r="Z39">
+        <v>16</v>
+      </c>
+      <c r="AA39">
+        <v>11.5585</v>
+      </c>
+      <c r="AB39">
+        <v>709.125</v>
+      </c>
+      <c r="AF39">
+        <v>16</v>
+      </c>
+      <c r="AG39">
+        <v>83.458200000000005</v>
+      </c>
+      <c r="AH39">
+        <v>11323.5</v>
+      </c>
+      <c r="AL39">
+        <v>4</v>
+      </c>
+      <c r="AM39">
         <v>14.1136</v>
       </c>
-      <c r="P39">
+      <c r="AN39">
         <v>831.79399999999998</v>
       </c>
     </row>
-    <row r="40" spans="1:16">
+    <row r="40" spans="1:40">
       <c r="B40" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="N40">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="O40">
+        <f t="shared" si="2"/>
+        <v>9.3031666666666662E-3</v>
+      </c>
+      <c r="P40">
+        <f t="shared" si="2"/>
+        <v>0.30254500000000001</v>
+      </c>
+      <c r="T40">
+        <v>32</v>
+      </c>
+      <c r="U40">
+        <v>2.11591</v>
+      </c>
+      <c r="V40">
+        <v>157.404</v>
+      </c>
+      <c r="W40">
+        <v>5706.38</v>
+      </c>
+      <c r="Z40">
+        <v>32</v>
+      </c>
+      <c r="AA40">
+        <v>7.3185799999999999</v>
+      </c>
+      <c r="AB40">
+        <v>428.51100000000002</v>
+      </c>
+      <c r="AC40">
+        <v>14250.5</v>
+      </c>
+      <c r="AF40">
+        <v>32</v>
+      </c>
+      <c r="AG40">
+        <v>43.302900000000001</v>
+      </c>
+      <c r="AH40">
+        <v>6579.71</v>
+      </c>
+      <c r="AL40">
+        <v>4</v>
+      </c>
+      <c r="AM40">
         <v>11.9115</v>
       </c>
-      <c r="P40">
+      <c r="AN40">
         <v>930.94200000000001</v>
       </c>
     </row>
-    <row r="41" spans="1:16">
+    <row r="41" spans="1:40">
       <c r="H41">
         <v>1</v>
       </c>
-      <c r="I41">
-        <v>359.10500000000002</v>
-      </c>
-      <c r="J41">
-        <v>19936.5</v>
-      </c>
+      <c r="I41" s="7">
+        <v>175.54400000000001</v>
+      </c>
+      <c r="J41" s="7">
+        <v>9153.82</v>
+      </c>
+      <c r="K41" s="7"/>
       <c r="N41">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="O41">
+        <f t="shared" si="2"/>
+        <v>9.3416833333333331E-3</v>
+      </c>
+      <c r="P41">
+        <f t="shared" si="2"/>
+        <v>0.29609000000000002</v>
+      </c>
+      <c r="T41">
+        <v>32</v>
+      </c>
+      <c r="U41">
+        <v>2.0946899999999999</v>
+      </c>
+      <c r="V41">
+        <v>132.84100000000001</v>
+      </c>
+      <c r="W41">
+        <v>5761.53</v>
+      </c>
+      <c r="Z41">
+        <v>32</v>
+      </c>
+      <c r="AA41">
+        <v>7.2561400000000003</v>
+      </c>
+      <c r="AB41">
+        <v>433.798</v>
+      </c>
+      <c r="AC41">
+        <v>14251.1</v>
+      </c>
+      <c r="AF41">
+        <v>32</v>
+      </c>
+      <c r="AG41">
+        <v>50.503300000000003</v>
+      </c>
+      <c r="AH41">
+        <v>6625.19</v>
+      </c>
+      <c r="AL41">
+        <v>4</v>
+      </c>
+      <c r="AM41">
         <v>13.3255</v>
       </c>
-      <c r="P41">
+      <c r="AN41">
         <v>849.98199999999997</v>
       </c>
     </row>
-    <row r="42" spans="1:16">
+    <row r="42" spans="1:40">
       <c r="H42">
         <v>1</v>
       </c>
-      <c r="I42">
-        <v>352.875</v>
-      </c>
-      <c r="J42">
-        <v>19494.7</v>
-      </c>
+      <c r="I42" s="7">
+        <v>169.36600000000001</v>
+      </c>
+      <c r="J42" s="7">
+        <v>9209.94</v>
+      </c>
+      <c r="K42" s="7"/>
       <c r="N42">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="O42">
+        <f t="shared" si="2"/>
+        <v>9.3135000000000006E-3</v>
+      </c>
+      <c r="P42">
+        <f t="shared" si="2"/>
+        <v>0.29515333333333332</v>
+      </c>
+      <c r="T42">
+        <v>32</v>
+      </c>
+      <c r="U42">
+        <v>2.1623999999999999</v>
+      </c>
+      <c r="V42">
+        <v>127.85599999999999</v>
+      </c>
+      <c r="W42">
+        <v>5715.92</v>
+      </c>
+      <c r="Z42">
+        <v>32</v>
+      </c>
+      <c r="AA42">
+        <v>6.3373400000000002</v>
+      </c>
+      <c r="AB42">
+        <v>415.45299999999997</v>
+      </c>
+      <c r="AF42">
+        <v>32</v>
+      </c>
+      <c r="AG42">
+        <v>92.506</v>
+      </c>
+      <c r="AH42">
+        <v>6287.75</v>
+      </c>
+      <c r="AL42">
+        <v>4</v>
+      </c>
+      <c r="AM42">
         <v>12.174899999999999</v>
       </c>
-      <c r="P42">
+      <c r="AN42">
         <v>1012.83</v>
       </c>
     </row>
-    <row r="43" spans="1:16">
+    <row r="43" spans="1:40">
       <c r="A43" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H43">
         <v>1</v>
       </c>
-      <c r="I43">
-        <v>356.05099999999999</v>
-      </c>
-      <c r="J43">
-        <v>20001</v>
-      </c>
+      <c r="I43" s="7">
+        <v>168.654</v>
+      </c>
+      <c r="J43" s="7">
+        <v>9166.4500000000007</v>
+      </c>
+      <c r="K43" s="7"/>
       <c r="N43">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="O43">
+        <f t="shared" si="2"/>
+        <v>9.3267000000000003E-3</v>
+      </c>
+      <c r="P43">
+        <f t="shared" si="2"/>
+        <v>0.29547166666666663</v>
+      </c>
+      <c r="T43">
+        <v>32</v>
+      </c>
+      <c r="U43">
+        <v>2.12507</v>
+      </c>
+      <c r="V43">
+        <v>149.95599999999999</v>
+      </c>
+      <c r="W43">
+        <v>5715.39</v>
+      </c>
+      <c r="Z43">
+        <v>32</v>
+      </c>
+      <c r="AA43">
+        <v>6.3307099999999998</v>
+      </c>
+      <c r="AB43">
+        <v>392.87299999999999</v>
+      </c>
+      <c r="AF43">
+        <v>32</v>
+      </c>
+      <c r="AG43">
+        <v>48.465600000000002</v>
+      </c>
+      <c r="AH43">
+        <v>6504.61</v>
+      </c>
+      <c r="AL43">
+        <v>4</v>
+      </c>
+      <c r="AM43">
         <v>12.4872</v>
       </c>
-      <c r="P43">
+      <c r="AN43">
         <v>930.60199999999998</v>
       </c>
     </row>
-    <row r="44" spans="1:16">
+    <row r="44" spans="1:40">
       <c r="H44">
         <v>2</v>
       </c>
-      <c r="I44">
-        <v>201.13900000000001</v>
-      </c>
-      <c r="J44">
-        <v>10399.1</v>
-      </c>
+      <c r="I44" s="7">
+        <v>94.716200000000001</v>
+      </c>
+      <c r="J44" s="7">
+        <v>4932.71</v>
+      </c>
+      <c r="K44" s="7"/>
       <c r="N44">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="O44">
+        <f t="shared" si="2"/>
+        <v>9.3301500000000006E-3</v>
+      </c>
+      <c r="P44">
+        <f t="shared" si="2"/>
+        <v>0.29611999999999999</v>
+      </c>
+      <c r="T44">
+        <v>32</v>
+      </c>
+      <c r="U44">
+        <v>2.0856300000000001</v>
+      </c>
+      <c r="V44">
+        <v>141.68100000000001</v>
+      </c>
+      <c r="W44">
+        <v>5730.66</v>
+      </c>
+      <c r="Z44">
+        <v>32</v>
+      </c>
+      <c r="AA44">
+        <v>7.31996</v>
+      </c>
+      <c r="AB44">
+        <v>408.35199999999998</v>
+      </c>
+      <c r="AF44">
+        <v>32</v>
+      </c>
+      <c r="AG44">
+        <v>90.778400000000005</v>
+      </c>
+      <c r="AH44">
+        <v>6560.15</v>
+      </c>
+      <c r="AL44">
+        <v>4</v>
+      </c>
+      <c r="AM44">
         <v>12.4079</v>
       </c>
-      <c r="P44">
+      <c r="AN44">
         <v>920.67</v>
       </c>
     </row>
-    <row r="45" spans="1:16">
+    <row r="45" spans="1:40">
       <c r="A45">
         <v>1</v>
       </c>
@@ -1946,23 +3361,68 @@
       <c r="H45">
         <v>2</v>
       </c>
-      <c r="I45">
-        <v>193.624</v>
-      </c>
-      <c r="J45">
-        <v>10227.4</v>
-      </c>
+      <c r="I45" s="7">
+        <v>94.711600000000004</v>
+      </c>
+      <c r="J45" s="7">
+        <v>4911.26</v>
+      </c>
+      <c r="K45" s="7"/>
       <c r="N45">
-        <v>8</v>
+        <v>64</v>
       </c>
       <c r="O45">
+        <f t="shared" si="2"/>
+        <v>4.9721833333333338E-3</v>
+      </c>
+      <c r="P45">
+        <f t="shared" si="2"/>
+        <v>0.15278149999999999</v>
+      </c>
+      <c r="T45">
+        <v>64</v>
+      </c>
+      <c r="U45">
+        <v>1.1104099999999999</v>
+      </c>
+      <c r="V45">
+        <v>123.077</v>
+      </c>
+      <c r="W45">
+        <v>5881.01</v>
+      </c>
+      <c r="Z45">
+        <v>64</v>
+      </c>
+      <c r="AA45">
+        <v>5.7715800000000002</v>
+      </c>
+      <c r="AB45">
+        <v>404.69400000000002</v>
+      </c>
+      <c r="AC45">
+        <v>15893.7</v>
+      </c>
+      <c r="AF45">
+        <v>64</v>
+      </c>
+      <c r="AG45">
+        <v>25.3552</v>
+      </c>
+      <c r="AH45">
+        <v>3306.35</v>
+      </c>
+      <c r="AL45">
+        <v>8</v>
+      </c>
+      <c r="AM45">
         <v>4.3688799999999999</v>
       </c>
-      <c r="P45">
+      <c r="AN45">
         <v>396.84199999999998</v>
       </c>
     </row>
-    <row r="46" spans="1:16">
+    <row r="46" spans="1:40">
       <c r="A46">
         <v>1</v>
       </c>
@@ -1978,23 +3438,68 @@
       <c r="H46">
         <v>2</v>
       </c>
-      <c r="I46">
-        <v>203.61799999999999</v>
-      </c>
-      <c r="J46">
-        <v>10282.799999999999</v>
-      </c>
+      <c r="I46" s="7">
+        <v>101.22799999999999</v>
+      </c>
+      <c r="J46" s="7">
+        <v>4902.7299999999996</v>
+      </c>
+      <c r="K46" s="7"/>
       <c r="N46">
-        <v>8</v>
+        <v>64</v>
       </c>
       <c r="O46">
+        <f t="shared" si="2"/>
+        <v>4.9183333333333336E-3</v>
+      </c>
+      <c r="P46">
+        <f t="shared" si="2"/>
+        <v>0.151531</v>
+      </c>
+      <c r="T46">
+        <v>64</v>
+      </c>
+      <c r="U46">
+        <v>1.1018600000000001</v>
+      </c>
+      <c r="V46">
+        <v>123.081</v>
+      </c>
+      <c r="W46">
+        <v>5974.55</v>
+      </c>
+      <c r="Z46">
+        <v>64</v>
+      </c>
+      <c r="AA46">
+        <v>5.7947699999999998</v>
+      </c>
+      <c r="AB46">
+        <v>447.16699999999997</v>
+      </c>
+      <c r="AC46">
+        <v>15834.4</v>
+      </c>
+      <c r="AF46">
+        <v>64</v>
+      </c>
+      <c r="AG46">
+        <v>38.870600000000003</v>
+      </c>
+      <c r="AH46">
+        <v>3320.09</v>
+      </c>
+      <c r="AL46">
+        <v>8</v>
+      </c>
+      <c r="AM46">
         <v>3.9904500000000001</v>
       </c>
-      <c r="P46">
+      <c r="AN46">
         <v>442.767</v>
       </c>
     </row>
-    <row r="47" spans="1:16">
+    <row r="47" spans="1:40">
       <c r="A47">
         <v>1</v>
       </c>
@@ -2010,23 +3515,65 @@
       <c r="H47">
         <v>4</v>
       </c>
-      <c r="I47">
-        <v>42.457099999999997</v>
-      </c>
-      <c r="J47">
-        <v>4628.01</v>
-      </c>
+      <c r="I47" s="7">
+        <v>25.995999999999999</v>
+      </c>
+      <c r="J47" s="7">
+        <v>1910.93</v>
+      </c>
+      <c r="K47" s="7"/>
       <c r="N47">
-        <v>8</v>
+        <v>64</v>
       </c>
       <c r="O47">
+        <f t="shared" si="2"/>
+        <v>4.9338333333333335E-3</v>
+      </c>
+      <c r="P47">
+        <f t="shared" si="2"/>
+        <v>0.14907566666666666</v>
+      </c>
+      <c r="T47">
+        <v>64</v>
+      </c>
+      <c r="U47">
+        <v>1.12337</v>
+      </c>
+      <c r="V47">
+        <v>138.62299999999999</v>
+      </c>
+      <c r="W47">
+        <v>6051.43</v>
+      </c>
+      <c r="Z47">
+        <v>64</v>
+      </c>
+      <c r="AA47">
+        <v>5.8171299999999997</v>
+      </c>
+      <c r="AB47">
+        <v>470.76</v>
+      </c>
+      <c r="AF47">
+        <v>64</v>
+      </c>
+      <c r="AG47">
+        <v>55.764499999999998</v>
+      </c>
+      <c r="AH47">
+        <v>3350.89</v>
+      </c>
+      <c r="AL47">
+        <v>8</v>
+      </c>
+      <c r="AM47">
         <v>4.00162</v>
       </c>
-      <c r="P47">
+      <c r="AN47">
         <v>398.834</v>
       </c>
     </row>
-    <row r="48" spans="1:16">
+    <row r="48" spans="1:40">
       <c r="A48">
         <v>1</v>
       </c>
@@ -2042,23 +3589,65 @@
       <c r="H48">
         <v>4</v>
       </c>
-      <c r="I48">
-        <v>50.296799999999998</v>
-      </c>
-      <c r="J48">
-        <v>4729.1000000000004</v>
-      </c>
+      <c r="I48" s="7">
+        <v>24.286300000000001</v>
+      </c>
+      <c r="J48" s="7">
+        <v>1917.57</v>
+      </c>
+      <c r="K48" s="7"/>
       <c r="N48">
-        <v>8</v>
+        <v>64</v>
       </c>
       <c r="O48">
+        <f t="shared" si="2"/>
+        <v>4.9621666666666668E-3</v>
+      </c>
+      <c r="P48">
+        <f t="shared" si="2"/>
+        <v>0.14682100000000001</v>
+      </c>
+      <c r="T48">
+        <v>64</v>
+      </c>
+      <c r="U48">
+        <v>1.0958000000000001</v>
+      </c>
+      <c r="V48">
+        <v>153.887</v>
+      </c>
+      <c r="W48">
+        <v>5888.11</v>
+      </c>
+      <c r="Z48">
+        <v>64</v>
+      </c>
+      <c r="AA48">
+        <v>7.1295200000000003</v>
+      </c>
+      <c r="AB48">
+        <v>524.46900000000005</v>
+      </c>
+      <c r="AF48">
+        <v>64</v>
+      </c>
+      <c r="AG48">
+        <v>24.578600000000002</v>
+      </c>
+      <c r="AH48">
+        <v>3461.02</v>
+      </c>
+      <c r="AL48">
+        <v>8</v>
+      </c>
+      <c r="AM48">
         <v>4.0081800000000003</v>
       </c>
-      <c r="P48">
+      <c r="AN48">
         <v>416.49299999999999</v>
       </c>
     </row>
-    <row r="49" spans="1:16">
+    <row r="49" spans="1:40">
       <c r="A49">
         <v>1</v>
       </c>
@@ -2074,23 +3663,65 @@
       <c r="H49">
         <v>4</v>
       </c>
-      <c r="I49">
-        <v>57.620800000000003</v>
-      </c>
-      <c r="J49">
-        <v>4653.9799999999996</v>
-      </c>
+      <c r="I49" s="7">
+        <v>26.204599999999999</v>
+      </c>
+      <c r="J49" s="7">
+        <v>2048.13</v>
+      </c>
+      <c r="K49" s="7"/>
       <c r="N49">
-        <v>8</v>
+        <v>64</v>
       </c>
       <c r="O49">
+        <f t="shared" si="2"/>
+        <v>4.9443166666666661E-3</v>
+      </c>
+      <c r="P49">
+        <f t="shared" si="2"/>
+        <v>0.14617050000000001</v>
+      </c>
+      <c r="T49">
+        <v>64</v>
+      </c>
+      <c r="U49">
+        <v>1.11053</v>
+      </c>
+      <c r="V49">
+        <v>147.714</v>
+      </c>
+      <c r="W49">
+        <v>6079.96</v>
+      </c>
+      <c r="Z49">
+        <v>64</v>
+      </c>
+      <c r="AA49">
+        <v>6.6221800000000002</v>
+      </c>
+      <c r="AB49">
+        <v>507.31099999999998</v>
+      </c>
+      <c r="AF49">
+        <v>64</v>
+      </c>
+      <c r="AG49">
+        <v>42.098399999999998</v>
+      </c>
+      <c r="AH49">
+        <v>3416.48</v>
+      </c>
+      <c r="AL49">
+        <v>8</v>
+      </c>
+      <c r="AM49">
         <v>4.0179999999999998</v>
       </c>
-      <c r="P49">
+      <c r="AN49">
         <v>414.233</v>
       </c>
     </row>
-    <row r="50" spans="1:16">
+    <row r="50" spans="1:40">
       <c r="A50">
         <v>2</v>
       </c>
@@ -2109,23 +3740,26 @@
       <c r="H50">
         <v>8</v>
       </c>
-      <c r="I50">
-        <v>16.8597</v>
-      </c>
-      <c r="J50">
-        <v>1614.16</v>
-      </c>
-      <c r="N50">
-        <v>8</v>
-      </c>
-      <c r="O50">
+      <c r="I50" s="7">
+        <v>8.9528599999999994</v>
+      </c>
+      <c r="J50" s="7">
+        <v>711.83100000000002</v>
+      </c>
+      <c r="K50" s="7">
+        <v>19367.400000000001</v>
+      </c>
+      <c r="AL50">
+        <v>8</v>
+      </c>
+      <c r="AM50">
         <v>4.30192</v>
       </c>
-      <c r="P50">
+      <c r="AN50">
         <v>404.476</v>
       </c>
     </row>
-    <row r="51" spans="1:16">
+    <row r="51" spans="1:40">
       <c r="A51">
         <v>2</v>
       </c>
@@ -2141,23 +3775,30 @@
       <c r="H51">
         <v>8</v>
       </c>
-      <c r="I51">
-        <v>16.860099999999999</v>
-      </c>
-      <c r="J51">
-        <v>1552.66</v>
-      </c>
+      <c r="I51" s="7">
+        <v>8.7197200000000006</v>
+      </c>
+      <c r="J51" s="7">
+        <v>705.12300000000005</v>
+      </c>
+      <c r="K51" s="7"/>
       <c r="N51">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="O51">
+        <v>1.82941</v>
+      </c>
+      <c r="AL51">
+        <v>8</v>
+      </c>
+      <c r="AM51">
         <v>3.9927600000000001</v>
       </c>
-      <c r="P51">
+      <c r="AN51">
         <v>402.28399999999999</v>
       </c>
     </row>
-    <row r="52" spans="1:16">
+    <row r="52" spans="1:40">
       <c r="A52">
         <v>2</v>
       </c>
@@ -2173,23 +3814,30 @@
       <c r="H52">
         <v>8</v>
       </c>
-      <c r="I52">
-        <v>16.8612</v>
-      </c>
-      <c r="J52">
-        <v>1534.83</v>
-      </c>
+      <c r="I52" s="7">
+        <v>8.9151699999999998</v>
+      </c>
+      <c r="J52" s="7">
+        <v>703.60500000000002</v>
+      </c>
+      <c r="K52" s="7"/>
       <c r="N52">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="O52">
+        <v>1.8195399999999999</v>
+      </c>
+      <c r="AL52">
+        <v>8</v>
+      </c>
+      <c r="AM52">
         <v>3.9741200000000001</v>
       </c>
-      <c r="P52">
+      <c r="AN52">
         <v>401.87599999999998</v>
       </c>
     </row>
-    <row r="53" spans="1:16">
+    <row r="53" spans="1:40">
       <c r="A53">
         <v>2</v>
       </c>
@@ -2205,26 +3853,32 @@
       <c r="H53">
         <v>16</v>
       </c>
-      <c r="I53">
-        <v>8.1015499999999996</v>
-      </c>
-      <c r="J53">
-        <v>627.221</v>
-      </c>
-      <c r="K53" s="3">
-        <v>10029.700000000001</v>
+      <c r="I53" s="7">
+        <v>4.1299700000000001</v>
+      </c>
+      <c r="J53" s="7">
+        <v>289.56</v>
+      </c>
+      <c r="K53" s="7">
+        <v>10131</v>
       </c>
       <c r="N53">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="O53">
+        <v>1.81975</v>
+      </c>
+      <c r="AL53">
+        <v>8</v>
+      </c>
+      <c r="AM53">
         <v>4.0193899999999996</v>
       </c>
-      <c r="P53">
+      <c r="AN53">
         <v>382.67399999999998</v>
       </c>
     </row>
-    <row r="54" spans="1:16">
+    <row r="54" spans="1:40">
       <c r="A54">
         <v>2</v>
       </c>
@@ -2240,26 +3894,32 @@
       <c r="H54">
         <v>16</v>
       </c>
-      <c r="I54">
-        <v>8.0801400000000001</v>
-      </c>
-      <c r="J54">
-        <v>584.09500000000003</v>
+      <c r="I54" s="7">
+        <v>4.2125700000000004</v>
+      </c>
+      <c r="J54" s="7">
+        <v>242.01599999999999</v>
       </c>
       <c r="K54" s="7">
-        <v>10023.299999999999</v>
+        <v>10285.799999999999</v>
       </c>
       <c r="N54">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="O54">
+        <v>1.8194699999999999</v>
+      </c>
+      <c r="AL54">
+        <v>8</v>
+      </c>
+      <c r="AM54">
         <v>4.3195300000000003</v>
       </c>
-      <c r="P54">
+      <c r="AN54">
         <v>439.31099999999998</v>
       </c>
     </row>
-    <row r="55" spans="1:16">
+    <row r="55" spans="1:40">
       <c r="A55">
         <v>4</v>
       </c>
@@ -2278,23 +3938,30 @@
       <c r="H55">
         <v>16</v>
       </c>
-      <c r="I55">
-        <v>8.0855899999999998</v>
-      </c>
-      <c r="J55">
-        <v>549.30999999999995</v>
-      </c>
+      <c r="I55" s="7">
+        <v>4.0243200000000003</v>
+      </c>
+      <c r="J55" s="7">
+        <v>257.77699999999999</v>
+      </c>
+      <c r="K55" s="7"/>
       <c r="N55">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="O55">
+        <v>1.82528</v>
+      </c>
+      <c r="AL55">
+        <v>16</v>
+      </c>
+      <c r="AM55">
         <v>2.4224800000000002</v>
       </c>
-      <c r="P55">
+      <c r="AN55">
         <v>443.43700000000001</v>
       </c>
     </row>
-    <row r="56" spans="1:16">
+    <row r="56" spans="1:40">
       <c r="A56">
         <v>4</v>
       </c>
@@ -2314,25 +3981,34 @@
         <v>32</v>
       </c>
       <c r="I56" s="7">
-        <v>1.99576</v>
-      </c>
-      <c r="J56">
-        <v>499.23700000000002</v>
+        <v>2.17964</v>
+      </c>
+      <c r="J56" s="7">
+        <v>141.73400000000001</v>
       </c>
       <c r="K56" s="7">
-        <v>10020.5</v>
+        <v>5090.71</v>
       </c>
       <c r="N56">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="O56">
+        <v>0.73208600000000001</v>
+      </c>
+      <c r="P56">
+        <v>22.016300000000001</v>
+      </c>
+      <c r="AL56">
+        <v>16</v>
+      </c>
+      <c r="AM56">
         <v>2.2925200000000001</v>
       </c>
-      <c r="P56">
+      <c r="AN56">
         <v>394.49599999999998</v>
       </c>
     </row>
-    <row r="57" spans="1:16">
+    <row r="57" spans="1:40">
       <c r="A57">
         <v>4</v>
       </c>
@@ -2352,28 +4028,33 @@
         <v>32</v>
       </c>
       <c r="I57" s="7">
-        <v>2.0158200000000002</v>
-      </c>
-      <c r="J57">
-        <v>460.988</v>
-      </c>
+        <v>2.2766000000000002</v>
+      </c>
+      <c r="J57" s="7"/>
       <c r="K57" s="7">
-        <v>10047.4</v>
-      </c>
-      <c r="L57" s="2" t="s">
-        <v>14</v>
-      </c>
+        <v>4608.91</v>
+      </c>
+      <c r="L57" s="2"/>
       <c r="N57">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="O57">
+        <v>0.73025899999999999</v>
+      </c>
+      <c r="P57">
+        <v>21.966999999999999</v>
+      </c>
+      <c r="AL57">
+        <v>16</v>
+      </c>
+      <c r="AM57">
         <v>2.6025100000000001</v>
       </c>
-      <c r="P57">
+      <c r="AN57">
         <v>379.82600000000002</v>
       </c>
     </row>
-    <row r="58" spans="1:16">
+    <row r="58" spans="1:40">
       <c r="A58">
         <v>4</v>
       </c>
@@ -2390,22 +4071,32 @@
         <v>32</v>
       </c>
       <c r="I58" s="7">
-        <v>1.98756</v>
-      </c>
-      <c r="J58">
-        <v>452.202</v>
+        <v>2.1740400000000002</v>
+      </c>
+      <c r="J58" s="7"/>
+      <c r="K58" s="7">
+        <v>4634.99</v>
       </c>
       <c r="N58">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="O58">
+        <v>0.72931599999999996</v>
+      </c>
+      <c r="P58">
+        <v>22.026599999999998</v>
+      </c>
+      <c r="AL58">
+        <v>16</v>
+      </c>
+      <c r="AM58">
         <v>2.2623000000000002</v>
       </c>
-      <c r="P58">
+      <c r="AN58">
         <v>472.43400000000003</v>
       </c>
     </row>
-    <row r="59" spans="1:16">
+    <row r="59" spans="1:40">
       <c r="A59">
         <v>4</v>
       </c>
@@ -2421,26 +4112,35 @@
       <c r="H59">
         <v>64</v>
       </c>
-      <c r="I59" s="3">
-        <v>1.0022200000000001</v>
-      </c>
-      <c r="J59" s="3">
-        <v>34.512300000000003</v>
+      <c r="I59" s="7">
+        <v>1.0692299999999999</v>
+      </c>
+      <c r="J59" s="7">
+        <v>30.816099999999999</v>
       </c>
       <c r="K59" s="7">
-        <v>4657.07</v>
+        <v>1955.58</v>
       </c>
       <c r="N59">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="O59">
+        <v>0.72885299999999997</v>
+      </c>
+      <c r="P59">
+        <v>22.151199999999999</v>
+      </c>
+      <c r="AL59">
+        <v>16</v>
+      </c>
+      <c r="AM59">
         <v>2.4241299999999999</v>
       </c>
-      <c r="P59">
+      <c r="AN59">
         <v>426.74599999999998</v>
       </c>
     </row>
-    <row r="60" spans="1:16">
+    <row r="60" spans="1:40">
       <c r="A60">
         <v>8</v>
       </c>
@@ -2462,26 +4162,35 @@
       <c r="H60">
         <v>64</v>
       </c>
-      <c r="I60" s="3">
-        <v>1.0070600000000001</v>
-      </c>
-      <c r="J60" s="3">
-        <v>26.9237</v>
-      </c>
-      <c r="K60" s="3">
-        <v>4709.95</v>
+      <c r="I60" s="7">
+        <v>1.15822</v>
+      </c>
+      <c r="J60" s="7">
+        <v>29.8247</v>
+      </c>
+      <c r="K60" s="7">
+        <v>1967.08</v>
       </c>
       <c r="N60">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="O60">
+        <v>0.72872800000000004</v>
+      </c>
+      <c r="P60">
+        <v>22.133600000000001</v>
+      </c>
+      <c r="AL60">
+        <v>16</v>
+      </c>
+      <c r="AM60">
         <v>2.26336</v>
       </c>
-      <c r="P60">
+      <c r="AN60">
         <v>427.02199999999999</v>
       </c>
     </row>
-    <row r="61" spans="1:16">
+    <row r="61" spans="1:40">
       <c r="A61">
         <v>8</v>
       </c>
@@ -2503,26 +4212,35 @@
       <c r="H61">
         <v>64</v>
       </c>
-      <c r="I61" s="3">
-        <v>1.00603</v>
-      </c>
-      <c r="J61" s="3">
-        <v>28.3809</v>
-      </c>
-      <c r="K61" s="2">
-        <v>4775.6000000000004</v>
+      <c r="I61" s="7">
+        <v>1.09161</v>
+      </c>
+      <c r="J61" s="7">
+        <v>29.697900000000001</v>
+      </c>
+      <c r="K61" s="7">
+        <v>1948.33</v>
       </c>
       <c r="N61">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="O61">
+        <v>0.424904</v>
+      </c>
+      <c r="P61">
+        <v>12.0937</v>
+      </c>
+      <c r="AL61">
+        <v>16</v>
+      </c>
+      <c r="AM61">
         <v>2.2760500000000001</v>
       </c>
-      <c r="P61">
+      <c r="AN61">
         <v>353.012</v>
       </c>
     </row>
-    <row r="62" spans="1:16">
+    <row r="62" spans="1:40">
       <c r="A62">
         <v>8</v>
       </c>
@@ -2544,23 +4262,26 @@
       <c r="H62">
         <v>124</v>
       </c>
-      <c r="I62">
-        <v>1.8499399999999999</v>
-      </c>
-      <c r="J62">
-        <v>28.442900000000002</v>
-      </c>
       <c r="N62">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="O62">
+        <v>0.42131999999999997</v>
+      </c>
+      <c r="P62">
+        <v>12.0677</v>
+      </c>
+      <c r="AL62">
+        <v>16</v>
+      </c>
+      <c r="AM62">
         <v>2.2768799999999998</v>
       </c>
-      <c r="P62">
+      <c r="AN62">
         <v>459.416</v>
       </c>
     </row>
-    <row r="63" spans="1:16">
+    <row r="63" spans="1:40">
       <c r="A63">
         <v>8</v>
       </c>
@@ -2579,23 +4300,26 @@
       <c r="H63">
         <v>124</v>
       </c>
-      <c r="I63">
-        <v>1.82697</v>
-      </c>
-      <c r="J63">
-        <v>64.484300000000005</v>
-      </c>
       <c r="N63">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="O63">
+        <v>0.42267900000000003</v>
+      </c>
+      <c r="P63">
+        <v>12.100199999999999</v>
+      </c>
+      <c r="AL63">
+        <v>16</v>
+      </c>
+      <c r="AM63">
         <v>2.2830499999999998</v>
       </c>
-      <c r="P63">
+      <c r="AN63">
         <v>463.56299999999999</v>
       </c>
     </row>
-    <row r="64" spans="1:16">
+    <row r="64" spans="1:40">
       <c r="A64">
         <v>8</v>
       </c>
@@ -2611,23 +4335,26 @@
       <c r="H64">
         <v>124</v>
       </c>
-      <c r="I64">
-        <v>1.8272600000000001</v>
-      </c>
-      <c r="J64">
-        <v>28.9465</v>
-      </c>
       <c r="N64">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="O64">
+        <v>0.42017300000000002</v>
+      </c>
+      <c r="P64">
+        <v>12.078799999999999</v>
+      </c>
+      <c r="AL64">
+        <v>16</v>
+      </c>
+      <c r="AM64">
         <v>2.28057</v>
       </c>
-      <c r="P64">
+      <c r="AN64">
         <v>416.21899999999999</v>
       </c>
     </row>
-    <row r="65" spans="1:16">
+    <row r="65" spans="1:40">
       <c r="A65">
         <v>16</v>
       </c>
@@ -2647,16 +4374,25 @@
         <v>5524.35</v>
       </c>
       <c r="N65">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="O65">
+        <v>0.42275000000000001</v>
+      </c>
+      <c r="P65">
+        <v>12.105399999999999</v>
+      </c>
+      <c r="AL65">
+        <v>32</v>
+      </c>
+      <c r="AM65">
         <v>1.5313699999999999</v>
       </c>
-      <c r="P65">
+      <c r="AN65">
         <v>191.916</v>
       </c>
     </row>
-    <row r="66" spans="1:16">
+    <row r="66" spans="1:40">
       <c r="A66">
         <v>16</v>
       </c>
@@ -2676,16 +4412,25 @@
         <v>5578.63</v>
       </c>
       <c r="N66">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="O66">
+        <v>0.215058</v>
+      </c>
+      <c r="P66">
+        <v>6.4152399999999998</v>
+      </c>
+      <c r="AL66">
+        <v>32</v>
+      </c>
+      <c r="AM66">
         <v>1.48475</v>
       </c>
-      <c r="P66">
+      <c r="AN66">
         <v>202.07400000000001</v>
       </c>
     </row>
-    <row r="67" spans="1:16">
+    <row r="67" spans="1:40">
       <c r="A67">
         <v>16</v>
       </c>
@@ -2705,16 +4450,25 @@
         <v>5549.76</v>
       </c>
       <c r="N67">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="O67">
+        <v>0.21332799999999999</v>
+      </c>
+      <c r="P67">
+        <v>6.41859</v>
+      </c>
+      <c r="AL67">
+        <v>32</v>
+      </c>
+      <c r="AM67">
         <v>1.5680799999999999</v>
       </c>
-      <c r="P67">
+      <c r="AN67">
         <v>214.15100000000001</v>
       </c>
     </row>
-    <row r="68" spans="1:16">
+    <row r="68" spans="1:40">
       <c r="A68">
         <v>16</v>
       </c>
@@ -2734,16 +4488,25 @@
         <v>5524.35</v>
       </c>
       <c r="N68">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="O68">
+        <v>0.21474099999999999</v>
+      </c>
+      <c r="P68">
+        <v>6.3698199999999998</v>
+      </c>
+      <c r="AL68">
+        <v>32</v>
+      </c>
+      <c r="AM68">
         <v>1.4837800000000001</v>
       </c>
-      <c r="P68">
+      <c r="AN68">
         <v>250.226</v>
       </c>
     </row>
-    <row r="69" spans="1:16">
+    <row r="69" spans="1:40">
       <c r="A69">
         <v>16</v>
       </c>
@@ -2760,16 +4523,25 @@
         <v>236.816</v>
       </c>
       <c r="N69">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="O69">
+        <v>0.21489</v>
+      </c>
+      <c r="P69">
+        <v>6.4153399999999996</v>
+      </c>
+      <c r="AL69">
+        <v>32</v>
+      </c>
+      <c r="AM69">
         <v>1.47604</v>
       </c>
-      <c r="P69">
+      <c r="AN69">
         <v>193.43</v>
       </c>
     </row>
-    <row r="70" spans="1:16">
+    <row r="70" spans="1:40">
       <c r="A70">
         <v>32</v>
       </c>
@@ -2789,16 +4561,25 @@
         <v>1975.16</v>
       </c>
       <c r="N70">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="O70">
+        <v>0.21452199999999999</v>
+      </c>
+      <c r="P70">
+        <v>6.4186399999999999</v>
+      </c>
+      <c r="AL70">
+        <v>32</v>
+      </c>
+      <c r="AM70">
         <v>1.5699099999999999</v>
       </c>
-      <c r="P70">
+      <c r="AN70">
         <v>239.16900000000001</v>
       </c>
     </row>
-    <row r="71" spans="1:16">
+    <row r="71" spans="1:40">
       <c r="A71">
         <v>32</v>
       </c>
@@ -2818,16 +4599,25 @@
         <v>1922.53</v>
       </c>
       <c r="N71">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="O71">
+        <v>0.111482</v>
+      </c>
+      <c r="P71">
+        <v>3.4758100000000001</v>
+      </c>
+      <c r="AL71">
+        <v>32</v>
+      </c>
+      <c r="AM71">
         <v>1.4711399999999999</v>
       </c>
-      <c r="P71">
+      <c r="AN71">
         <v>199.828</v>
       </c>
     </row>
-    <row r="72" spans="1:16">
+    <row r="72" spans="1:40">
       <c r="A72">
         <v>32</v>
       </c>
@@ -2844,16 +4634,25 @@
         <v>82.326700000000002</v>
       </c>
       <c r="N72">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="O72">
+        <v>0.11082</v>
+      </c>
+      <c r="P72">
+        <v>3.4501499999999998</v>
+      </c>
+      <c r="AL72">
+        <v>32</v>
+      </c>
+      <c r="AM72">
         <v>1.4715100000000001</v>
       </c>
-      <c r="P72">
+      <c r="AN72">
         <v>203.13200000000001</v>
       </c>
     </row>
-    <row r="73" spans="1:16">
+    <row r="73" spans="1:40">
       <c r="A73">
         <v>32</v>
       </c>
@@ -2870,16 +4669,25 @@
         <v>106.52200000000001</v>
       </c>
       <c r="N73">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="O73">
+        <v>0.11096399999999999</v>
+      </c>
+      <c r="P73">
+        <v>3.4399600000000001</v>
+      </c>
+      <c r="AL73">
+        <v>32</v>
+      </c>
+      <c r="AM73">
         <v>1.55629</v>
       </c>
-      <c r="P73">
+      <c r="AN73">
         <v>238.333</v>
       </c>
     </row>
-    <row r="74" spans="1:16">
+    <row r="74" spans="1:40">
       <c r="A74">
         <v>32</v>
       </c>
@@ -2896,16 +4704,25 @@
         <v>81.409400000000005</v>
       </c>
       <c r="N74">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="O74">
+        <v>0.10969</v>
+      </c>
+      <c r="P74">
+        <v>3.4076399999999998</v>
+      </c>
+      <c r="AL74">
+        <v>32</v>
+      </c>
+      <c r="AM74">
         <v>1.4871099999999999</v>
       </c>
-      <c r="P74">
+      <c r="AN74">
         <v>195.01900000000001</v>
       </c>
     </row>
-    <row r="75" spans="1:16">
+    <row r="75" spans="1:40">
       <c r="A75">
         <v>64</v>
       </c>
@@ -2925,16 +4742,25 @@
         <v>842.38699999999994</v>
       </c>
       <c r="N75">
-        <v>64</v>
+        <v>16</v>
       </c>
       <c r="O75">
+        <v>0.109816</v>
+      </c>
+      <c r="P75">
+        <v>3.4153899999999999</v>
+      </c>
+      <c r="AL75">
+        <v>64</v>
+      </c>
+      <c r="AM75">
         <v>1.3966799999999999</v>
       </c>
-      <c r="P75">
+      <c r="AN75">
         <v>31.647099999999998</v>
       </c>
     </row>
-    <row r="76" spans="1:16">
+    <row r="76" spans="1:40">
       <c r="A76">
         <v>64</v>
       </c>
@@ -2954,16 +4780,25 @@
         <v>897.548</v>
       </c>
       <c r="N76">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="O76">
+        <v>5.5819000000000001E-2</v>
+      </c>
+      <c r="P76">
+        <v>1.8152699999999999</v>
+      </c>
+      <c r="AL76">
+        <v>64</v>
+      </c>
+      <c r="AM76">
         <v>1.38195</v>
       </c>
-      <c r="P76">
+      <c r="AN76">
         <v>53.1434</v>
       </c>
     </row>
-    <row r="77" spans="1:16">
+    <row r="77" spans="1:40">
       <c r="A77">
         <v>64</v>
       </c>
@@ -2983,16 +4818,25 @@
         <v>892.93299999999999</v>
       </c>
       <c r="N77">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="O77">
+        <v>5.6050099999999999E-2</v>
+      </c>
+      <c r="P77">
+        <v>1.77654</v>
+      </c>
+      <c r="AL77">
+        <v>64</v>
+      </c>
+      <c r="AM77">
         <v>1.37395</v>
       </c>
-      <c r="P77">
+      <c r="AN77">
         <v>47.1267</v>
       </c>
     </row>
-    <row r="78" spans="1:16">
+    <row r="78" spans="1:40">
       <c r="A78">
         <v>64</v>
       </c>
@@ -3012,16 +4856,25 @@
         <v>919.52499999999998</v>
       </c>
       <c r="N78">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="O78">
+        <v>5.5881E-2</v>
+      </c>
+      <c r="P78">
+        <v>1.77092</v>
+      </c>
+      <c r="AL78">
+        <v>64</v>
+      </c>
+      <c r="AM78">
         <v>1.4312199999999999</v>
       </c>
-      <c r="P78">
+      <c r="AN78">
         <v>43.902099999999997</v>
       </c>
     </row>
-    <row r="79" spans="1:16">
+    <row r="79" spans="1:40">
       <c r="A79">
         <v>64</v>
       </c>
@@ -3041,71 +4894,137 @@
         <v>795.726</v>
       </c>
       <c r="N79">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="O79">
+        <v>5.5960200000000002E-2</v>
+      </c>
+      <c r="P79">
+        <v>1.7728299999999999</v>
+      </c>
+      <c r="AL79">
+        <v>64</v>
+      </c>
+      <c r="AM79">
         <v>1.4228799999999999</v>
       </c>
-      <c r="P79">
+      <c r="AN79">
         <v>39.096699999999998</v>
       </c>
     </row>
-    <row r="80" spans="1:16">
+    <row r="80" spans="1:40">
       <c r="N80">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="O80">
+        <v>5.59809E-2</v>
+      </c>
+      <c r="P80">
+        <v>1.7767200000000001</v>
+      </c>
+      <c r="AL80">
+        <v>64</v>
+      </c>
+      <c r="AM80">
         <v>1.3692899999999999</v>
       </c>
-      <c r="P80">
+      <c r="AN80">
         <v>43.0304</v>
       </c>
     </row>
-    <row r="81" spans="14:16">
+    <row r="81" spans="14:40">
       <c r="N81">
         <v>64</v>
       </c>
       <c r="O81">
+        <v>2.9833100000000001E-2</v>
+      </c>
+      <c r="P81">
+        <v>0.91668899999999998</v>
+      </c>
+      <c r="AL81">
+        <v>64</v>
+      </c>
+      <c r="AM81">
         <v>1.3653999999999999</v>
       </c>
-      <c r="P81">
+      <c r="AN81">
         <v>45.570300000000003</v>
       </c>
     </row>
-    <row r="82" spans="14:16">
+    <row r="82" spans="14:40">
       <c r="N82">
         <v>64</v>
       </c>
       <c r="O82">
+        <v>2.9510000000000002E-2</v>
+      </c>
+      <c r="P82">
+        <v>0.90918600000000005</v>
+      </c>
+      <c r="AL82">
+        <v>64</v>
+      </c>
+      <c r="AM82">
         <v>1.36619</v>
       </c>
-      <c r="P82">
+      <c r="AN82">
         <v>48.552100000000003</v>
       </c>
     </row>
-    <row r="83" spans="14:16">
+    <row r="83" spans="14:40">
       <c r="N83">
         <v>64</v>
       </c>
       <c r="O83">
+        <v>2.9603000000000001E-2</v>
+      </c>
+      <c r="P83">
+        <v>0.89445399999999997</v>
+      </c>
+      <c r="AL83">
+        <v>64</v>
+      </c>
+      <c r="AM83">
         <v>1.36643</v>
       </c>
-      <c r="P83">
+      <c r="AN83">
         <v>42.653300000000002</v>
       </c>
     </row>
-    <row r="84" spans="14:16">
+    <row r="84" spans="14:40">
       <c r="N84">
         <v>64</v>
       </c>
       <c r="O84">
+        <v>2.9773000000000001E-2</v>
+      </c>
+      <c r="P84">
+        <v>0.88092599999999999</v>
+      </c>
+      <c r="AL84">
+        <v>64</v>
+      </c>
+      <c r="AM84">
         <v>1.3651599999999999</v>
       </c>
-      <c r="P84">
+      <c r="AN84">
         <v>40.652000000000001</v>
       </c>
     </row>
+    <row r="85" spans="14:40">
+      <c r="N85">
+        <v>64</v>
+      </c>
+      <c r="O85">
+        <v>2.9665899999999999E-2</v>
+      </c>
+      <c r="P85">
+        <v>0.877023</v>
+      </c>
+    </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Updated because of bad nodes
git-svn-id: svn+ssh://software-srn.sandia.gov/svn/mapreduce/trunk@618 3fc257bb-8550-0410-81b3-a5c103da83f7
</commit_message>
<xml_diff>
--- a/paper/results.xlsx
+++ b/paper/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3840" yWindow="40" windowWidth="21600" windowHeight="13380" tabRatio="500"/>
+    <workbookView minimized="1" xWindow="3840" yWindow="40" windowWidth="21600" windowHeight="13380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -223,12 +223,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
   <fonts count="5">
     <font>
       <sz val="10"/>
@@ -676,11 +670,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="455759240"/>
-        <c:axId val="455768632"/>
+        <c:axId val="456810984"/>
+        <c:axId val="456820376"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="455759240"/>
+        <c:axId val="456810984"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -707,12 +701,12 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="455768632"/>
+        <c:crossAx val="456820376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="455768632"/>
+        <c:axId val="456820376"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -740,7 +734,7 @@
         <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="455759240"/>
+        <c:crossAx val="456810984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -981,13 +975,13 @@
                   <c:v>190.895</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="0.00">
-                  <c:v>114.7153888888889</c:v>
+                  <c:v>46.67866666666666</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="0.00">
-                  <c:v>56.43566666666666</c:v>
+                  <c:v>21.552</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="0.00">
-                  <c:v>10.95971666666667</c:v>
+                  <c:v>5.33575</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1290,11 +1284,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="455859352"/>
-        <c:axId val="455865128"/>
+        <c:axId val="456911096"/>
+        <c:axId val="456916872"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="455859352"/>
+        <c:axId val="456911096"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1321,13 +1315,13 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="455865128"/>
+        <c:crossAx val="456916872"/>
         <c:crossesAt val="0.001"/>
         <c:crossBetween val="midCat"/>
         <c:minorUnit val="10.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="455865128"/>
+        <c:axId val="456916872"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1355,7 +1349,7 @@
         <c:numFmt formatCode="0.E+00" sourceLinked="0"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="455859352"/>
+        <c:crossAx val="456911096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1618,11 +1612,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="455883592"/>
-        <c:axId val="455892552"/>
+        <c:axId val="456935336"/>
+        <c:axId val="456944296"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="455883592"/>
+        <c:axId val="456935336"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1649,12 +1643,12 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="455892552"/>
+        <c:crossAx val="456944296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="455892552"/>
+        <c:axId val="456944296"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1682,7 +1676,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="455883592"/>
+        <c:crossAx val="456935336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1723,7 +1717,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -1873,11 +1866,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="455920568"/>
-        <c:axId val="455929192"/>
+        <c:axId val="456972312"/>
+        <c:axId val="456980936"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="455920568"/>
+        <c:axId val="456972312"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1899,17 +1892,16 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="455929192"/>
+        <c:crossAx val="456980936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="455929192"/>
+        <c:axId val="456980936"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1932,19 +1924,17 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="455920568"/>
+        <c:crossAx val="456972312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -2041,7 +2031,7 @@
                   <c:v>14250.8</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>15864.05</c:v>
+                  <c:v>11913.76666666667</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2176,7 +2166,7 @@
                   <c:v>415.7974</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>470.8802000000001</c:v>
+                  <c:v>279.0272</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2326,7 +2316,7 @@
                   <c:v>6.912546000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.227036</c:v>
+                  <c:v>4.56282</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2407,11 +2397,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="455987864"/>
-        <c:axId val="455993864"/>
+        <c:axId val="457039720"/>
+        <c:axId val="457045688"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="455987864"/>
+        <c:axId val="457039720"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2438,12 +2428,12 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="455993864"/>
+        <c:crossAx val="457045688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="455993864"/>
+        <c:axId val="457045688"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2471,7 +2461,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="455987864"/>
+        <c:crossAx val="457039720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2512,7 +2502,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -2938,11 +2927,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="456043736"/>
-        <c:axId val="456049736"/>
+        <c:axId val="457095480"/>
+        <c:axId val="457101480"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="456043736"/>
+        <c:axId val="457095480"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2964,17 +2953,16 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="456049736"/>
+        <c:crossAx val="457101480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="456049736"/>
+        <c:axId val="457101480"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2997,19 +2985,17 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="456043736"/>
+        <c:crossAx val="457095480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -3207,11 +3193,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="jjj" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="jj_1" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="jj_1" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="jjj" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3537,8 +3523,8 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AZ85"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="AH10" sqref="AH10"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="M53" sqref="M53:M61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -4229,7 +4215,7 @@
       <c r="L9" s="1"/>
       <c r="M9" s="3">
         <f>AVERAGE(M27:M29)</f>
-        <v>114.71538888888888</v>
+        <v>46.678666666666665</v>
       </c>
       <c r="O9">
         <f>AVERAGE(O35:O39)</f>
@@ -4356,7 +4342,7 @@
       <c r="L10" s="1"/>
       <c r="M10" s="3">
         <f>AVERAGE(M30:M32)</f>
-        <v>56.435666666666663</v>
+        <v>21.552000000000003</v>
       </c>
       <c r="O10">
         <f>AVERAGE(O40:O44)</f>
@@ -4491,7 +4477,7 @@
       <c r="L11" s="1"/>
       <c r="M11" s="3">
         <f>AVERAGE(M33:M35)</f>
-        <v>10.959716666666667</v>
+        <v>5.33575</v>
       </c>
       <c r="O11">
         <f>AVERAGE(O45:O49)</f>
@@ -4525,15 +4511,15 @@
       </c>
       <c r="AA11">
         <f>AVERAGE(AA45:AA49)</f>
-        <v>6.227036</v>
+        <v>4.5628200000000003</v>
       </c>
       <c r="AB11">
         <f>AVERAGE(AB45:AB49)</f>
-        <v>470.88020000000006</v>
+        <v>279.02719999999999</v>
       </c>
       <c r="AC11">
         <f>AVERAGE(AC45:AC49)</f>
-        <v>15864.05</v>
+        <v>11913.766666666668</v>
       </c>
       <c r="AF11">
         <f>AVERAGE(AF45:AF49)</f>
@@ -5497,7 +5483,7 @@
       </c>
       <c r="M27">
         <f t="shared" si="3"/>
-        <v>113.6245</v>
+        <v>46.771999999999998</v>
       </c>
       <c r="N27">
         <v>4</v>
@@ -5583,7 +5569,7 @@
       </c>
       <c r="M28">
         <f t="shared" si="3"/>
-        <v>113.062</v>
+        <v>46.135666666666673</v>
       </c>
       <c r="N28">
         <v>4</v>
@@ -5659,7 +5645,7 @@
       </c>
       <c r="M29">
         <f t="shared" si="3"/>
-        <v>117.45966666666668</v>
+        <v>47.12833333333333</v>
       </c>
       <c r="N29">
         <v>4</v>
@@ -5733,7 +5719,7 @@
       </c>
       <c r="M30">
         <f t="shared" si="3"/>
-        <v>56.435666666666663</v>
+        <v>21.552000000000003</v>
       </c>
       <c r="N30">
         <v>8</v>
@@ -6017,7 +6003,7 @@
       </c>
       <c r="M33">
         <f t="shared" si="3"/>
-        <v>10.967483333333334</v>
+        <v>5.3251999999999997</v>
       </c>
       <c r="N33">
         <v>8</v>
@@ -6109,7 +6095,7 @@
       </c>
       <c r="M34">
         <f t="shared" si="3"/>
-        <v>10.961550000000001</v>
+        <v>5.3508500000000003</v>
       </c>
       <c r="N34">
         <v>8</v>
@@ -6186,7 +6172,7 @@
       </c>
       <c r="M35">
         <f t="shared" si="3"/>
-        <v>10.950116666666666</v>
+        <v>5.3311999999999999</v>
       </c>
       <c r="N35">
         <v>16</v>
@@ -7149,13 +7135,13 @@
         <v>64</v>
       </c>
       <c r="AA45">
-        <v>5.7715800000000002</v>
+        <v>4.1922699999999997</v>
       </c>
       <c r="AB45">
-        <v>404.69400000000002</v>
+        <v>261.56400000000002</v>
       </c>
       <c r="AC45">
-        <v>15893.7</v>
+        <v>12168.7</v>
       </c>
       <c r="AF45">
         <v>3.1915100000000001</v>
@@ -7251,13 +7237,13 @@
         <v>64</v>
       </c>
       <c r="AA46">
-        <v>5.7947699999999998</v>
+        <v>4.7901600000000002</v>
       </c>
       <c r="AB46">
-        <v>447.16699999999997</v>
+        <v>272.78500000000003</v>
       </c>
       <c r="AC46">
-        <v>15834.4</v>
+        <v>11834.5</v>
       </c>
       <c r="AF46">
         <v>3.18513</v>
@@ -7353,10 +7339,13 @@
         <v>64</v>
       </c>
       <c r="AA47">
-        <v>5.8171299999999997</v>
+        <v>4.5233600000000003</v>
       </c>
       <c r="AB47">
-        <v>470.76</v>
+        <v>286.85899999999998</v>
+      </c>
+      <c r="AC47">
+        <v>11738.1</v>
       </c>
       <c r="AF47">
         <v>3.2003200000000001</v>
@@ -7452,10 +7441,10 @@
         <v>64</v>
       </c>
       <c r="AA48">
-        <v>7.1295200000000003</v>
+        <v>4.7907500000000001</v>
       </c>
       <c r="AB48">
-        <v>524.46900000000005</v>
+        <v>294.23</v>
       </c>
       <c r="AF48">
         <v>3.1998099999999998</v>
@@ -7548,10 +7537,10 @@
         <v>64</v>
       </c>
       <c r="AA49">
-        <v>6.6221800000000002</v>
+        <v>4.5175599999999996</v>
       </c>
       <c r="AB49">
-        <v>507.31099999999998</v>
+        <v>279.69799999999998</v>
       </c>
       <c r="AF49">
         <v>3.1928100000000001</v>
@@ -7654,7 +7643,7 @@
         <v>10131</v>
       </c>
       <c r="M53">
-        <v>681.74699999999996</v>
+        <v>280.63200000000001</v>
       </c>
       <c r="N53">
         <v>1</v>
@@ -7677,7 +7666,7 @@
         <v>10285.799999999999</v>
       </c>
       <c r="M54">
-        <v>678.37199999999996</v>
+        <v>276.81400000000002</v>
       </c>
       <c r="N54">
         <v>1</v>
@@ -7698,7 +7687,7 @@
       </c>
       <c r="K55" s="4"/>
       <c r="M55">
-        <v>704.75800000000004</v>
+        <v>282.77</v>
       </c>
       <c r="N55">
         <v>1</v>
@@ -7721,7 +7710,7 @@
         <v>5090.71</v>
       </c>
       <c r="M56">
-        <v>338.61399999999998</v>
+        <v>129.31200000000001</v>
       </c>
       <c r="N56">
         <v>2</v>
@@ -7746,7 +7735,7 @@
       </c>
       <c r="L57" s="2"/>
       <c r="M57">
-        <v>362.31700000000001</v>
+        <v>130.73099999999999</v>
       </c>
       <c r="N57">
         <v>2</v>
@@ -7770,7 +7759,7 @@
         <v>4634.99</v>
       </c>
       <c r="M58">
-        <v>368.358</v>
+        <v>128.55000000000001</v>
       </c>
       <c r="N58">
         <v>2</v>
@@ -7796,7 +7785,7 @@
         <v>1955.58</v>
       </c>
       <c r="M59">
-        <v>65.804900000000004</v>
+        <v>31.9512</v>
       </c>
       <c r="N59">
         <v>2</v>
@@ -7822,7 +7811,7 @@
         <v>1967.08</v>
       </c>
       <c r="M60">
-        <v>65.769300000000001</v>
+        <v>32.1051</v>
       </c>
       <c r="N60">
         <v>2</v>
@@ -7848,7 +7837,7 @@
         <v>1948.33</v>
       </c>
       <c r="M61">
-        <v>65.700699999999998</v>
+        <v>31.987200000000001</v>
       </c>
       <c r="N61">
         <v>4</v>

</xml_diff>

<commit_message>
added some XMT results.
git-svn-id: svn+ssh://software-srn.sandia.gov/svn/mapreduce/trunk@627 3fc257bb-8550-0410-81b3-a5c103da83f7
</commit_message>
<xml_diff>
--- a/paper/results.xlsx
+++ b/paper/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="9120" yWindow="1080" windowWidth="21600" windowHeight="13380" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="420" yWindow="-120" windowWidth="21600" windowHeight="13380" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="CC" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <definedName name="jj_1" localSheetId="6">Sheet1!$N$41:$O$64</definedName>
     <definedName name="jjj" localSheetId="6">Sheet1!$BD$15:$BE$84</definedName>
   </definedNames>
-  <calcPr calcId="130407" concurrentCalc="0"/>
+  <calcPr calcId="130406" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="57">
   <si>
     <t>R-MAT 24 (MR-MPI)</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -78,10 +78,6 @@
   </si>
   <si>
     <t>Number of Processors</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>R-MAT 28</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
@@ -264,11 +260,37 @@
     <t>R-MAT 28</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
+  <si>
+    <t>XMT</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>R-MAT 20 (XMT)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>R-MAT 24 (XMT)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>R-MAT 28 (XMT)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>XMT</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
   <fonts count="5">
     <font>
       <sz val="10"/>
@@ -698,11 +720,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="754933416"/>
-        <c:axId val="754919912"/>
+        <c:axId val="591463880"/>
+        <c:axId val="591457800"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="754933416"/>
+        <c:axId val="591463880"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -724,16 +746,17 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="754919912"/>
+        <c:crossAx val="591457800"/>
         <c:crossesAt val="0.1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="754919912"/>
+        <c:axId val="591457800"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -756,17 +779,19 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="754933416"/>
+        <c:crossAx val="591463880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -1203,11 +1228,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="788695352"/>
-        <c:axId val="788701320"/>
+        <c:axId val="591655064"/>
+        <c:axId val="591661032"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="788695352"/>
+        <c:axId val="591655064"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1232,12 +1257,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="788701320"/>
+        <c:crossAx val="591661032"/>
         <c:crossesAt val="0.0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="788701320"/>
+        <c:axId val="591661032"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1264,7 +1289,7 @@
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="788695352"/>
+        <c:crossAx val="591655064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1711,11 +1736,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="788758808"/>
-        <c:axId val="788764808"/>
+        <c:axId val="591718264"/>
+        <c:axId val="591724264"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="788758808"/>
+        <c:axId val="591718264"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1741,12 +1766,12 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="788764808"/>
+        <c:crossAx val="591724264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="788764808"/>
+        <c:axId val="591724264"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1773,7 +1798,7 @@
         <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="788758808"/>
+        <c:crossAx val="591718264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2016,313 +2041,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="788805256"/>
-        <c:axId val="788815384"/>
+        <c:axId val="591763560"/>
+        <c:axId val="591773656"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="788805256"/>
-        <c:scaling>
-          <c:logBase val="10.0"/>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Number of Processors</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:minorTickMark val="in"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="788815384"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="788815384"/>
-        <c:scaling>
-          <c:logBase val="10.0"/>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Time (secs)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-        </c:title>
-        <c:numFmt formatCode="0" sourceLinked="0"/>
-        <c:minorTickMark val="in"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="788805256"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="1"/>
-  <c:lang val="en-US"/>
-  <c:style val="2"/>
-  <c:chart>
-    <c:autoTitleDeleted val="1"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$AA$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>R-MAT 20 (MR-MPI)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$Z$5:$Z$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>64.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$AA$5:$AA$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>150.766</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>106.484</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>53.9303</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>18.2997</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4.126341999999999</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.11674</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.108394</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$AB$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>R-MAT 24 (MR-MPI)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$Z$5:$Z$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>64.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$AB$5:$AB$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>8259.74</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4943.416666666666</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1943.665</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>629.3022500000001</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>251.5002</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>141.9476</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>99.42392</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$AC$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>R-MAT 28 (MR-MPI)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$Z$5:$Z$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>64.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$AC$5:$AC$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="3">
-                  <c:v>23233.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>11092.4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5725.976000000001</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>4201.97</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-        </c:ser>
-        <c:axId val="788857400"/>
-        <c:axId val="788867528"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="788857400"/>
+        <c:axId val="591763560"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2349,12 +2072,317 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="788867528"/>
+        <c:crossAx val="591773656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="788867528"/>
+        <c:axId val="591773656"/>
+        <c:scaling>
+          <c:logBase val="10.0"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time (secs)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:minorTickMark val="in"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="591763560"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="1"/>
+  <c:lang val="en-US"/>
+  <c:style val="2"/>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$AA$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>R-MAT 20 (MR-MPI)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$Z$5:$Z$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$AA$5:$AA$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>150.766</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>106.484</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>53.9303</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18.2997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.126341999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.11674</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.108394</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$AB$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>R-MAT 24 (MR-MPI)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$Z$5:$Z$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$AB$5:$AB$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>8259.74</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4943.416666666666</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1943.665</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>629.3022500000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>251.5002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>141.9476</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>99.42392</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$AC$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>R-MAT 28 (MR-MPI)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$Z$5:$Z$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$AC$5:$AC$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="3">
+                  <c:v>23233.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11092.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5725.976000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4201.97</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="591817128"/>
+        <c:axId val="591827256"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="591817128"/>
+        <c:scaling>
+          <c:logBase val="10.0"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of Processors</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:minorTickMark val="in"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="591827256"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="591827256"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2382,7 +2410,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="788857400"/>
+        <c:crossAx val="591817128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2551,11 +2579,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="788904696"/>
-        <c:axId val="788917096"/>
+        <c:axId val="591863912"/>
+        <c:axId val="591876376"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="788904696"/>
+        <c:axId val="591863912"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2581,12 +2609,12 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="788917096"/>
+        <c:crossAx val="591876376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="788917096"/>
+        <c:axId val="591876376"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2613,7 +2641,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="788904696"/>
+        <c:crossAx val="591863912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3157,11 +3185,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="789038120"/>
-        <c:axId val="789043896"/>
+        <c:axId val="591996904"/>
+        <c:axId val="592002680"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="789038120"/>
+        <c:axId val="591996904"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -3188,13 +3216,13 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="789043896"/>
+        <c:crossAx val="592002680"/>
         <c:crossesAt val="0.001"/>
         <c:crossBetween val="midCat"/>
         <c:minorUnit val="10.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="789043896"/>
+        <c:axId val="592002680"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -3222,7 +3250,7 @@
         <c:numFmt formatCode="0.E+00" sourceLinked="0"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="789038120"/>
+        <c:crossAx val="591996904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3263,6 +3291,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -3691,11 +3720,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="789078776"/>
-        <c:axId val="789084776"/>
+        <c:axId val="592037000"/>
+        <c:axId val="592043000"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="789078776"/>
+        <c:axId val="592037000"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -3717,16 +3746,17 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="789084776"/>
+        <c:crossAx val="592043000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="789084776"/>
+        <c:axId val="592043000"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -3749,17 +3779,19 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="789078776"/>
+        <c:crossAx val="592037000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -3773,7 +3805,7 @@
 
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr/>
+  <sheetPr published="0"/>
   <sheetViews>
     <sheetView zoomScale="97" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
@@ -3785,7 +3817,7 @@
 
 <file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr/>
+  <sheetPr published="0"/>
   <sheetViews>
     <sheetView zoomScale="97" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
@@ -3797,7 +3829,7 @@
 
 <file path=xl/chartsheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr/>
+  <sheetPr published="0"/>
   <sheetViews>
     <sheetView zoomScale="116" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
@@ -3809,7 +3841,7 @@
 
 <file path=xl/chartsheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr/>
+  <sheetPr published="0"/>
   <sheetViews>
     <sheetView zoomScale="116" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
@@ -3821,9 +3853,9 @@
 
 <file path=xl/chartsheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr/>
+  <sheetPr published="0"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="116" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="116" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -3833,7 +3865,7 @@
 
 <file path=xl/chartsheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr/>
+  <sheetPr published="0"/>
   <sheetViews>
     <sheetView zoomScale="116" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
@@ -4071,11 +4103,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="jjj" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="jj_1" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="jj_1" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="jjj" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4401,8 +4433,8 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:BO85"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="X1" workbookViewId="0">
-      <selection activeCell="AC50" sqref="AC50"/>
+    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -4416,22 +4448,22 @@
   <sheetData>
     <row r="1" spans="1:67">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="T1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Z1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AL1" t="s">
         <v>17</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AX1" t="s">
         <v>18</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>19</v>
       </c>
       <c r="BD1" t="s">
         <v>2</v>
@@ -4439,13 +4471,13 @@
     </row>
     <row r="2" spans="1:67">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N2" t="s">
         <v>5</v>
       </c>
       <c r="P2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="BD2" t="s">
         <v>5</v>
@@ -4453,46 +4485,52 @@
     </row>
     <row r="3" spans="1:67">
       <c r="C3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" t="s">
+        <v>52</v>
+      </c>
+      <c r="O3" t="s">
+        <v>43</v>
+      </c>
+      <c r="S3" t="s">
         <v>13</v>
       </c>
-      <c r="O3" t="s">
-        <v>44</v>
-      </c>
-      <c r="S3" t="s">
+      <c r="U3" t="s">
         <v>14</v>
       </c>
-      <c r="U3" t="s">
+      <c r="V3" t="s">
         <v>15</v>
       </c>
-      <c r="V3" t="s">
-        <v>16</v>
-      </c>
       <c r="W3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AM3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AR3" t="s">
+        <v>24</v>
+      </c>
+      <c r="AU3" t="s">
         <v>25</v>
       </c>
-      <c r="AU3" t="s">
-        <v>26</v>
+      <c r="BB3" t="s">
+        <v>56</v>
       </c>
       <c r="BJ3" t="s">
+        <v>22</v>
+      </c>
+      <c r="BK3" t="s">
         <v>23</v>
       </c>
-      <c r="BK3" t="s">
-        <v>24</v>
-      </c>
       <c r="BL3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:67">
@@ -4500,28 +4538,37 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" t="s">
         <v>51</v>
       </c>
-      <c r="C4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D4" t="s">
-        <v>52</v>
-      </c>
       <c r="E4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G4" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+      <c r="I4" t="s">
+        <v>53</v>
+      </c>
+      <c r="J4" t="s">
+        <v>54</v>
+      </c>
+      <c r="K4" t="s">
+        <v>55</v>
       </c>
       <c r="N4" t="s">
         <v>6</v>
       </c>
       <c r="O4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P4" t="s">
         <v>0</v>
@@ -4530,52 +4577,52 @@
         <v>1</v>
       </c>
       <c r="R4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="S4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="U4" t="s">
+        <v>32</v>
+      </c>
+      <c r="V4" t="s">
         <v>33</v>
       </c>
-      <c r="V4" t="s">
+      <c r="W4" t="s">
         <v>34</v>
-      </c>
-      <c r="W4" t="s">
-        <v>35</v>
       </c>
       <c r="Z4" t="s">
         <v>6</v>
       </c>
       <c r="AA4" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB4" t="s">
         <v>46</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>47</v>
       </c>
       <c r="AC4" t="s">
         <v>1</v>
       </c>
       <c r="AD4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AL4" t="s">
         <v>6</v>
       </c>
       <c r="AM4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AN4" t="s">
+        <v>38</v>
+      </c>
+      <c r="AO4" t="s">
         <v>39</v>
       </c>
-      <c r="AO4" t="s">
-        <v>40</v>
-      </c>
       <c r="AP4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AR4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AS4" t="s">
         <v>3</v>
@@ -4584,49 +4631,52 @@
         <v>4</v>
       </c>
       <c r="AU4" t="s">
+        <v>40</v>
+      </c>
+      <c r="AV4" t="s">
         <v>41</v>
       </c>
-      <c r="AV4" t="s">
+      <c r="AW4" t="s">
         <v>42</v>
-      </c>
-      <c r="AW4" t="s">
-        <v>43</v>
       </c>
       <c r="AX4" t="s">
         <v>6</v>
       </c>
       <c r="AY4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AZ4" t="s">
         <v>0</v>
       </c>
-      <c r="BA4" t="s">
-        <v>7</v>
+      <c r="BB4" t="s">
+        <v>53</v>
+      </c>
+      <c r="BC4" t="s">
+        <v>54</v>
       </c>
       <c r="BD4" t="s">
         <v>6</v>
       </c>
       <c r="BE4" t="s">
+        <v>26</v>
+      </c>
+      <c r="BF4" t="s">
         <v>27</v>
       </c>
-      <c r="BF4" t="s">
+      <c r="BG4" t="s">
         <v>28</v>
       </c>
-      <c r="BG4" t="s">
+      <c r="BH4" t="s">
+        <v>7</v>
+      </c>
+      <c r="BJ4" t="s">
+        <v>31</v>
+      </c>
+      <c r="BK4" t="s">
         <v>29</v>
       </c>
-      <c r="BH4" t="s">
-        <v>8</v>
-      </c>
-      <c r="BJ4" t="s">
-        <v>32</v>
-      </c>
-      <c r="BK4" t="s">
+      <c r="BL4" t="s">
         <v>30</v>
-      </c>
-      <c r="BL4" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:67">
@@ -4648,8 +4698,19 @@
         <v>1726.2860000000001</v>
       </c>
       <c r="G5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5">
+        <f>AVERAGE(I15:I17)</f>
+        <v>1078.9452739999999</v>
+      </c>
+      <c r="J5" t="e">
+        <f>AVERAGE(J15:J17)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K5" t="e">
+        <f>AVERAGE(K15:K17)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L5" s="5"/>
       <c r="M5" s="5"/>
       <c r="N5">
@@ -4709,6 +4770,14 @@
         <f>AVERAGE(AY15:AY19)</f>
         <v>1960.7150000000001</v>
       </c>
+      <c r="BB5" t="e">
+        <f>AVERAGE(BB15:BB17)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="BC5" t="e">
+        <f>AVERAGE(BC15:BC17)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="BD5">
         <v>1</v>
       </c>
@@ -4758,16 +4827,19 @@
         <v>1778.7939999999999</v>
       </c>
       <c r="G6" s="5"/>
-      <c r="H6">
-        <f t="shared" ref="H6:I11" si="1">B$5/(B6*$A6)</f>
-        <v>1.2320568390955431</v>
-      </c>
+      <c r="H6" s="5"/>
       <c r="I6">
-        <f t="shared" si="1"/>
-        <v>1.1743878905836482</v>
-      </c>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
+        <f>AVERAGE(I18:I20)</f>
+        <v>547.77801666666664</v>
+      </c>
+      <c r="J6" t="e">
+        <f>AVERAGE(J18:J20)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K6" t="e">
+        <f>AVERAGE(K18:K20)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L6" s="5"/>
       <c r="M6" s="5"/>
       <c r="N6">
@@ -4803,11 +4875,11 @@
         <v>4943.416666666667</v>
       </c>
       <c r="AF6">
-        <f t="shared" ref="AF6:AG11" si="2">(AA$5*$Z5)/(AA6*$Z6)</f>
+        <f t="shared" ref="AF6:AG11" si="1">(AA$5*$Z5)/(AA6*$Z6)</f>
         <v>0.7079279516171445</v>
       </c>
       <c r="AG6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.83542826317830099</v>
       </c>
       <c r="AL6">
@@ -4842,9 +4914,13 @@
         <f>AVERAGE(AY20:AY24)</f>
         <v>1225.6000000000001</v>
       </c>
-      <c r="BB6">
-        <f t="shared" ref="BB6:BB11" si="3">(AY$5*$AX$5)/(AY6*$AX6)</f>
-        <v>0.79990004895561351</v>
+      <c r="BB6" t="e">
+        <f>AVERAGE(BB18:BB20)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="BC6" t="e">
+        <f>AVERAGE(BC18:BC20)</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="BD6">
         <v>2</v>
@@ -4898,15 +4974,19 @@
         <v>415.86</v>
       </c>
       <c r="G7" s="5"/>
-      <c r="H7">
-        <f t="shared" si="1"/>
-        <v>2.4370477732062477</v>
-      </c>
+      <c r="H7" s="5"/>
       <c r="I7">
-        <f t="shared" si="1"/>
-        <v>1.834988539043976</v>
-      </c>
-      <c r="K7" s="5"/>
+        <f>AVERAGE(I21:I23)</f>
+        <v>283.11835533333334</v>
+      </c>
+      <c r="J7" t="e">
+        <f>AVERAGE(J21:J23)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K7" t="e">
+        <f>AVERAGE(K21:K23)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
       <c r="N7">
@@ -4946,11 +5026,11 @@
         <v>1943.665</v>
       </c>
       <c r="AF7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.3977856603801577</v>
       </c>
       <c r="AG7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2.1247848780525449</v>
       </c>
       <c r="AL7">
@@ -4989,9 +5069,13 @@
         <f>AVERAGE(AZ25:AZ29)</f>
         <v>26946.7</v>
       </c>
-      <c r="BB7">
-        <f t="shared" si="3"/>
-        <v>0.85643181619638331</v>
+      <c r="BB7" t="e">
+        <f>AVERAGE(BB21:BB23)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="BC7" t="e">
+        <f>AVERAGE(BC21:BC23)</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="BD7">
         <v>4</v>
@@ -5048,19 +5132,19 @@
         <f>AVERAGE(G30:G34)</f>
         <v>5339.2460000000001</v>
       </c>
-      <c r="H8">
-        <f t="shared" si="1"/>
-        <v>2.6869566052063516</v>
-      </c>
+      <c r="H8" s="5"/>
       <c r="I8">
-        <f t="shared" si="1"/>
-        <v>2.6884118988752106</v>
-      </c>
-      <c r="J8" s="5">
-        <f>(D$7*$A$7)/(D8*$A8)</f>
-        <v>0.97449866673980812</v>
-      </c>
-      <c r="K8" s="5"/>
+        <f>AVERAGE(I24:I26)</f>
+        <v>148.15255566666667</v>
+      </c>
+      <c r="J8" t="e">
+        <f>AVERAGE(J24:J26)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K8" t="e">
+        <f>AVERAGE(K24:K26)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L8" s="5"/>
       <c r="M8" s="5"/>
       <c r="N8">
@@ -5107,11 +5191,11 @@
         <v>23233</v>
       </c>
       <c r="AF8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>4.1193571479313871</v>
       </c>
       <c r="AG8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>6.5626175657245778</v>
       </c>
       <c r="AL8">
@@ -5150,13 +5234,13 @@
         <f>AVERAGE(AZ30:AZ34)</f>
         <v>11218.55</v>
       </c>
-      <c r="BB8">
-        <f t="shared" si="3"/>
-        <v>1.138333089493766</v>
-      </c>
-      <c r="BC8">
-        <f>(AZ$7*$AX$7)/(AZ8*$AX8)</f>
-        <v>1.2009885412999006</v>
+      <c r="BB8" t="e">
+        <f>AVERAGE(BB24:BB26)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="BC8" t="e">
+        <f>AVERAGE(BC24:BC26)</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="BD8">
         <v>8</v>
@@ -5213,19 +5297,19 @@
         <f>AVERAGE(G35:G39)</f>
         <v>4771.5380000000005</v>
       </c>
-      <c r="H9">
-        <f t="shared" si="1"/>
-        <v>2.3772703082184026</v>
-      </c>
+      <c r="H9" s="5"/>
       <c r="I9">
-        <f t="shared" si="1"/>
-        <v>1.7193409896209899</v>
-      </c>
-      <c r="J9" s="5">
-        <f>(D$7*$A$7)/(D9*$A9)</f>
-        <v>0.51505469079147037</v>
-      </c>
-      <c r="K9" s="5"/>
+        <f>AVERAGE(I27:I29)</f>
+        <v>81.215220666666653</v>
+      </c>
+      <c r="J9" t="e">
+        <f>AVERAGE(J27:J29)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K9" t="e">
+        <f>AVERAGE(K27:K29)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L9" s="5"/>
       <c r="M9" s="5"/>
       <c r="N9">
@@ -5272,11 +5356,11 @@
         <v>11092.400000000001</v>
       </c>
       <c r="AF9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>18.268723242038597</v>
       </c>
       <c r="AG9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>16.420941215951316</v>
       </c>
       <c r="AH9">
@@ -5323,13 +5407,13 @@
         <f>AVERAGE(AZ35:AZ39)</f>
         <v>7944.1559999999999</v>
       </c>
-      <c r="BB9">
-        <f t="shared" si="3"/>
-        <v>1.4396893507947242</v>
-      </c>
-      <c r="BC9">
-        <f>(AZ$7*$AX$7)/(AZ9*$AX9)</f>
-        <v>0.84800386598651889</v>
+      <c r="BB9" t="e">
+        <f>AVERAGE(BB27:BB29)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="BC9" t="e">
+        <f>AVERAGE(BC27:BC29)</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="BD9">
         <v>16</v>
@@ -5389,19 +5473,19 @@
         <f>AVERAGE(G40:G44)</f>
         <v>2144.6379999999999</v>
       </c>
-      <c r="H10">
-        <f t="shared" si="1"/>
-        <v>1.7282102864898932</v>
-      </c>
+      <c r="H10" s="5"/>
       <c r="I10">
-        <f t="shared" si="1"/>
-        <v>1.5160162495182494</v>
-      </c>
-      <c r="J10" s="5">
-        <f>(D$7*$A$7)/(D10*$A10)</f>
-        <v>0.6019144138182233</v>
-      </c>
-      <c r="K10" s="5"/>
+        <f>AVERAGE(I30:I32)</f>
+        <v>53.875178000000005</v>
+      </c>
+      <c r="J10" t="e">
+        <f>AVERAGE(J30:J32)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K10" t="e">
+        <f>AVERAGE(K30:K32)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L10" s="5"/>
       <c r="M10" s="5"/>
       <c r="N10">
@@ -5448,11 +5532,11 @@
         <v>5725.9760000000006</v>
       </c>
       <c r="AF10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>35.612781919366583</v>
       </c>
       <c r="AG10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>29.094327766020694</v>
       </c>
       <c r="AH10">
@@ -5503,13 +5587,13 @@
         <f>AVERAGE(AZ40:AZ44)</f>
         <v>6511.4820000000009</v>
       </c>
-      <c r="BB10">
-        <f t="shared" si="3"/>
-        <v>0.94104095928752096</v>
-      </c>
-      <c r="BC10">
-        <f>(AZ$7*$AX$7)/(AZ10*$AX10)</f>
-        <v>0.51729199282129623</v>
+      <c r="BB10" t="e">
+        <f>AVERAGE(BB30:BB32)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="BC10" t="e">
+        <f>AVERAGE(BC30:BC32)</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="BD10">
         <v>32</v>
@@ -5577,19 +5661,19 @@
         <f>AVERAGE(G45:G49)</f>
         <v>792.52080000000001</v>
       </c>
-      <c r="H11">
-        <f t="shared" si="1"/>
-        <v>1.0986964902487528</v>
-      </c>
+      <c r="H11" s="5"/>
       <c r="I11">
-        <f t="shared" si="1"/>
-        <v>3.9262590909711141</v>
-      </c>
-      <c r="J11" s="5">
-        <f>(D$7*$A$7)/(D11*$A11)</f>
-        <v>0.7633459174906827</v>
-      </c>
-      <c r="K11" s="5"/>
+        <f>AVERAGE(I33:I35)</f>
+        <v>42.362321000000001</v>
+      </c>
+      <c r="J11" t="e">
+        <f>AVERAGE(J33:J35)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K11" t="e">
+        <f>AVERAGE(K33:K35)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L11" s="5"/>
       <c r="M11" s="5"/>
       <c r="N11">
@@ -5640,11 +5724,11 @@
         <v>4201.97</v>
       </c>
       <c r="AF11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>68.011014133963201</v>
       </c>
       <c r="AG11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>41.537992064686243</v>
       </c>
       <c r="AH11">
@@ -5695,13 +5779,13 @@
         <f>AVERAGE(AZ45:AZ49)</f>
         <v>3370.9660000000003</v>
       </c>
-      <c r="BB11">
-        <f t="shared" si="3"/>
-        <v>0.82060896244280601</v>
-      </c>
-      <c r="BC11">
-        <f>(AZ$7*$AX$7)/(AZ11*$AX11)</f>
-        <v>0.49961012659279264</v>
+      <c r="BB11" t="e">
+        <f>AVERAGE(BB33:BB35)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="BC11" t="e">
+        <f>AVERAGE(BC33:BC35)</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="BD11">
         <v>64</v>
@@ -5751,12 +5835,12 @@
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
-      <c r="J12" s="3"/>
+      <c r="H12" s="3"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
@@ -5766,7 +5850,7 @@
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="R12" s="1"/>
       <c r="BD12">
@@ -5790,6 +5874,12 @@
       <c r="F15">
         <v>1720.91</v>
       </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <v>1079.593286</v>
+      </c>
       <c r="N15">
         <v>1</v>
       </c>
@@ -5798,7 +5888,7 @@
         <v>29.257333333333335</v>
       </c>
       <c r="P15">
-        <f t="shared" ref="P15:P35" si="4">P41/6</f>
+        <f t="shared" ref="P15:P35" si="2">P41/6</f>
         <v>1525.6366666666665</v>
       </c>
       <c r="T15">
@@ -5837,6 +5927,9 @@
       </c>
       <c r="AY15">
         <v>1955.19</v>
+      </c>
+      <c r="BA15">
+        <v>1</v>
       </c>
       <c r="BD15">
         <v>1</v>
@@ -5867,22 +5960,28 @@
       <c r="F16">
         <v>1654.11</v>
       </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>1077.4435309999999</v>
+      </c>
       <c r="N16">
         <v>1</v>
       </c>
       <c r="O16">
-        <f t="shared" ref="O16:O35" si="5">O42/6</f>
+        <f t="shared" ref="O16:O35" si="3">O42/6</f>
         <v>28.227666666666668</v>
       </c>
       <c r="P16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>1534.99</v>
       </c>
       <c r="T16">
         <v>1</v>
       </c>
       <c r="U16">
-        <f t="shared" ref="U16:V49" si="6">U52/6</f>
+        <f t="shared" ref="U16:V49" si="4">U52/6</f>
         <v>0.30325666666666667</v>
       </c>
       <c r="Z16">
@@ -5911,6 +6010,9 @@
       </c>
       <c r="AY16">
         <v>1966.24</v>
+      </c>
+      <c r="BA16">
+        <v>1</v>
       </c>
       <c r="BD16">
         <v>1</v>
@@ -5935,22 +6037,28 @@
       <c r="F17">
         <v>1979.91</v>
       </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>1079.7990050000001</v>
+      </c>
       <c r="N17">
         <v>1</v>
       </c>
       <c r="O17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>28.108999999999998</v>
       </c>
       <c r="P17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>1527.7416666666668</v>
       </c>
       <c r="T17">
         <v>1</v>
       </c>
       <c r="U17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.30329166666666668</v>
       </c>
       <c r="Z17">
@@ -5966,6 +6074,9 @@
         <v>344.649</v>
       </c>
       <c r="AX17">
+        <v>1</v>
+      </c>
+      <c r="BA17">
         <v>1</v>
       </c>
       <c r="BD17">
@@ -5991,22 +6102,28 @@
       <c r="F18">
         <v>1633.32</v>
       </c>
+      <c r="H18">
+        <v>2</v>
+      </c>
+      <c r="I18">
+        <v>549.52244399999995</v>
+      </c>
       <c r="N18">
         <v>2</v>
       </c>
       <c r="O18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>15.786033333333334</v>
       </c>
       <c r="P18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>822.11833333333334</v>
       </c>
       <c r="T18">
         <v>1</v>
       </c>
       <c r="U18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.30324499999999999</v>
       </c>
       <c r="Z18">
@@ -6023,6 +6140,9 @@
       </c>
       <c r="AX18">
         <v>1</v>
+      </c>
+      <c r="BA18">
+        <v>2</v>
       </c>
       <c r="BD18">
         <v>1</v>
@@ -6047,22 +6167,28 @@
       <c r="F19">
         <v>1643.18</v>
       </c>
+      <c r="H19">
+        <v>2</v>
+      </c>
+      <c r="I19">
+        <v>548.068759</v>
+      </c>
       <c r="N19">
         <v>2</v>
       </c>
       <c r="O19">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>15.785266666666667</v>
       </c>
       <c r="P19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>818.54333333333341</v>
       </c>
       <c r="T19">
         <v>1</v>
       </c>
       <c r="U19">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.30421333333333334</v>
       </c>
       <c r="Z19">
@@ -6076,6 +6202,9 @@
       </c>
       <c r="AX19">
         <v>1</v>
+      </c>
+      <c r="BA19">
+        <v>2</v>
       </c>
       <c r="BD19">
         <v>1</v>
@@ -6100,26 +6229,32 @@
       <c r="F20">
         <v>1701.39</v>
       </c>
+      <c r="H20">
+        <v>2</v>
+      </c>
+      <c r="I20">
+        <v>545.74284699999998</v>
+      </c>
       <c r="N20">
         <v>2</v>
       </c>
       <c r="O20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>16.871333333333332</v>
       </c>
       <c r="P20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>817.12166666666656</v>
       </c>
       <c r="T20">
         <v>2</v>
       </c>
       <c r="U20">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.12201433333333334</v>
       </c>
       <c r="V20">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>3.6693833333333337</v>
       </c>
       <c r="Z20">
@@ -6151,6 +6286,9 @@
       </c>
       <c r="AY20">
         <v>1237.76</v>
+      </c>
+      <c r="BA20">
+        <v>2</v>
       </c>
       <c r="BD20">
         <v>2</v>
@@ -6181,30 +6319,36 @@
       <c r="F21">
         <v>1691.11</v>
       </c>
+      <c r="H21">
+        <v>4</v>
+      </c>
+      <c r="I21">
+        <v>282.240116</v>
+      </c>
       <c r="N21">
         <v>4</v>
       </c>
       <c r="O21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>4.3326666666666664</v>
       </c>
       <c r="P21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>318.48833333333334</v>
       </c>
       <c r="S21">
-        <f t="shared" ref="S21:S35" si="7">S47/6</f>
+        <f t="shared" ref="S21:S35" si="5">S47/6</f>
         <v>353.12833333333333</v>
       </c>
       <c r="T21">
         <v>2</v>
       </c>
       <c r="U21">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.12170983333333334</v>
       </c>
       <c r="V21">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>3.6611666666666665</v>
       </c>
       <c r="Z21">
@@ -6236,6 +6380,9 @@
       </c>
       <c r="AY21">
         <v>1222.57</v>
+      </c>
+      <c r="BA21">
+        <v>4</v>
       </c>
       <c r="BD21">
         <v>2</v>
@@ -6266,30 +6413,36 @@
       <c r="F22">
         <v>1614.29</v>
       </c>
+      <c r="H22">
+        <v>4</v>
+      </c>
+      <c r="I22">
+        <v>282.75658600000003</v>
+      </c>
       <c r="N22">
         <v>4</v>
       </c>
       <c r="O22">
+        <f t="shared" si="3"/>
+        <v>4.0477166666666671</v>
+      </c>
+      <c r="P22">
+        <f t="shared" si="2"/>
+        <v>319.59499999999997</v>
+      </c>
+      <c r="S22">
         <f t="shared" si="5"/>
-        <v>4.0477166666666671</v>
-      </c>
-      <c r="P22">
-        <f t="shared" si="4"/>
-        <v>319.59499999999997</v>
-      </c>
-      <c r="S22">
-        <f t="shared" si="7"/>
         <v>354.64166666666665</v>
       </c>
       <c r="T22">
         <v>2</v>
       </c>
       <c r="U22">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.12155266666666666</v>
       </c>
       <c r="V22">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>3.6710999999999996</v>
       </c>
       <c r="Z22">
@@ -6321,6 +6474,9 @@
       </c>
       <c r="AY22">
         <v>1216.47</v>
+      </c>
+      <c r="BA22">
+        <v>4</v>
       </c>
       <c r="BD22">
         <v>2</v>
@@ -6351,30 +6507,36 @@
       <c r="F23">
         <v>2187.87</v>
       </c>
+      <c r="H23">
+        <v>4</v>
+      </c>
+      <c r="I23">
+        <v>284.35836399999999</v>
+      </c>
       <c r="N23">
         <v>4</v>
       </c>
       <c r="O23">
+        <f t="shared" si="3"/>
+        <v>4.3674333333333335</v>
+      </c>
+      <c r="P23">
+        <f t="shared" si="2"/>
+        <v>341.35500000000002</v>
+      </c>
+      <c r="S23">
         <f t="shared" si="5"/>
-        <v>4.3674333333333335</v>
-      </c>
-      <c r="P23">
-        <f t="shared" si="4"/>
-        <v>341.35500000000002</v>
-      </c>
-      <c r="S23">
-        <f t="shared" si="7"/>
         <v>353.95166666666665</v>
       </c>
       <c r="T23">
         <v>2</v>
       </c>
       <c r="U23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.1214755</v>
       </c>
       <c r="V23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>3.6918666666666664</v>
       </c>
       <c r="Z23">
@@ -6397,6 +6559,9 @@
       </c>
       <c r="AX23">
         <v>2</v>
+      </c>
+      <c r="BA23">
+        <v>4</v>
       </c>
       <c r="BD23">
         <v>2</v>
@@ -6427,15 +6592,21 @@
       <c r="F24">
         <v>1699.31</v>
       </c>
+      <c r="H24">
+        <v>8</v>
+      </c>
+      <c r="I24">
+        <v>149.199085</v>
+      </c>
       <c r="N24">
         <v>8</v>
       </c>
       <c r="O24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>1.4921433333333332</v>
       </c>
       <c r="P24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>118.63850000000001</v>
       </c>
       <c r="Q24">
@@ -6443,18 +6614,18 @@
         <v>3873.4800000000005</v>
       </c>
       <c r="S24">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>188.99666666666667</v>
       </c>
       <c r="T24">
         <v>2</v>
       </c>
       <c r="U24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.12145466666666667</v>
       </c>
       <c r="V24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>3.6889333333333334</v>
       </c>
       <c r="Z24">
@@ -6468,6 +6639,9 @@
       </c>
       <c r="AX24">
         <v>2</v>
+      </c>
+      <c r="BA24">
+        <v>8</v>
       </c>
       <c r="BD24">
         <v>2</v>
@@ -6501,30 +6675,36 @@
       <c r="G25">
         <v>25111.599999999999</v>
       </c>
+      <c r="H25">
+        <v>8</v>
+      </c>
+      <c r="I25">
+        <v>146.720304</v>
+      </c>
       <c r="N25">
         <v>8</v>
       </c>
       <c r="O25">
+        <f t="shared" si="3"/>
+        <v>1.4532866666666668</v>
+      </c>
+      <c r="P25">
+        <f t="shared" si="2"/>
+        <v>117.52050000000001</v>
+      </c>
+      <c r="S25">
         <f t="shared" si="5"/>
-        <v>1.4532866666666668</v>
-      </c>
-      <c r="P25">
-        <f t="shared" si="4"/>
-        <v>117.52050000000001</v>
-      </c>
-      <c r="S25">
-        <f t="shared" si="7"/>
         <v>182.02500000000001</v>
       </c>
       <c r="T25">
         <v>4</v>
       </c>
       <c r="U25">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>7.0817333333333329E-2</v>
       </c>
       <c r="V25">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>2.0156166666666668</v>
       </c>
       <c r="Z25">
@@ -6559,6 +6739,9 @@
       </c>
       <c r="AZ25">
         <v>26727.5</v>
+      </c>
+      <c r="BA25">
+        <v>8</v>
       </c>
       <c r="BD25">
         <v>4</v>
@@ -6592,30 +6775,36 @@
       <c r="F26">
         <v>372.5</v>
       </c>
+      <c r="H26">
+        <v>8</v>
+      </c>
+      <c r="I26">
+        <v>148.53827799999999</v>
+      </c>
       <c r="N26">
         <v>8</v>
       </c>
       <c r="O26">
+        <f t="shared" si="3"/>
+        <v>1.4858616666666666</v>
+      </c>
+      <c r="P26">
+        <f t="shared" si="2"/>
+        <v>117.2675</v>
+      </c>
+      <c r="S26">
         <f t="shared" si="5"/>
-        <v>1.4858616666666666</v>
-      </c>
-      <c r="P26">
-        <f t="shared" si="4"/>
-        <v>117.2675</v>
-      </c>
-      <c r="S26">
-        <f t="shared" si="7"/>
         <v>201.66333333333333</v>
       </c>
       <c r="T26">
         <v>4</v>
       </c>
       <c r="U26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>7.0219999999999991E-2</v>
       </c>
       <c r="V26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>2.0112833333333335</v>
       </c>
       <c r="Z26">
@@ -6650,6 +6839,9 @@
       </c>
       <c r="AZ26">
         <v>27165.9</v>
+      </c>
+      <c r="BA26">
+        <v>8</v>
       </c>
       <c r="BD26">
         <v>4</v>
@@ -6683,34 +6875,40 @@
       <c r="F27">
         <v>566.19200000000001</v>
       </c>
+      <c r="H27">
+        <v>16</v>
+      </c>
+      <c r="I27">
+        <v>81.227279999999993</v>
+      </c>
       <c r="N27">
         <v>16</v>
       </c>
       <c r="O27">
+        <f t="shared" si="3"/>
+        <v>0.68832833333333332</v>
+      </c>
+      <c r="P27">
+        <f t="shared" si="2"/>
+        <v>48.26</v>
+      </c>
+      <c r="Q27">
+        <f t="shared" ref="Q27:Q35" si="6">Q53/5</f>
+        <v>2026.2</v>
+      </c>
+      <c r="S27">
         <f t="shared" si="5"/>
-        <v>0.68832833333333332</v>
-      </c>
-      <c r="P27">
-        <f t="shared" si="4"/>
-        <v>48.26</v>
-      </c>
-      <c r="Q27">
-        <f t="shared" ref="Q27:Q35" si="8">Q53/5</f>
-        <v>2026.2</v>
-      </c>
-      <c r="S27">
-        <f t="shared" si="7"/>
         <v>46.771999999999998</v>
       </c>
       <c r="T27">
         <v>4</v>
       </c>
       <c r="U27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>7.0446500000000009E-2</v>
       </c>
       <c r="V27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>2.0166999999999997</v>
       </c>
       <c r="Z27">
@@ -6742,6 +6940,9 @@
       </c>
       <c r="AY27">
         <v>574.04200000000003</v>
+      </c>
+      <c r="BA27">
+        <v>16</v>
       </c>
       <c r="BD27">
         <v>4</v>
@@ -6775,34 +6976,40 @@
       <c r="F28">
         <v>394.35899999999998</v>
       </c>
+      <c r="H28">
+        <v>16</v>
+      </c>
+      <c r="I28">
+        <v>81.025633999999997</v>
+      </c>
       <c r="N28">
         <v>16</v>
       </c>
       <c r="O28">
+        <f t="shared" si="3"/>
+        <v>0.70209500000000002</v>
+      </c>
+      <c r="P28">
+        <f t="shared" si="2"/>
+        <v>40.335999999999999</v>
+      </c>
+      <c r="Q28">
+        <f t="shared" si="6"/>
+        <v>2057.16</v>
+      </c>
+      <c r="S28">
         <f t="shared" si="5"/>
-        <v>0.70209500000000002</v>
-      </c>
-      <c r="P28">
-        <f t="shared" si="4"/>
-        <v>40.335999999999999</v>
-      </c>
-      <c r="Q28">
-        <f t="shared" si="8"/>
-        <v>2057.16</v>
-      </c>
-      <c r="S28">
-        <f t="shared" si="7"/>
         <v>46.135666666666673</v>
       </c>
       <c r="T28">
         <v>4</v>
       </c>
       <c r="U28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>7.0028833333333332E-2</v>
       </c>
       <c r="V28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>2.0131333333333332</v>
       </c>
       <c r="Z28">
@@ -6831,6 +7038,9 @@
       </c>
       <c r="AX28">
         <v>4</v>
+      </c>
+      <c r="BA28">
+        <v>16</v>
       </c>
       <c r="BD28">
         <v>4</v>
@@ -6861,30 +7071,36 @@
       <c r="F29">
         <v>370.11700000000002</v>
       </c>
+      <c r="H29">
+        <v>16</v>
+      </c>
+      <c r="I29">
+        <v>81.392747999999997</v>
+      </c>
       <c r="N29">
         <v>16</v>
       </c>
       <c r="O29">
+        <f t="shared" si="3"/>
+        <v>0.67072000000000009</v>
+      </c>
+      <c r="P29">
+        <f t="shared" si="2"/>
+        <v>42.962833333333329</v>
+      </c>
+      <c r="S29">
         <f t="shared" si="5"/>
-        <v>0.67072000000000009</v>
-      </c>
-      <c r="P29">
-        <f t="shared" si="4"/>
-        <v>42.962833333333329</v>
-      </c>
-      <c r="S29">
-        <f t="shared" si="7"/>
         <v>47.12833333333333</v>
       </c>
       <c r="T29">
         <v>4</v>
       </c>
       <c r="U29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>7.0458333333333331E-2</v>
       </c>
       <c r="V29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>2.0175666666666667</v>
       </c>
       <c r="Z29">
@@ -6901,6 +7117,9 @@
       </c>
       <c r="AX29">
         <v>4</v>
+      </c>
+      <c r="BA29">
+        <v>16</v>
       </c>
       <c r="BD29">
         <v>4</v>
@@ -6937,34 +7156,40 @@
       <c r="G30">
         <v>5372.73</v>
       </c>
+      <c r="H30">
+        <v>32</v>
+      </c>
+      <c r="I30">
+        <v>54.579166999999998</v>
+      </c>
       <c r="N30">
         <v>32</v>
       </c>
       <c r="O30">
+        <f t="shared" si="3"/>
+        <v>0.36327333333333334</v>
+      </c>
+      <c r="P30">
+        <f t="shared" si="2"/>
+        <v>23.622333333333334</v>
+      </c>
+      <c r="Q30">
+        <f t="shared" si="6"/>
+        <v>1018.1420000000001</v>
+      </c>
+      <c r="S30">
         <f t="shared" si="5"/>
-        <v>0.36327333333333334</v>
-      </c>
-      <c r="P30">
-        <f t="shared" si="4"/>
-        <v>23.622333333333334</v>
-      </c>
-      <c r="Q30">
-        <f t="shared" si="8"/>
-        <v>1018.1420000000001</v>
-      </c>
-      <c r="S30">
-        <f t="shared" si="7"/>
         <v>21.552000000000003</v>
       </c>
       <c r="T30">
         <v>8</v>
       </c>
       <c r="U30">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>3.5843E-2</v>
       </c>
       <c r="V30">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>1.0692066666666666</v>
       </c>
       <c r="Z30">
@@ -7002,6 +7227,9 @@
       </c>
       <c r="AZ30">
         <v>11377.8</v>
+      </c>
+      <c r="BA30">
+        <v>32</v>
       </c>
       <c r="BD30">
         <v>8</v>
@@ -7041,26 +7269,32 @@
       <c r="G31">
         <v>5308.38</v>
       </c>
+      <c r="H31">
+        <v>32</v>
+      </c>
+      <c r="I31">
+        <v>52.603828</v>
+      </c>
       <c r="N31">
         <v>32</v>
       </c>
       <c r="O31">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0.37943333333333334</v>
       </c>
       <c r="Q31">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>921.78199999999993</v>
       </c>
       <c r="T31">
         <v>8</v>
       </c>
       <c r="U31">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>3.5554666666666665E-2</v>
       </c>
       <c r="V31">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>1.0697650000000001</v>
       </c>
       <c r="Z31">
@@ -7095,6 +7329,9 @@
       </c>
       <c r="AZ31">
         <v>11059.3</v>
+      </c>
+      <c r="BA31">
+        <v>32</v>
       </c>
       <c r="BD31">
         <v>8</v>
@@ -7134,26 +7371,32 @@
       <c r="G32">
         <v>5314.03</v>
       </c>
+      <c r="H32">
+        <v>32</v>
+      </c>
+      <c r="I32">
+        <v>54.442538999999996</v>
+      </c>
       <c r="N32">
         <v>32</v>
       </c>
       <c r="O32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0.36234000000000005</v>
       </c>
       <c r="Q32">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>926.99799999999993</v>
       </c>
       <c r="T32">
         <v>8</v>
       </c>
       <c r="U32">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>3.5790166666666665E-2</v>
       </c>
       <c r="V32">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>1.0616366666666666</v>
       </c>
       <c r="Z32">
@@ -7185,6 +7428,9 @@
       </c>
       <c r="AY32">
         <v>207.96</v>
+      </c>
+      <c r="BA32">
+        <v>32</v>
       </c>
       <c r="BD32">
         <v>8</v>
@@ -7221,34 +7467,40 @@
       <c r="G33">
         <v>5342.14</v>
       </c>
+      <c r="H33">
+        <v>64</v>
+      </c>
+      <c r="I33">
+        <v>42.766230999999998</v>
+      </c>
       <c r="N33">
         <v>64</v>
       </c>
       <c r="O33">
+        <f t="shared" si="3"/>
+        <v>0.17820499999999997</v>
+      </c>
+      <c r="P33">
+        <f t="shared" si="2"/>
+        <v>5.1360166666666665</v>
+      </c>
+      <c r="Q33">
+        <f t="shared" si="6"/>
+        <v>391.11599999999999</v>
+      </c>
+      <c r="S33">
         <f t="shared" si="5"/>
-        <v>0.17820499999999997</v>
-      </c>
-      <c r="P33">
-        <f t="shared" si="4"/>
-        <v>5.1360166666666665</v>
-      </c>
-      <c r="Q33">
-        <f t="shared" si="8"/>
-        <v>391.11599999999999</v>
-      </c>
-      <c r="S33">
-        <f t="shared" si="7"/>
         <v>5.3251999999999997</v>
       </c>
       <c r="T33">
         <v>8</v>
       </c>
       <c r="U33">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>3.5815E-2</v>
       </c>
       <c r="V33">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>1.0692233333333332</v>
       </c>
       <c r="Z33">
@@ -7280,6 +7532,9 @@
       </c>
       <c r="AY33">
         <v>220.911</v>
+      </c>
+      <c r="BA33">
+        <v>64</v>
       </c>
       <c r="BD33">
         <v>8</v>
@@ -7316,34 +7571,40 @@
       <c r="G34">
         <v>5358.95</v>
       </c>
+      <c r="H34">
+        <v>64</v>
+      </c>
+      <c r="I34">
+        <v>41.716487000000001</v>
+      </c>
       <c r="N34">
         <v>64</v>
       </c>
       <c r="O34">
+        <f t="shared" si="3"/>
+        <v>0.19303666666666666</v>
+      </c>
+      <c r="P34">
+        <f t="shared" si="2"/>
+        <v>4.9707833333333333</v>
+      </c>
+      <c r="Q34">
+        <f t="shared" si="6"/>
+        <v>393.416</v>
+      </c>
+      <c r="S34">
         <f t="shared" si="5"/>
-        <v>0.19303666666666666</v>
-      </c>
-      <c r="P34">
-        <f t="shared" si="4"/>
-        <v>4.9707833333333333</v>
-      </c>
-      <c r="Q34">
-        <f t="shared" si="8"/>
-        <v>393.416</v>
-      </c>
-      <c r="S34">
-        <f t="shared" si="7"/>
         <v>5.3508500000000003</v>
       </c>
       <c r="T34">
         <v>8</v>
       </c>
       <c r="U34">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>3.5753666666666663E-2</v>
       </c>
       <c r="V34">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>1.0697733333333332</v>
       </c>
       <c r="Z34">
@@ -7360,6 +7621,9 @@
       </c>
       <c r="AX34">
         <v>8</v>
+      </c>
+      <c r="BA34">
+        <v>64</v>
       </c>
       <c r="BD34">
         <v>8</v>
@@ -7396,34 +7660,40 @@
       <c r="G35">
         <v>4782.57</v>
       </c>
+      <c r="H35">
+        <v>64</v>
+      </c>
+      <c r="I35">
+        <v>42.604244999999999</v>
+      </c>
       <c r="N35">
         <v>64</v>
       </c>
       <c r="O35">
+        <f t="shared" si="3"/>
+        <v>0.18193499999999999</v>
+      </c>
+      <c r="P35">
+        <f t="shared" si="2"/>
+        <v>4.9496500000000001</v>
+      </c>
+      <c r="Q35">
+        <f t="shared" si="6"/>
+        <v>389.666</v>
+      </c>
+      <c r="S35">
         <f t="shared" si="5"/>
-        <v>0.18193499999999999</v>
-      </c>
-      <c r="P35">
-        <f t="shared" si="4"/>
-        <v>4.9496500000000001</v>
-      </c>
-      <c r="Q35">
-        <f t="shared" si="8"/>
-        <v>389.666</v>
-      </c>
-      <c r="S35">
-        <f t="shared" si="7"/>
         <v>5.3311999999999999</v>
       </c>
       <c r="T35">
         <v>16</v>
       </c>
       <c r="U35">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>1.8580333333333334E-2</v>
       </c>
       <c r="V35">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.57930166666666671</v>
       </c>
       <c r="Z35">
@@ -7464,6 +7734,9 @@
       </c>
       <c r="AZ35">
         <v>5599.24</v>
+      </c>
+      <c r="BA35">
+        <v>64</v>
       </c>
       <c r="BD35">
         <v>16</v>
@@ -7518,11 +7791,11 @@
         <v>16</v>
       </c>
       <c r="U36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>1.847E-2</v>
       </c>
       <c r="V36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.57502500000000001</v>
       </c>
       <c r="Z36">
@@ -7614,11 +7887,11 @@
         <v>16</v>
       </c>
       <c r="U37">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>1.8494E-2</v>
       </c>
       <c r="V37">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.57332666666666665</v>
       </c>
       <c r="Z37">
@@ -7704,11 +7977,11 @@
         <v>16</v>
       </c>
       <c r="U38">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>1.8281666666666665E-2</v>
       </c>
       <c r="V38">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.56794</v>
       </c>
       <c r="Z38">
@@ -7783,11 +8056,11 @@
         <v>16</v>
       </c>
       <c r="U39">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>1.8302666666666665E-2</v>
       </c>
       <c r="V39">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.56923166666666669</v>
       </c>
       <c r="Z39">
@@ -7862,11 +8135,11 @@
         <v>32</v>
       </c>
       <c r="U40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>9.3031666666666662E-3</v>
       </c>
       <c r="V40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.30254500000000001</v>
       </c>
       <c r="Z40">
@@ -7966,11 +8239,11 @@
         <v>32</v>
       </c>
       <c r="U41">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>9.3416833333333331E-3</v>
       </c>
       <c r="V41">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.29609000000000002</v>
       </c>
       <c r="Z41">
@@ -8067,11 +8340,11 @@
         <v>32</v>
       </c>
       <c r="U42">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>9.3135000000000006E-3</v>
       </c>
       <c r="V42">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.29515333333333332</v>
       </c>
       <c r="Z42">
@@ -8165,11 +8438,11 @@
         <v>32</v>
       </c>
       <c r="U43">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>9.3267000000000003E-3</v>
       </c>
       <c r="V43">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.29547166666666663</v>
       </c>
       <c r="Z43">
@@ -8257,11 +8530,11 @@
         <v>32</v>
       </c>
       <c r="U44">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>9.3301500000000006E-3</v>
       </c>
       <c r="V44">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.29611999999999999</v>
       </c>
       <c r="Z44">
@@ -8349,11 +8622,11 @@
         <v>64</v>
       </c>
       <c r="U45">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>4.9721833333333338E-3</v>
       </c>
       <c r="V45">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.15278149999999999</v>
       </c>
       <c r="W45">
@@ -8457,11 +8730,11 @@
         <v>64</v>
       </c>
       <c r="U46">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>4.9183333333333336E-3</v>
       </c>
       <c r="V46">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.151531</v>
       </c>
       <c r="W46">
@@ -8562,11 +8835,11 @@
         <v>64</v>
       </c>
       <c r="U47">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>4.9338333333333335E-3</v>
       </c>
       <c r="V47">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.14907566666666666</v>
       </c>
       <c r="W47">
@@ -8667,11 +8940,11 @@
         <v>64</v>
       </c>
       <c r="U48">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>4.9621666666666668E-3</v>
       </c>
       <c r="V48">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.14682100000000001</v>
       </c>
       <c r="W48">
@@ -8769,11 +9042,11 @@
         <v>64</v>
       </c>
       <c r="U49">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>4.9443166666666661E-3</v>
       </c>
       <c r="V49">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.14617050000000001</v>
       </c>
       <c r="W49">
@@ -9403,6 +9676,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Lots of small edits + some new XMT results.
git-svn-id: svn+ssh://software-srn.sandia.gov/svn/mapreduce/trunk@628 3fc257bb-8550-0410-81b3-a5c103da83f7
</commit_message>
<xml_diff>
--- a/paper/results.xlsx
+++ b/paper/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="-120" windowWidth="21600" windowHeight="13380" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="6500" yWindow="520" windowWidth="21600" windowHeight="13380" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="CC" sheetId="2" r:id="rId1"/>
@@ -52,6 +52,10 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="57">
+  <si>
+    <t>R-MAT 28 (MTGL/XMT)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
   <si>
     <t>R-MAT 24 (MR-MPI)</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -249,15 +253,19 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>R-MAT 24</t>
+    <t>XMT</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>R-MAT 20</t>
+    <t>R-MAT 20 (MR-MPI)</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>R-MAT 28</t>
+    <t>R-MAT 24 (MR-MPI)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>R-MAT 28 (MR-MPI)</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
@@ -265,19 +273,11 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>R-MAT 20 (XMT)</t>
+    <t>R-MAT 20 (MTGL/XMT)</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>R-MAT 24 (XMT)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>R-MAT 28 (XMT)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>XMT</t>
+    <t>R-MAT 24 (MTGL/XMT)</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -285,12 +285,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
   <fonts count="5">
     <font>
       <sz val="10"/>
@@ -720,11 +714,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="591463880"/>
-        <c:axId val="591457800"/>
+        <c:axId val="591457496"/>
+        <c:axId val="591451400"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="591463880"/>
+        <c:axId val="591457496"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -751,12 +745,12 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="591457800"/>
+        <c:crossAx val="591451400"/>
         <c:crossesAt val="0.1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="591457800"/>
+        <c:axId val="591451400"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -784,7 +778,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="591463880"/>
+        <c:crossAx val="591457496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1228,11 +1222,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="591655064"/>
-        <c:axId val="591661032"/>
+        <c:axId val="591648584"/>
+        <c:axId val="591654552"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="591655064"/>
+        <c:axId val="591648584"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1257,12 +1251,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="591661032"/>
+        <c:crossAx val="591654552"/>
         <c:crossesAt val="0.0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="591661032"/>
+        <c:axId val="591654552"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1289,7 +1283,7 @@
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="591655064"/>
+        <c:crossAx val="591648584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1736,11 +1730,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="591718264"/>
-        <c:axId val="591724264"/>
+        <c:axId val="591711784"/>
+        <c:axId val="591717784"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="591718264"/>
+        <c:axId val="591711784"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1766,12 +1760,12 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="591724264"/>
+        <c:crossAx val="591717784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="591724264"/>
+        <c:axId val="591717784"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1798,7 +1792,7 @@
         <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="591718264"/>
+        <c:crossAx val="591711784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1831,7 +1825,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>R-MAT 28</c:v>
+                  <c:v>R-MAT 28 (MR-MPI)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1892,15 +1886,15 @@
           </c:yVal>
         </c:ser>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="4"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$4</c:f>
+              <c:f>Sheet1!$J$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>R-MAT 24</c:v>
+                  <c:v>R-MAT 24 (MTGL/XMT)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1937,45 +1931,45 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$5:$C$11</c:f>
+              <c:f>Sheet1!$J$5:$J$11</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>3683.12</c:v>
+                  <c:v>13107.52489833333</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1568.102</c:v>
+                  <c:v>6720.852236</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>501.7906</c:v>
+                  <c:v>3522.589385333333</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>171.2498</c:v>
+                  <c:v>1851.324676666667</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>133.8856</c:v>
+                  <c:v>1018.079687666667</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>75.92102</c:v>
+                  <c:v>877.4851626666667</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>14.6574</c:v>
+                  <c:v>804.2931573333331</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
         </c:ser>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="1"/>
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$4</c:f>
+              <c:f>Sheet1!$C$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>R-MAT 20</c:v>
+                  <c:v>R-MAT 24 (MR-MPI)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2012,6 +2006,156 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
+              <c:f>Sheet1!$C$5:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>3683.12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1568.102</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>501.7906</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>171.2498</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>133.8856</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>75.92102</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14.6574</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$I$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>R-MAT 20 (MTGL/XMT)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$5:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$I$5:$I$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1078.945274</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>547.7780166666666</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>283.1183553333333</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>148.1525556666667</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>81.21522066666665</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>53.875178</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>42.362321</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>R-MAT 20 (MR-MPI)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$5:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
               <c:f>Sheet1!$B$5:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
@@ -2041,11 +2185,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="591763560"/>
-        <c:axId val="591773656"/>
+        <c:axId val="591771864"/>
+        <c:axId val="591777928"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="591763560"/>
+        <c:axId val="591771864"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2072,12 +2216,12 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="591773656"/>
+        <c:crossAx val="591777928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="591773656"/>
+        <c:axId val="591777928"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2105,7 +2249,7 @@
         <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="591763560"/>
+        <c:crossAx val="591771864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2340,17 +2484,17 @@
                   <c:v>5725.976000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4201.97</c:v>
+                  <c:v>2827.016000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="591817128"/>
-        <c:axId val="591827256"/>
+        <c:axId val="591818168"/>
+        <c:axId val="591828264"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="591817128"/>
+        <c:axId val="591818168"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2377,12 +2521,12 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="591827256"/>
+        <c:crossAx val="591828264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="591827256"/>
+        <c:axId val="591828264"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2410,7 +2554,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="591817128"/>
+        <c:crossAx val="591818168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2436,83 +2580,8 @@
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="1"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$AY$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>R-MAT 20 (MR-MPI)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$AX$5:$AX$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>64.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$AY$5:$AY$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>1960.715</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1225.6</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>572.35</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>215.3055</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>85.11884000000001</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>65.11124</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>37.33346</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
           <c:tx>
             <c:strRef>
               <c:f>Sheet1!$AZ$4</c:f>
@@ -2579,11 +2648,224 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="591863912"/>
-        <c:axId val="591876376"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$BC$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>R-MAT 24 (MTGL/XMT)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$AX$5:$AX$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$BC$5:$BC$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="4">
+                  <c:v>2327.839021</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1716.615575</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1879.305053</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$AY$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>R-MAT 20 (MR-MPI)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$AX$5:$AX$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$AY$5:$AY$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1960.715</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1225.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>572.35</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>215.3055</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>85.11884000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>65.11124</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>37.33346</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$BB$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>R-MAT 20 (MTGL/XMT)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$AX$5:$AX$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$BB$5:$BB$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>551.8413753333334</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>318.8881283333333</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>200.4971896666667</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>134.2743096666667</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>99.84311133333334</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>84.12149466666666</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>88.65103666666668</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="591866936"/>
+        <c:axId val="591885368"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="591863912"/>
+        <c:axId val="591866936"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2605,16 +2887,17 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="591876376"/>
+        <c:crossAx val="591885368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="591876376"/>
+        <c:axId val="591885368"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2637,17 +2920,19 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="591863912"/>
+        <c:crossAx val="591866936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -3185,11 +3470,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="591996904"/>
-        <c:axId val="592002680"/>
+        <c:axId val="592007272"/>
+        <c:axId val="592013048"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="591996904"/>
+        <c:axId val="592007272"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -3216,13 +3501,13 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="592002680"/>
+        <c:crossAx val="592013048"/>
         <c:crossesAt val="0.001"/>
         <c:crossBetween val="midCat"/>
         <c:minorUnit val="10.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="592002680"/>
+        <c:axId val="592013048"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -3250,7 +3535,7 @@
         <c:numFmt formatCode="0.E+00" sourceLinked="0"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="591996904"/>
+        <c:crossAx val="592007272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3720,11 +4005,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="592037000"/>
-        <c:axId val="592043000"/>
+        <c:axId val="592047496"/>
+        <c:axId val="592053496"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="592037000"/>
+        <c:axId val="592047496"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -3751,12 +4036,12 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="592043000"/>
+        <c:crossAx val="592053496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="592043000"/>
+        <c:axId val="592053496"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -3784,7 +4069,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="592037000"/>
+        <c:crossAx val="592047496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3855,7 +4140,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr published="0"/>
   <sheetViews>
-    <sheetView zoomScale="116" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="116" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -4433,8 +4718,8 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:BO85"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView view="pageLayout" topLeftCell="X4" workbookViewId="0">
+      <selection activeCell="AC45" sqref="AC45:AC49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -4448,235 +4733,235 @@
   <sheetData>
     <row r="1" spans="1:67">
       <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" t="s">
+        <v>9</v>
+      </c>
+      <c r="T1" t="s">
         <v>20</v>
       </c>
-      <c r="N1" t="s">
-        <v>8</v>
-      </c>
-      <c r="T1" t="s">
+      <c r="Z1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AX1" t="s">
         <v>19</v>
       </c>
-      <c r="Z1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>17</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>18</v>
-      </c>
       <c r="BD1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:67">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="N2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="BD2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:67">
       <c r="C3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="O3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="S3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="U3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="V3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="W3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AM3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AR3" t="s">
+        <v>25</v>
+      </c>
+      <c r="AU3" t="s">
+        <v>26</v>
+      </c>
+      <c r="BB3" t="s">
+        <v>54</v>
+      </c>
+      <c r="BJ3" t="s">
+        <v>23</v>
+      </c>
+      <c r="BK3" t="s">
         <v>24</v>
       </c>
-      <c r="AU3" t="s">
-        <v>25</v>
-      </c>
-      <c r="BB3" t="s">
-        <v>56</v>
-      </c>
-      <c r="BJ3" t="s">
-        <v>22</v>
-      </c>
-      <c r="BK3" t="s">
+      <c r="BL3" t="s">
         <v>23</v>
-      </c>
-      <c r="BL3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:67">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D4" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J4" t="s">
+        <v>56</v>
+      </c>
+      <c r="K4" t="s">
+        <v>0</v>
+      </c>
+      <c r="N4" t="s">
         <v>7</v>
       </c>
-      <c r="F4" t="s">
+      <c r="O4" t="s">
+        <v>45</v>
+      </c>
+      <c r="P4" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>2</v>
+      </c>
+      <c r="R4" t="s">
+        <v>8</v>
+      </c>
+      <c r="S4" t="s">
+        <v>30</v>
+      </c>
+      <c r="U4" t="s">
+        <v>33</v>
+      </c>
+      <c r="V4" t="s">
+        <v>34</v>
+      </c>
+      <c r="W4" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB4" t="s">
         <v>47</v>
       </c>
-      <c r="G4" t="s">
+      <c r="AC4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>7</v>
+      </c>
+      <c r="AM4" t="s">
+        <v>37</v>
+      </c>
+      <c r="AN4" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO4" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AR4" t="s">
+        <v>36</v>
+      </c>
+      <c r="AS4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AT4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AU4" t="s">
+        <v>41</v>
+      </c>
+      <c r="AV4" t="s">
+        <v>42</v>
+      </c>
+      <c r="AW4" t="s">
+        <v>43</v>
+      </c>
+      <c r="AX4" t="s">
+        <v>7</v>
+      </c>
+      <c r="AY4" t="s">
+        <v>37</v>
+      </c>
+      <c r="AZ4" t="s">
+        <v>1</v>
+      </c>
+      <c r="BB4" t="s">
+        <v>55</v>
+      </c>
+      <c r="BC4" t="s">
+        <v>56</v>
+      </c>
+      <c r="BD4" t="s">
+        <v>7</v>
+      </c>
+      <c r="BE4" t="s">
+        <v>27</v>
+      </c>
+      <c r="BF4" t="s">
+        <v>28</v>
+      </c>
+      <c r="BG4" t="s">
+        <v>29</v>
+      </c>
+      <c r="BH4" t="s">
+        <v>8</v>
+      </c>
+      <c r="BJ4" t="s">
+        <v>32</v>
+      </c>
+      <c r="BK4" t="s">
         <v>30</v>
       </c>
-      <c r="I4" t="s">
-        <v>53</v>
-      </c>
-      <c r="J4" t="s">
-        <v>54</v>
-      </c>
-      <c r="K4" t="s">
-        <v>55</v>
-      </c>
-      <c r="N4" t="s">
-        <v>6</v>
-      </c>
-      <c r="O4" t="s">
-        <v>44</v>
-      </c>
-      <c r="P4" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>1</v>
-      </c>
-      <c r="R4" t="s">
-        <v>7</v>
-      </c>
-      <c r="S4" t="s">
-        <v>29</v>
-      </c>
-      <c r="U4" t="s">
-        <v>32</v>
-      </c>
-      <c r="V4" t="s">
-        <v>33</v>
-      </c>
-      <c r="W4" t="s">
-        <v>34</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>6</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>45</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>46</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>1</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>7</v>
-      </c>
-      <c r="AL4" t="s">
-        <v>6</v>
-      </c>
-      <c r="AM4" t="s">
-        <v>36</v>
-      </c>
-      <c r="AN4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AO4" t="s">
-        <v>39</v>
-      </c>
-      <c r="AP4" t="s">
-        <v>7</v>
-      </c>
-      <c r="AR4" t="s">
-        <v>35</v>
-      </c>
-      <c r="AS4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AT4" t="s">
-        <v>4</v>
-      </c>
-      <c r="AU4" t="s">
-        <v>40</v>
-      </c>
-      <c r="AV4" t="s">
-        <v>41</v>
-      </c>
-      <c r="AW4" t="s">
-        <v>42</v>
-      </c>
-      <c r="AX4" t="s">
-        <v>6</v>
-      </c>
-      <c r="AY4" t="s">
-        <v>36</v>
-      </c>
-      <c r="AZ4" t="s">
-        <v>0</v>
-      </c>
-      <c r="BB4" t="s">
-        <v>53</v>
-      </c>
-      <c r="BC4" t="s">
-        <v>54</v>
-      </c>
-      <c r="BD4" t="s">
-        <v>6</v>
-      </c>
-      <c r="BE4" t="s">
-        <v>26</v>
-      </c>
-      <c r="BF4" t="s">
-        <v>27</v>
-      </c>
-      <c r="BG4" t="s">
-        <v>28</v>
-      </c>
-      <c r="BH4" t="s">
-        <v>7</v>
-      </c>
-      <c r="BJ4" t="s">
+      <c r="BL4" t="s">
         <v>31</v>
-      </c>
-      <c r="BK4" t="s">
-        <v>29</v>
-      </c>
-      <c r="BL4" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:67">
@@ -4703,9 +4988,9 @@
         <f>AVERAGE(I15:I17)</f>
         <v>1078.9452739999999</v>
       </c>
-      <c r="J5" t="e">
+      <c r="J5">
         <f>AVERAGE(J15:J17)</f>
-        <v>#DIV/0!</v>
+        <v>13107.524898333331</v>
       </c>
       <c r="K5" t="e">
         <f>AVERAGE(K15:K17)</f>
@@ -4770,13 +5055,9 @@
         <f>AVERAGE(AY15:AY19)</f>
         <v>1960.7150000000001</v>
       </c>
-      <c r="BB5" t="e">
+      <c r="BB5">
         <f>AVERAGE(BB15:BB17)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="BC5" t="e">
-        <f>AVERAGE(BC15:BC17)</f>
-        <v>#DIV/0!</v>
+        <v>551.84137533333342</v>
       </c>
       <c r="BD5">
         <v>1</v>
@@ -4832,9 +5113,9 @@
         <f>AVERAGE(I18:I20)</f>
         <v>547.77801666666664</v>
       </c>
-      <c r="J6" t="e">
+      <c r="J6">
         <f>AVERAGE(J18:J20)</f>
-        <v>#DIV/0!</v>
+        <v>6720.8522359999997</v>
       </c>
       <c r="K6" t="e">
         <f>AVERAGE(K18:K20)</f>
@@ -4914,13 +5195,9 @@
         <f>AVERAGE(AY20:AY24)</f>
         <v>1225.6000000000001</v>
       </c>
-      <c r="BB6" t="e">
+      <c r="BB6">
         <f>AVERAGE(BB18:BB20)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="BC6" t="e">
-        <f>AVERAGE(BC18:BC20)</f>
-        <v>#DIV/0!</v>
+        <v>318.88812833333333</v>
       </c>
       <c r="BD6">
         <v>2</v>
@@ -4979,9 +5256,9 @@
         <f>AVERAGE(I21:I23)</f>
         <v>283.11835533333334</v>
       </c>
-      <c r="J7" t="e">
+      <c r="J7">
         <f>AVERAGE(J21:J23)</f>
-        <v>#DIV/0!</v>
+        <v>3522.5893853333332</v>
       </c>
       <c r="K7" t="e">
         <f>AVERAGE(K21:K23)</f>
@@ -5069,13 +5346,9 @@
         <f>AVERAGE(AZ25:AZ29)</f>
         <v>26946.7</v>
       </c>
-      <c r="BB7" t="e">
+      <c r="BB7">
         <f>AVERAGE(BB21:BB23)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="BC7" t="e">
-        <f>AVERAGE(BC21:BC23)</f>
-        <v>#DIV/0!</v>
+        <v>200.49718966666669</v>
       </c>
       <c r="BD7">
         <v>4</v>
@@ -5137,9 +5410,9 @@
         <f>AVERAGE(I24:I26)</f>
         <v>148.15255566666667</v>
       </c>
-      <c r="J8" t="e">
+      <c r="J8">
         <f>AVERAGE(J24:J26)</f>
-        <v>#DIV/0!</v>
+        <v>1851.3246766666668</v>
       </c>
       <c r="K8" t="e">
         <f>AVERAGE(K24:K26)</f>
@@ -5234,13 +5507,9 @@
         <f>AVERAGE(AZ30:AZ34)</f>
         <v>11218.55</v>
       </c>
-      <c r="BB8" t="e">
+      <c r="BB8">
         <f>AVERAGE(BB24:BB26)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="BC8" t="e">
-        <f>AVERAGE(BC24:BC26)</f>
-        <v>#DIV/0!</v>
+        <v>134.27430966666665</v>
       </c>
       <c r="BD8">
         <v>8</v>
@@ -5302,9 +5571,9 @@
         <f>AVERAGE(I27:I29)</f>
         <v>81.215220666666653</v>
       </c>
-      <c r="J9" t="e">
+      <c r="J9">
         <f>AVERAGE(J27:J29)</f>
-        <v>#DIV/0!</v>
+        <v>1018.0796876666667</v>
       </c>
       <c r="K9" t="e">
         <f>AVERAGE(K27:K29)</f>
@@ -5407,13 +5676,13 @@
         <f>AVERAGE(AZ35:AZ39)</f>
         <v>7944.1559999999999</v>
       </c>
-      <c r="BB9" t="e">
+      <c r="BB9">
         <f>AVERAGE(BB27:BB29)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="BC9" t="e">
+        <v>99.84311133333334</v>
+      </c>
+      <c r="BC9">
         <f>AVERAGE(BC27:BC29)</f>
-        <v>#DIV/0!</v>
+        <v>2327.8390209999998</v>
       </c>
       <c r="BD9">
         <v>16</v>
@@ -5478,9 +5747,9 @@
         <f>AVERAGE(I30:I32)</f>
         <v>53.875178000000005</v>
       </c>
-      <c r="J10" t="e">
+      <c r="J10">
         <f>AVERAGE(J30:J32)</f>
-        <v>#DIV/0!</v>
+        <v>877.48516266666672</v>
       </c>
       <c r="K10" t="e">
         <f>AVERAGE(K30:K32)</f>
@@ -5587,13 +5856,13 @@
         <f>AVERAGE(AZ40:AZ44)</f>
         <v>6511.4820000000009</v>
       </c>
-      <c r="BB10" t="e">
+      <c r="BB10">
         <f>AVERAGE(BB30:BB32)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="BC10" t="e">
+        <v>84.121494666666663</v>
+      </c>
+      <c r="BC10">
         <f>AVERAGE(BC30:BC32)</f>
-        <v>#DIV/0!</v>
+        <v>1716.615575</v>
       </c>
       <c r="BD10">
         <v>32</v>
@@ -5666,9 +5935,9 @@
         <f>AVERAGE(I33:I35)</f>
         <v>42.362321000000001</v>
       </c>
-      <c r="J11" t="e">
+      <c r="J11">
         <f>AVERAGE(J33:J35)</f>
-        <v>#DIV/0!</v>
+        <v>804.29315733333317</v>
       </c>
       <c r="K11" t="e">
         <f>AVERAGE(K33:K35)</f>
@@ -5721,7 +5990,7 @@
       </c>
       <c r="AC11">
         <f>AVERAGE(AC45:AC49)</f>
-        <v>4201.97</v>
+        <v>2827.0160000000005</v>
       </c>
       <c r="AF11">
         <f t="shared" si="1"/>
@@ -5733,7 +6002,7 @@
       </c>
       <c r="AH11">
         <f>(AC$8*$Z$8)/(AC11*$Z11)</f>
-        <v>0.69113415850184556</v>
+        <v>1.0272757564866981</v>
       </c>
       <c r="AL11">
         <v>64</v>
@@ -5779,13 +6048,13 @@
         <f>AVERAGE(AZ45:AZ49)</f>
         <v>3370.9660000000003</v>
       </c>
-      <c r="BB11" t="e">
+      <c r="BB11">
         <f>AVERAGE(BB33:BB35)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="BC11" t="e">
+        <v>88.651036666666684</v>
+      </c>
+      <c r="BC11">
         <f>AVERAGE(BC33:BC35)</f>
-        <v>#DIV/0!</v>
+        <v>1879.305053</v>
       </c>
       <c r="BD11">
         <v>64</v>
@@ -5835,7 +6104,7 @@
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -5850,7 +6119,7 @@
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="R12" s="1"/>
       <c r="BD12">
@@ -5880,6 +6149,9 @@
       <c r="I15">
         <v>1079.593286</v>
       </c>
+      <c r="J15">
+        <v>13494.399758</v>
+      </c>
       <c r="N15">
         <v>1</v>
       </c>
@@ -5930,6 +6202,9 @@
       </c>
       <c r="BA15">
         <v>1</v>
+      </c>
+      <c r="BB15">
+        <v>551.73830799999996</v>
       </c>
       <c r="BD15">
         <v>1</v>
@@ -5966,6 +6241,9 @@
       <c r="I16">
         <v>1077.4435309999999</v>
       </c>
+      <c r="J16">
+        <v>13015.933239</v>
+      </c>
       <c r="N16">
         <v>1</v>
       </c>
@@ -6013,6 +6291,9 @@
       </c>
       <c r="BA16">
         <v>1</v>
+      </c>
+      <c r="BB16">
+        <v>549.54735500000004</v>
       </c>
       <c r="BD16">
         <v>1</v>
@@ -6043,6 +6324,9 @@
       <c r="I17">
         <v>1079.7990050000001</v>
       </c>
+      <c r="J17">
+        <v>12812.241698</v>
+      </c>
       <c r="N17">
         <v>1</v>
       </c>
@@ -6078,6 +6362,9 @@
       </c>
       <c r="BA17">
         <v>1</v>
+      </c>
+      <c r="BB17">
+        <v>554.23846300000002</v>
       </c>
       <c r="BD17">
         <v>1</v>
@@ -6108,6 +6395,9 @@
       <c r="I18">
         <v>549.52244399999995</v>
       </c>
+      <c r="J18">
+        <v>6809.384094</v>
+      </c>
       <c r="N18">
         <v>2</v>
       </c>
@@ -6143,6 +6433,9 @@
       </c>
       <c r="BA18">
         <v>2</v>
+      </c>
+      <c r="BB18">
+        <v>312.27436999999998</v>
       </c>
       <c r="BD18">
         <v>1</v>
@@ -6173,6 +6466,9 @@
       <c r="I19">
         <v>548.068759</v>
       </c>
+      <c r="J19">
+        <v>6707.3225060000004</v>
+      </c>
       <c r="N19">
         <v>2</v>
       </c>
@@ -6205,6 +6501,9 @@
       </c>
       <c r="BA19">
         <v>2</v>
+      </c>
+      <c r="BB19">
+        <v>324.36091399999998</v>
       </c>
       <c r="BD19">
         <v>1</v>
@@ -6235,6 +6534,9 @@
       <c r="I20">
         <v>545.74284699999998</v>
       </c>
+      <c r="J20">
+        <v>6645.8501079999996</v>
+      </c>
       <c r="N20">
         <v>2</v>
       </c>
@@ -6289,6 +6591,9 @@
       </c>
       <c r="BA20">
         <v>2</v>
+      </c>
+      <c r="BB20">
+        <v>320.02910100000003</v>
       </c>
       <c r="BD20">
         <v>2</v>
@@ -6325,6 +6630,9 @@
       <c r="I21">
         <v>282.240116</v>
       </c>
+      <c r="J21">
+        <v>3493.2108069999999</v>
+      </c>
       <c r="N21">
         <v>4</v>
       </c>
@@ -6383,6 +6691,9 @@
       </c>
       <c r="BA21">
         <v>4</v>
+      </c>
+      <c r="BB21">
+        <v>201.885918</v>
       </c>
       <c r="BD21">
         <v>2</v>
@@ -6419,6 +6730,9 @@
       <c r="I22">
         <v>282.75658600000003</v>
       </c>
+      <c r="J22">
+        <v>3533.1350459999999</v>
+      </c>
       <c r="N22">
         <v>4</v>
       </c>
@@ -6477,6 +6791,9 @@
       </c>
       <c r="BA22">
         <v>4</v>
+      </c>
+      <c r="BB22">
+        <v>198.84424100000001</v>
       </c>
       <c r="BD22">
         <v>2</v>
@@ -6513,6 +6830,9 @@
       <c r="I23">
         <v>284.35836399999999</v>
       </c>
+      <c r="J23">
+        <v>3541.4223029999998</v>
+      </c>
       <c r="N23">
         <v>4</v>
       </c>
@@ -6562,6 +6882,9 @@
       </c>
       <c r="BA23">
         <v>4</v>
+      </c>
+      <c r="BB23">
+        <v>200.76141000000001</v>
       </c>
       <c r="BD23">
         <v>2</v>
@@ -6598,6 +6921,9 @@
       <c r="I24">
         <v>149.199085</v>
       </c>
+      <c r="J24">
+        <v>1850.1276539999999</v>
+      </c>
       <c r="N24">
         <v>8</v>
       </c>
@@ -6642,6 +6968,9 @@
       </c>
       <c r="BA24">
         <v>8</v>
+      </c>
+      <c r="BB24">
+        <v>136.488382</v>
       </c>
       <c r="BD24">
         <v>2</v>
@@ -6681,6 +7010,9 @@
       <c r="I25">
         <v>146.720304</v>
       </c>
+      <c r="J25">
+        <v>1857.499595</v>
+      </c>
       <c r="N25">
         <v>8</v>
       </c>
@@ -6742,6 +7074,9 @@
       </c>
       <c r="BA25">
         <v>8</v>
+      </c>
+      <c r="BB25">
+        <v>132.94589999999999</v>
       </c>
       <c r="BD25">
         <v>4</v>
@@ -6781,6 +7116,9 @@
       <c r="I26">
         <v>148.53827799999999</v>
       </c>
+      <c r="J26">
+        <v>1846.346781</v>
+      </c>
       <c r="N26">
         <v>8</v>
       </c>
@@ -6842,6 +7180,9 @@
       </c>
       <c r="BA26">
         <v>8</v>
+      </c>
+      <c r="BB26">
+        <v>133.38864699999999</v>
       </c>
       <c r="BD26">
         <v>4</v>
@@ -6881,6 +7222,9 @@
       <c r="I27">
         <v>81.227279999999993</v>
       </c>
+      <c r="J27">
+        <v>1029.648694</v>
+      </c>
       <c r="N27">
         <v>16</v>
       </c>
@@ -6943,6 +7287,12 @@
       </c>
       <c r="BA27">
         <v>16</v>
+      </c>
+      <c r="BB27">
+        <v>98.152606000000006</v>
+      </c>
+      <c r="BC27">
+        <v>2327.8390209999998</v>
       </c>
       <c r="BD27">
         <v>4</v>
@@ -6982,6 +7332,9 @@
       <c r="I28">
         <v>81.025633999999997</v>
       </c>
+      <c r="J28">
+        <v>1008.453992</v>
+      </c>
       <c r="N28">
         <v>16</v>
       </c>
@@ -7041,6 +7394,9 @@
       </c>
       <c r="BA28">
         <v>16</v>
+      </c>
+      <c r="BB28">
+        <v>99.586156000000003</v>
       </c>
       <c r="BD28">
         <v>4</v>
@@ -7077,6 +7433,9 @@
       <c r="I29">
         <v>81.392747999999997</v>
       </c>
+      <c r="J29">
+        <v>1016.136377</v>
+      </c>
       <c r="N29">
         <v>16</v>
       </c>
@@ -7120,6 +7479,9 @@
       </c>
       <c r="BA29">
         <v>16</v>
+      </c>
+      <c r="BB29">
+        <v>101.790572</v>
       </c>
       <c r="BD29">
         <v>4</v>
@@ -7162,6 +7524,9 @@
       <c r="I30">
         <v>54.579166999999998</v>
       </c>
+      <c r="J30">
+        <v>853.04366100000004</v>
+      </c>
       <c r="N30">
         <v>32</v>
       </c>
@@ -7230,6 +7595,12 @@
       </c>
       <c r="BA30">
         <v>32</v>
+      </c>
+      <c r="BB30">
+        <v>85.10042</v>
+      </c>
+      <c r="BC30">
+        <v>1716.615575</v>
       </c>
       <c r="BD30">
         <v>8</v>
@@ -7275,6 +7646,9 @@
       <c r="I31">
         <v>52.603828</v>
       </c>
+      <c r="J31">
+        <v>912.73653200000001</v>
+      </c>
       <c r="N31">
         <v>32</v>
       </c>
@@ -7332,6 +7706,9 @@
       </c>
       <c r="BA31">
         <v>32</v>
+      </c>
+      <c r="BB31">
+        <v>84.232462999999996</v>
       </c>
       <c r="BD31">
         <v>8</v>
@@ -7377,6 +7754,9 @@
       <c r="I32">
         <v>54.442538999999996</v>
       </c>
+      <c r="J32">
+        <v>866.67529500000001</v>
+      </c>
       <c r="N32">
         <v>32</v>
       </c>
@@ -7431,6 +7811,9 @@
       </c>
       <c r="BA32">
         <v>32</v>
+      </c>
+      <c r="BB32">
+        <v>83.031600999999995</v>
       </c>
       <c r="BD32">
         <v>8</v>
@@ -7473,6 +7856,9 @@
       <c r="I33">
         <v>42.766230999999998</v>
       </c>
+      <c r="J33">
+        <v>794.46825999999999</v>
+      </c>
       <c r="N33">
         <v>64</v>
       </c>
@@ -7535,6 +7921,12 @@
       </c>
       <c r="BA33">
         <v>64</v>
+      </c>
+      <c r="BB33">
+        <v>82.366442000000006</v>
+      </c>
+      <c r="BC33">
+        <v>1879.305053</v>
       </c>
       <c r="BD33">
         <v>8</v>
@@ -7577,6 +7969,9 @@
       <c r="I34">
         <v>41.716487000000001</v>
       </c>
+      <c r="J34">
+        <v>818.44250299999999</v>
+      </c>
       <c r="N34">
         <v>64</v>
       </c>
@@ -7624,6 +8019,9 @@
       </c>
       <c r="BA34">
         <v>64</v>
+      </c>
+      <c r="BB34">
+        <v>91.394540000000006</v>
       </c>
       <c r="BD34">
         <v>8</v>
@@ -7666,6 +8064,9 @@
       <c r="I35">
         <v>42.604244999999999</v>
       </c>
+      <c r="J35">
+        <v>799.96870899999999</v>
+      </c>
       <c r="N35">
         <v>64</v>
       </c>
@@ -7737,6 +8138,9 @@
       </c>
       <c r="BA35">
         <v>64</v>
+      </c>
+      <c r="BB35">
+        <v>92.192127999999997</v>
       </c>
       <c r="BD35">
         <v>16</v>
@@ -8750,6 +9154,9 @@
       <c r="AB46">
         <v>84.731099999999998</v>
       </c>
+      <c r="AC46">
+        <v>2468.12</v>
+      </c>
       <c r="AL46">
         <v>64</v>
       </c>
@@ -8855,6 +9262,9 @@
       <c r="AB47">
         <v>102.068</v>
       </c>
+      <c r="AC47">
+        <v>2525.42</v>
+      </c>
       <c r="AL47">
         <v>64</v>
       </c>
@@ -8960,6 +9370,9 @@
       <c r="AB48">
         <v>104.024</v>
       </c>
+      <c r="AC48">
+        <v>2469.37</v>
+      </c>
       <c r="AL48">
         <v>64</v>
       </c>
@@ -9062,6 +9475,9 @@
       <c r="AB49">
         <v>112.36199999999999</v>
       </c>
+      <c r="AC49">
+        <v>2470.1999999999998</v>
+      </c>
       <c r="AL49">
         <v>64</v>
       </c>
@@ -9676,7 +10092,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Removed XMT R-MAT and Triangle results for now. Change Cohen's affiliation.
git-svn-id: svn+ssh://software-srn.sandia.gov/svn/mapreduce/trunk@629 3fc257bb-8550-0410-81b3-a5c103da83f7
</commit_message>
<xml_diff>
--- a/paper/results.xlsx
+++ b/paper/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6500" yWindow="520" windowWidth="21600" windowHeight="13380" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="6500" yWindow="520" windowWidth="24540" windowHeight="17360" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="CC" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <definedName name="jj_1" localSheetId="6">Sheet1!$N$41:$O$64</definedName>
     <definedName name="jjj" localSheetId="6">Sheet1!$BD$15:$BE$84</definedName>
   </definedNames>
-  <calcPr calcId="130406" concurrentCalc="0"/>
+  <calcPr calcId="130407" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
@@ -714,11 +714,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="591457496"/>
-        <c:axId val="591451400"/>
+        <c:axId val="754933688"/>
+        <c:axId val="754927592"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="591457496"/>
+        <c:axId val="754933688"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -745,12 +745,12 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="591451400"/>
+        <c:crossAx val="754927592"/>
         <c:crossesAt val="0.1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="591451400"/>
+        <c:axId val="754927592"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -778,7 +778,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="591457496"/>
+        <c:crossAx val="754933688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1222,11 +1222,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="591648584"/>
-        <c:axId val="591654552"/>
+        <c:axId val="788695640"/>
+        <c:axId val="788701608"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="591648584"/>
+        <c:axId val="788695640"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1251,12 +1251,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="591654552"/>
+        <c:crossAx val="788701608"/>
         <c:crossesAt val="0.0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="591654552"/>
+        <c:axId val="788701608"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1283,7 +1283,7 @@
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="591648584"/>
+        <c:crossAx val="788695640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1730,11 +1730,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="591711784"/>
-        <c:axId val="591717784"/>
+        <c:axId val="788759000"/>
+        <c:axId val="788765000"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="591711784"/>
+        <c:axId val="788759000"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1760,12 +1760,12 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="591717784"/>
+        <c:crossAx val="788765000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="591717784"/>
+        <c:axId val="788765000"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1792,7 +1792,7 @@
         <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="591711784"/>
+        <c:crossAx val="788759000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1886,15 +1886,15 @@
           </c:yVal>
         </c:ser>
         <c:ser>
-          <c:idx val="4"/>
+          <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$J$4</c:f>
+              <c:f>Sheet1!$C$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>R-MAT 24 (MTGL/XMT)</c:v>
+                  <c:v>R-MAT 24 (MR-MPI)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1931,45 +1931,45 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$J$5:$J$11</c:f>
+              <c:f>Sheet1!$C$5:$C$11</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>13107.52489833333</c:v>
+                  <c:v>3683.12</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6720.852236</c:v>
+                  <c:v>1568.102</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3522.589385333333</c:v>
+                  <c:v>501.7906</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1851.324676666667</c:v>
+                  <c:v>171.2498</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1018.079687666667</c:v>
+                  <c:v>133.8856</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>877.4851626666667</c:v>
+                  <c:v>75.92102</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>804.2931573333331</c:v>
+                  <c:v>14.6574</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
         </c:ser>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="0"/>
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$4</c:f>
+              <c:f>Sheet1!$B$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>R-MAT 24 (MR-MPI)</c:v>
+                  <c:v>R-MAT 20 (MR-MPI)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2006,156 +2006,6 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$5:$C$11</c:f>
-              <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>3683.12</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1568.102</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>501.7906</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>171.2498</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>133.8856</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>75.92102</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>14.6574</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$I$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>R-MAT 20 (MTGL/XMT)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$A$5:$A$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>64.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$I$5:$I$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>1078.945274</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>547.7780166666666</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>283.1183553333333</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>148.1525556666667</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>81.21522066666665</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>53.875178</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>42.362321</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-        </c:ser>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$B$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>R-MAT 20 (MR-MPI)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$A$5:$A$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>64.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
               <c:f>Sheet1!$B$5:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
@@ -2185,11 +2035,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="591771864"/>
-        <c:axId val="591777928"/>
+        <c:axId val="788817960"/>
+        <c:axId val="788824024"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="591771864"/>
+        <c:axId val="788817960"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2216,12 +2066,12 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="591777928"/>
+        <c:crossAx val="788824024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="591777928"/>
+        <c:axId val="788824024"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2249,7 +2099,7 @@
         <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="591771864"/>
+        <c:crossAx val="788817960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2490,11 +2340,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="591818168"/>
-        <c:axId val="591828264"/>
+        <c:axId val="788865272"/>
+        <c:axId val="788875400"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="591818168"/>
+        <c:axId val="788865272"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2521,12 +2371,12 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="591828264"/>
+        <c:crossAx val="788875400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="591828264"/>
+        <c:axId val="788875400"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2554,7 +2404,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="591818168"/>
+        <c:crossAx val="788865272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2576,7 +2426,17 @@
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.106337262216009"/>
+          <c:y val="0.0305263145243964"/>
+          <c:w val="0.67446486337991"/>
+          <c:h val="0.859849706832349"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:ser>
@@ -2649,15 +2509,15 @@
           </c:yVal>
         </c:ser>
         <c:ser>
-          <c:idx val="3"/>
+          <c:idx val="0"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$BC$4</c:f>
+              <c:f>Sheet1!$AY$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>R-MAT 24 (MTGL/XMT)</c:v>
+                  <c:v>R-MAT 20 (MR-MPI)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2694,69 +2554,6 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$BC$5:$BC$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="4">
-                  <c:v>2327.839021</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1716.615575</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1879.305053</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-        </c:ser>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$AY$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>R-MAT 20 (MR-MPI)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$AX$5:$AX$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>64.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
               <c:f>Sheet1!$AY$5:$AY$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -2786,86 +2583,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$BB$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>R-MAT 20 (MTGL/XMT)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$AX$5:$AX$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>64.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$BB$5:$BB$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>551.8413753333334</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>318.8881283333333</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>200.4971896666667</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>134.2743096666667</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>99.84311133333334</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>84.12149466666666</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>88.65103666666668</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-        </c:ser>
-        <c:axId val="591866936"/>
-        <c:axId val="591885368"/>
+        <c:axId val="788914392"/>
+        <c:axId val="788932824"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="591866936"/>
+        <c:axId val="788914392"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2892,12 +2614,12 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="591885368"/>
+        <c:crossAx val="788932824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="591885368"/>
+        <c:axId val="788932824"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2925,7 +2647,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="591866936"/>
+        <c:crossAx val="788914392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2961,7 +2683,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -3470,11 +3191,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="592007272"/>
-        <c:axId val="592013048"/>
+        <c:axId val="789055176"/>
+        <c:axId val="789060952"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="592007272"/>
+        <c:axId val="789055176"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -3496,18 +3217,17 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="592013048"/>
+        <c:crossAx val="789060952"/>
         <c:crossesAt val="0.001"/>
         <c:crossBetween val="midCat"/>
         <c:minorUnit val="10.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="592013048"/>
+        <c:axId val="789060952"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -3530,19 +3250,17 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="0.E+00" sourceLinked="0"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="592007272"/>
+        <c:crossAx val="789055176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -3576,7 +3294,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -4005,11 +3722,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="592047496"/>
-        <c:axId val="592053496"/>
+        <c:axId val="789095832"/>
+        <c:axId val="789101832"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="592047496"/>
+        <c:axId val="789095832"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -4031,17 +3748,16 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="592053496"/>
+        <c:crossAx val="789101832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="592053496"/>
+        <c:axId val="789101832"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -4064,19 +3780,17 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="592047496"/>
+        <c:crossAx val="789095832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -4090,7 +3804,7 @@
 
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr published="0"/>
+  <sheetPr/>
   <sheetViews>
     <sheetView zoomScale="97" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
@@ -4102,7 +3816,7 @@
 
 <file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr published="0"/>
+  <sheetPr/>
   <sheetViews>
     <sheetView zoomScale="97" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
@@ -4114,7 +3828,7 @@
 
 <file path=xl/chartsheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr published="0"/>
+  <sheetPr/>
   <sheetViews>
     <sheetView zoomScale="116" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
@@ -4126,7 +3840,19 @@
 
 <file path=xl/chartsheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr published="0"/>
+  <sheetPr/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="116" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
   <sheetViews>
     <sheetView zoomScale="116" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
@@ -4136,21 +3862,9 @@
 </chartsheet>
 </file>
 
-<file path=xl/chartsheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr published="0"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="116" workbookViewId="0" zoomToFit="1"/>
-  </sheetViews>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <drawing r:id="rId1"/>
-</chartsheet>
-</file>
-
 <file path=xl/chartsheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr published="0"/>
+  <sheetPr/>
   <sheetViews>
     <sheetView zoomScale="116" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
@@ -4388,11 +4102,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="jj_1" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="jjj" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="jjj" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="jj_1" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4715,7 +4429,6 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:BO85"/>
   <sheetViews>
     <sheetView view="pageLayout" topLeftCell="X4" workbookViewId="0">

</xml_diff>

<commit_message>
Updated with RMAT-20 results; still waiting for RMAT-28 runs.
git-svn-id: svn+ssh://software-srn.sandia.gov/svn/mapreduce/trunk@648 3fc257bb-8550-0410-81b3-a5c103da83f7
</commit_message>
<xml_diff>
--- a/paper/results.xlsx
+++ b/paper/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6500" yWindow="520" windowWidth="24540" windowHeight="17360" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="-180" yWindow="0" windowWidth="24540" windowHeight="17360" tabRatio="500" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="CC" sheetId="2" r:id="rId1"/>
@@ -14,6 +14,7 @@
     <sheet name="Luby" sheetId="6" r:id="rId5"/>
     <sheet name="Tri" sheetId="7" r:id="rId6"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId7"/>
+    <sheet name="Sheet2" sheetId="8" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="jj" localSheetId="6">Sheet1!#REF!</definedName>
@@ -51,7 +52,79 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="83">
+  <si>
+    <t>reduce x</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>MPI_Allreduce</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Percentage</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Detail MR-MPI</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Step 5</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Add y to x</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Convert x</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Total Time for 6 iterations</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Time per iteration</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Detail MR-MPI Step 2</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>RMAT-20</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Copy x to y</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Add A to y</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Convert y</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reduce y</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Aggregate y</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Convert y</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reduce y</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
   <si>
     <t>R-MAT 28 (MTGL/XMT)</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -280,11 +353,49 @@
     <t>R-MAT 24 (MTGL/XMT)</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
+  <si>
+    <t>PageRank Detail</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>RMAT-20</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Step 1</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Step 2</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Step 3</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Step 4</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Step 5</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>MR-MPI</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
   <fonts count="5">
     <font>
       <sz val="10"/>
@@ -328,13 +439,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -714,11 +826,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="754933688"/>
-        <c:axId val="754927592"/>
+        <c:axId val="824048888"/>
+        <c:axId val="824045512"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="754933688"/>
+        <c:axId val="824048888"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -745,12 +857,12 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="754927592"/>
+        <c:crossAx val="824045512"/>
         <c:crossesAt val="0.1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="754927592"/>
+        <c:axId val="824045512"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -778,7 +890,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="754933688"/>
+        <c:crossAx val="824048888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1222,11 +1334,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="788695640"/>
-        <c:axId val="788701608"/>
+        <c:axId val="863507336"/>
+        <c:axId val="863514008"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="788695640"/>
+        <c:axId val="863507336"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1251,12 +1363,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="788701608"/>
+        <c:crossAx val="863514008"/>
         <c:crossesAt val="0.0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="788701608"/>
+        <c:axId val="863514008"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1283,7 +1395,7 @@
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="788695640"/>
+        <c:crossAx val="863507336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1730,11 +1842,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="788759000"/>
-        <c:axId val="788765000"/>
+        <c:axId val="863570936"/>
+        <c:axId val="863578280"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="788759000"/>
+        <c:axId val="863570936"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1760,12 +1872,12 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="788765000"/>
+        <c:crossAx val="863578280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="788765000"/>
+        <c:axId val="863578280"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1792,7 +1904,7 @@
         <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="788759000"/>
+        <c:crossAx val="863570936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2035,11 +2147,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="788817960"/>
-        <c:axId val="788824024"/>
+        <c:axId val="863615864"/>
+        <c:axId val="863627336"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="788817960"/>
+        <c:axId val="863615864"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2066,12 +2178,12 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="788824024"/>
+        <c:crossAx val="863627336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="788824024"/>
+        <c:axId val="863627336"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2099,7 +2211,7 @@
         <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="788817960"/>
+        <c:crossAx val="863615864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2340,11 +2452,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="788865272"/>
-        <c:axId val="788875400"/>
+        <c:axId val="863668312"/>
+        <c:axId val="863679784"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="788865272"/>
+        <c:axId val="863668312"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2366,17 +2478,16 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="788875400"/>
+        <c:crossAx val="863679784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="788875400"/>
+        <c:axId val="863679784"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2399,19 +2510,17 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="788865272"/>
+        <c:crossAx val="863668312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -2583,11 +2692,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="788914392"/>
-        <c:axId val="788932824"/>
+        <c:axId val="863715512"/>
+        <c:axId val="863727912"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="788914392"/>
+        <c:axId val="863715512"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2609,17 +2718,16 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="788932824"/>
+        <c:crossAx val="863727912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="788932824"/>
+        <c:axId val="863727912"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2642,19 +2750,17 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="788914392"/>
+        <c:crossAx val="863715512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -2683,6 +2789,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -3191,11 +3298,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="789055176"/>
-        <c:axId val="789060952"/>
+        <c:axId val="863849304"/>
+        <c:axId val="863856424"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="789055176"/>
+        <c:axId val="863849304"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -3217,17 +3324,18 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="789060952"/>
+        <c:crossAx val="863856424"/>
         <c:crossesAt val="0.001"/>
         <c:crossBetween val="midCat"/>
         <c:minorUnit val="10.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="789060952"/>
+        <c:axId val="863856424"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -3250,17 +3358,19 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="0.E+00" sourceLinked="0"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="789055176"/>
+        <c:crossAx val="863849304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -3722,11 +3832,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="789095832"/>
-        <c:axId val="789101832"/>
+        <c:axId val="863889960"/>
+        <c:axId val="863897304"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="789095832"/>
+        <c:axId val="863889960"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -3752,12 +3862,12 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="789101832"/>
+        <c:crossAx val="863897304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="789101832"/>
+        <c:axId val="863897304"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -3784,7 +3894,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="789095832"/>
+        <c:crossAx val="863889960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3842,7 +3952,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="116" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="116" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -4102,11 +4212,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="jjj" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="jj_1" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="jj_1" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="jjj" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4431,7 +4541,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:BO85"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="X4" workbookViewId="0">
+    <sheetView view="pageLayout" topLeftCell="K1" workbookViewId="0">
       <selection activeCell="AC45" sqref="AC45:AC49"/>
     </sheetView>
   </sheetViews>
@@ -4446,235 +4556,235 @@
   <sheetData>
     <row r="1" spans="1:67">
       <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="N1" t="s">
+        <v>27</v>
+      </c>
+      <c r="T1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>37</v>
+      </c>
+      <c r="BD1" t="s">
         <v>21</v>
-      </c>
-      <c r="N1" t="s">
-        <v>9</v>
-      </c>
-      <c r="T1" t="s">
-        <v>20</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>17</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>18</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>19</v>
-      </c>
-      <c r="BD1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:67">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="N2" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="P2" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="BD2" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:67">
       <c r="C3" t="s">
-        <v>49</v>
+        <v>67</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="G3" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="I3" t="s">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="O3" t="s">
+        <v>62</v>
+      </c>
+      <c r="S3" t="s">
+        <v>32</v>
+      </c>
+      <c r="U3" t="s">
+        <v>33</v>
+      </c>
+      <c r="V3" t="s">
+        <v>34</v>
+      </c>
+      <c r="W3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AR3" t="s">
+        <v>43</v>
+      </c>
+      <c r="AU3" t="s">
         <v>44</v>
       </c>
-      <c r="S3" t="s">
-        <v>14</v>
-      </c>
-      <c r="U3" t="s">
-        <v>15</v>
-      </c>
-      <c r="V3" t="s">
-        <v>16</v>
-      </c>
-      <c r="W3" t="s">
-        <v>16</v>
-      </c>
-      <c r="AM3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AR3" t="s">
-        <v>25</v>
-      </c>
-      <c r="AU3" t="s">
-        <v>26</v>
-      </c>
       <c r="BB3" t="s">
-        <v>54</v>
+        <v>72</v>
       </c>
       <c r="BJ3" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="BK3" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="BL3" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:67">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G4" t="s">
+        <v>49</v>
+      </c>
+      <c r="I4" t="s">
+        <v>73</v>
+      </c>
+      <c r="J4" t="s">
+        <v>74</v>
+      </c>
+      <c r="K4" t="s">
+        <v>18</v>
+      </c>
+      <c r="N4" t="s">
+        <v>25</v>
+      </c>
+      <c r="O4" t="s">
+        <v>63</v>
+      </c>
+      <c r="P4" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>20</v>
+      </c>
+      <c r="R4" t="s">
+        <v>26</v>
+      </c>
+      <c r="S4" t="s">
+        <v>48</v>
+      </c>
+      <c r="U4" t="s">
         <v>51</v>
       </c>
-      <c r="C4" t="s">
+      <c r="V4" t="s">
         <v>52</v>
       </c>
-      <c r="D4" t="s">
+      <c r="W4" t="s">
         <v>53</v>
       </c>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="Z4" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>20</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>26</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>25</v>
+      </c>
+      <c r="AM4" t="s">
+        <v>55</v>
+      </c>
+      <c r="AN4" t="s">
+        <v>57</v>
+      </c>
+      <c r="AO4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AP4" t="s">
+        <v>26</v>
+      </c>
+      <c r="AR4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AS4" t="s">
+        <v>22</v>
+      </c>
+      <c r="AT4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AU4" t="s">
+        <v>59</v>
+      </c>
+      <c r="AV4" t="s">
+        <v>60</v>
+      </c>
+      <c r="AW4" t="s">
+        <v>61</v>
+      </c>
+      <c r="AX4" t="s">
+        <v>25</v>
+      </c>
+      <c r="AY4" t="s">
+        <v>55</v>
+      </c>
+      <c r="AZ4" t="s">
+        <v>19</v>
+      </c>
+      <c r="BB4" t="s">
+        <v>73</v>
+      </c>
+      <c r="BC4" t="s">
+        <v>74</v>
+      </c>
+      <c r="BD4" t="s">
+        <v>25</v>
+      </c>
+      <c r="BE4" t="s">
+        <v>45</v>
+      </c>
+      <c r="BF4" t="s">
+        <v>46</v>
+      </c>
+      <c r="BG4" t="s">
+        <v>47</v>
+      </c>
+      <c r="BH4" t="s">
+        <v>26</v>
+      </c>
+      <c r="BJ4" t="s">
+        <v>50</v>
+      </c>
+      <c r="BK4" t="s">
         <v>48</v>
       </c>
-      <c r="G4" t="s">
-        <v>31</v>
-      </c>
-      <c r="I4" t="s">
-        <v>55</v>
-      </c>
-      <c r="J4" t="s">
-        <v>56</v>
-      </c>
-      <c r="K4" t="s">
-        <v>0</v>
-      </c>
-      <c r="N4" t="s">
-        <v>7</v>
-      </c>
-      <c r="O4" t="s">
-        <v>45</v>
-      </c>
-      <c r="P4" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>2</v>
-      </c>
-      <c r="R4" t="s">
-        <v>8</v>
-      </c>
-      <c r="S4" t="s">
-        <v>30</v>
-      </c>
-      <c r="U4" t="s">
-        <v>33</v>
-      </c>
-      <c r="V4" t="s">
-        <v>34</v>
-      </c>
-      <c r="W4" t="s">
-        <v>35</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>7</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>46</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>47</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>2</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>8</v>
-      </c>
-      <c r="AL4" t="s">
-        <v>7</v>
-      </c>
-      <c r="AM4" t="s">
-        <v>37</v>
-      </c>
-      <c r="AN4" t="s">
-        <v>39</v>
-      </c>
-      <c r="AO4" t="s">
-        <v>40</v>
-      </c>
-      <c r="AP4" t="s">
-        <v>8</v>
-      </c>
-      <c r="AR4" t="s">
-        <v>36</v>
-      </c>
-      <c r="AS4" t="s">
-        <v>4</v>
-      </c>
-      <c r="AT4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AU4" t="s">
-        <v>41</v>
-      </c>
-      <c r="AV4" t="s">
-        <v>42</v>
-      </c>
-      <c r="AW4" t="s">
-        <v>43</v>
-      </c>
-      <c r="AX4" t="s">
-        <v>7</v>
-      </c>
-      <c r="AY4" t="s">
-        <v>37</v>
-      </c>
-      <c r="AZ4" t="s">
-        <v>1</v>
-      </c>
-      <c r="BB4" t="s">
-        <v>55</v>
-      </c>
-      <c r="BC4" t="s">
-        <v>56</v>
-      </c>
-      <c r="BD4" t="s">
-        <v>7</v>
-      </c>
-      <c r="BE4" t="s">
-        <v>27</v>
-      </c>
-      <c r="BF4" t="s">
-        <v>28</v>
-      </c>
-      <c r="BG4" t="s">
-        <v>29</v>
-      </c>
-      <c r="BH4" t="s">
-        <v>8</v>
-      </c>
-      <c r="BJ4" t="s">
-        <v>32</v>
-      </c>
-      <c r="BK4" t="s">
-        <v>30</v>
-      </c>
       <c r="BL4" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:67">
@@ -5817,7 +5927,7 @@
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -5832,7 +5942,7 @@
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="1" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="R12" s="1"/>
       <c r="BD12">
@@ -9815,4 +9925,867 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <dimension ref="A1:O72"/>
+  <sheetViews>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetData>
+    <row r="1" spans="1:15">
+      <c r="A1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4">
+        <f>AVERAGE(B20:B24)</f>
+        <v>0.12209159999999999</v>
+      </c>
+      <c r="C4">
+        <f>AVERAGE(C20:C24)</f>
+        <v>1.8215660000000002E-3</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4">
+        <v>1.5562099999999999E-3</v>
+      </c>
+      <c r="I4">
+        <f>H4/SUM($H$4:$H$10)*100</f>
+        <v>1.1230334322205473</v>
+      </c>
+      <c r="M4" t="s">
+        <v>5</v>
+      </c>
+      <c r="N4">
+        <v>4.6457999999999997E-4</v>
+      </c>
+      <c r="O4">
+        <f>N4/$B$16*100</f>
+        <v>2.2441382286356504</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5">
+        <f>AVERAGE(B26:B30)</f>
+        <v>0.82619520000000013</v>
+      </c>
+      <c r="C5">
+        <f>AVERAGE(C26:C30)</f>
+        <v>2.7317799999999996E-2</v>
+      </c>
+      <c r="G5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5">
+        <v>4.0733200000000001E-3</v>
+      </c>
+      <c r="I5">
+        <f>H5/SUM($H$4:$H$10)*100</f>
+        <v>2.9394969445849854</v>
+      </c>
+      <c r="M5" t="s">
+        <v>6</v>
+      </c>
+      <c r="N5">
+        <v>1.9678310000000001E-2</v>
+      </c>
+      <c r="O5">
+        <f>N5/$B$16*100</f>
+        <v>95.055421554830616</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6">
+        <f>AVERAGE(B32:B36)</f>
+        <v>9.2634680000000004E-3</v>
+      </c>
+      <c r="C6">
+        <f>AVERAGE(C32:C36)</f>
+        <v>9.2148839999999996E-4</v>
+      </c>
+      <c r="G6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6">
+        <v>3.2574150000000003E-2</v>
+      </c>
+      <c r="I6">
+        <f>H6/SUM($H$4:$H$10)*100</f>
+        <v>23.507019924153518</v>
+      </c>
+      <c r="M6" t="s">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>5.31E-4</v>
+      </c>
+      <c r="O6">
+        <f>N6/$B$16*100</f>
+        <v>2.5649778281577564</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7">
+        <f>AVERAGE(B38:B42)</f>
+        <v>7.9746239999999996E-3</v>
+      </c>
+      <c r="C7">
+        <f>AVERAGE(C38:C42)</f>
+        <v>8.4199900000000007E-4</v>
+      </c>
+      <c r="G7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7">
+        <v>1.070432E-2</v>
+      </c>
+      <c r="I7">
+        <f>H7/SUM($H$4:$H$10)*100</f>
+        <v>7.724734598278542</v>
+      </c>
+      <c r="M7" t="s">
+        <v>1</v>
+      </c>
+      <c r="N7" s="6">
+        <v>4.9336999999999999E-5</v>
+      </c>
+      <c r="O7">
+        <f>N7/$B$16*100</f>
+        <v>0.23832073654956537</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8">
+        <f>AVERAGE(B44:B48)</f>
+        <v>0.12421160000000001</v>
+      </c>
+      <c r="C8">
+        <f>AVERAGE(C44:C48)</f>
+        <v>8.8839539999999997E-4</v>
+      </c>
+      <c r="G8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8">
+        <v>3.4496720000000002E-2</v>
+      </c>
+      <c r="I8">
+        <f>H8/SUM($H$4:$H$10)*100</f>
+        <v>24.894435752212875</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="G9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9">
+        <v>5.296878E-2</v>
+      </c>
+      <c r="I9">
+        <f>H9/SUM($H$4:$H$10)*100</f>
+        <v>38.224732397256851</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10">
+        <v>2.1985099999999999E-3</v>
+      </c>
+      <c r="I10">
+        <f>H10/SUM($H$4:$H$10)*100</f>
+        <v>1.5865469512926889</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" t="s">
+        <v>76</v>
+      </c>
+      <c r="B11" t="s">
+        <v>82</v>
+      </c>
+      <c r="C11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" t="s">
+        <v>77</v>
+      </c>
+      <c r="B12">
+        <f>B4/6</f>
+        <v>2.0348599999999998E-2</v>
+      </c>
+      <c r="C12">
+        <f t="shared" ref="C12:C16" si="0">C4/6</f>
+        <v>3.0359433333333334E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" t="s">
+        <v>78</v>
+      </c>
+      <c r="B13">
+        <f t="shared" ref="B13:C16" si="1">B5/6</f>
+        <v>0.13769920000000002</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>4.5529666666666658E-3</v>
+      </c>
+      <c r="H13">
+        <v>1.09129E-2</v>
+      </c>
+      <c r="I13">
+        <f>AVERAGE(H13,H15,H17,H19,H21,H23,H25,H27,H29,H31,H33,H35,H37,H39,H41,H43,H45,H47,H49,H51,H53,H55,H57,H59,H61,H63,H65,H67,H69,H71)</f>
+        <v>1.070432E-2</v>
+      </c>
+      <c r="N13" s="6">
+        <v>4.8875799999999997E-5</v>
+      </c>
+      <c r="O13">
+        <f>AVERAGE(N13:N42)</f>
+        <v>4.9336753333333326E-5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" t="s">
+        <v>79</v>
+      </c>
+      <c r="B14">
+        <f t="shared" ref="B14:C16" si="2">B6/6</f>
+        <v>1.5439113333333334E-3</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>1.5358139999999999E-4</v>
+      </c>
+      <c r="H14">
+        <v>2.29597E-3</v>
+      </c>
+      <c r="I14">
+        <f>AVERAGE(H14,H16,H18,H20,H22,H24,H26,H28,H30,H32,H34,H36,H38,H40,H42,H44,H46,H48,H50,H52,H54,H56,H58,H60,H62,H64,H66,H68,H70,H72)</f>
+        <v>2.1985126666666664E-3</v>
+      </c>
+      <c r="N14" s="6">
+        <v>6.38962E-5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B15">
+        <f t="shared" ref="B15:C16" si="3">B7/6</f>
+        <v>1.329104E-3</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>1.4033316666666669E-4</v>
+      </c>
+      <c r="H15">
+        <v>1.0596E-2</v>
+      </c>
+      <c r="N15" s="6">
+        <v>4.8160600000000001E-5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="A16" t="s">
+        <v>81</v>
+      </c>
+      <c r="B16">
+        <f t="shared" ref="B16:C16" si="4">B8/6</f>
+        <v>2.0701933333333335E-2</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>1.4806589999999999E-4</v>
+      </c>
+      <c r="H16">
+        <v>2.0680400000000002E-3</v>
+      </c>
+      <c r="N16" s="6">
+        <v>4.1007999999999998E-5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14">
+      <c r="H17">
+        <v>1.08261E-2</v>
+      </c>
+      <c r="N17" s="6">
+        <v>4.3869000000000003E-5</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14">
+      <c r="H18">
+        <v>2.2931100000000001E-3</v>
+      </c>
+      <c r="N18" s="6">
+        <v>4.00543E-5</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14">
+      <c r="H19">
+        <v>1.05679E-2</v>
+      </c>
+      <c r="N19" s="6">
+        <v>5.2928900000000001E-5</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14">
+      <c r="B20">
+        <v>0.12275999999999999</v>
+      </c>
+      <c r="C20">
+        <v>1.76859E-3</v>
+      </c>
+      <c r="H20">
+        <v>2.0639899999999999E-3</v>
+      </c>
+      <c r="N20" s="6">
+        <v>7.3909800000000002E-5</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14">
+      <c r="B21">
+        <v>0.121657</v>
+      </c>
+      <c r="C21">
+        <v>1.8277199999999999E-3</v>
+      </c>
+      <c r="H21">
+        <v>1.0808E-2</v>
+      </c>
+      <c r="N21" s="6">
+        <v>3.5047499999999999E-5</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14">
+      <c r="B22">
+        <v>0.12152399999999999</v>
+      </c>
+      <c r="C22">
+        <v>1.82128E-3</v>
+      </c>
+      <c r="H22">
+        <v>2.29597E-3</v>
+      </c>
+      <c r="N22" s="6">
+        <v>4.5061100000000001E-5</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14">
+      <c r="B23">
+        <v>0.12164</v>
+      </c>
+      <c r="C23">
+        <v>1.7950500000000001E-3</v>
+      </c>
+      <c r="H23">
+        <v>1.0623E-2</v>
+      </c>
+      <c r="N23" s="6">
+        <v>4.79221E-5</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14">
+      <c r="B24">
+        <v>0.122877</v>
+      </c>
+      <c r="C24">
+        <v>1.8951899999999999E-3</v>
+      </c>
+      <c r="H24">
+        <v>2.0730499999999999E-3</v>
+      </c>
+      <c r="N24" s="6">
+        <v>3.6001199999999997E-5</v>
+      </c>
+    </row>
+    <row r="25" spans="2:14">
+      <c r="H25">
+        <v>1.0822099999999999E-2</v>
+      </c>
+      <c r="N25" s="6">
+        <v>4.2915299999999999E-5</v>
+      </c>
+    </row>
+    <row r="26" spans="2:14">
+      <c r="B26">
+        <v>0.82776899999999998</v>
+      </c>
+      <c r="C26">
+        <v>2.7384499999999999E-2</v>
+      </c>
+      <c r="H26">
+        <v>2.2940600000000001E-3</v>
+      </c>
+      <c r="N26" s="6">
+        <v>3.3855400000000001E-5</v>
+      </c>
+    </row>
+    <row r="27" spans="2:14">
+      <c r="B27">
+        <v>0.82511500000000004</v>
+      </c>
+      <c r="C27">
+        <v>2.7247E-2</v>
+      </c>
+      <c r="H27">
+        <v>1.0600999999999999E-2</v>
+      </c>
+      <c r="N27" s="6">
+        <v>3.3140199999999998E-5</v>
+      </c>
+    </row>
+    <row r="28" spans="2:14">
+      <c r="B28">
+        <v>0.82740899999999995</v>
+      </c>
+      <c r="C28">
+        <v>2.73101E-2</v>
+      </c>
+      <c r="H28">
+        <v>2.1271699999999998E-3</v>
+      </c>
+      <c r="N28" s="6">
+        <v>4.6014799999999999E-5</v>
+      </c>
+    </row>
+    <row r="29" spans="2:14">
+      <c r="B29">
+        <v>0.82318199999999997</v>
+      </c>
+      <c r="C29">
+        <v>2.7354699999999999E-2</v>
+      </c>
+      <c r="H29">
+        <v>1.0898100000000001E-2</v>
+      </c>
+      <c r="N29">
+        <v>1.4805800000000001E-4</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14">
+      <c r="B30">
+        <v>0.82750100000000004</v>
+      </c>
+      <c r="C30">
+        <v>2.72927E-2</v>
+      </c>
+      <c r="H30">
+        <v>2.27904E-3</v>
+      </c>
+      <c r="N30" s="6">
+        <v>5.1975299999999997E-5</v>
+      </c>
+    </row>
+    <row r="31" spans="2:14">
+      <c r="H31">
+        <v>1.06509E-2</v>
+      </c>
+      <c r="N31" s="6">
+        <v>3.9100600000000003E-5</v>
+      </c>
+    </row>
+    <row r="32" spans="2:14">
+      <c r="B32">
+        <v>9.1590899999999999E-3</v>
+      </c>
+      <c r="C32">
+        <v>8.9788400000000005E-4</v>
+      </c>
+      <c r="H32">
+        <v>2.08092E-3</v>
+      </c>
+      <c r="N32" s="6">
+        <v>3.9100600000000003E-5</v>
+      </c>
+    </row>
+    <row r="33" spans="2:14">
+      <c r="B33">
+        <v>9.2520699999999994E-3</v>
+      </c>
+      <c r="C33">
+        <v>8.9550000000000003E-4</v>
+      </c>
+      <c r="H33">
+        <v>1.07229E-2</v>
+      </c>
+      <c r="N33" s="6">
+        <v>4.1007999999999998E-5</v>
+      </c>
+    </row>
+    <row r="34" spans="2:14">
+      <c r="B34">
+        <v>9.2201200000000001E-3</v>
+      </c>
+      <c r="C34">
+        <v>9.0789799999999997E-4</v>
+      </c>
+      <c r="H34">
+        <v>2.27809E-3</v>
+      </c>
+      <c r="N34" s="6">
+        <v>6.0081499999999997E-5</v>
+      </c>
+    </row>
+    <row r="35" spans="2:14">
+      <c r="B35">
+        <v>9.4020400000000004E-3</v>
+      </c>
+      <c r="C35">
+        <v>1.02878E-3</v>
+      </c>
+      <c r="H35">
+        <v>1.06699E-2</v>
+      </c>
+      <c r="N35" s="6">
+        <v>4.8875799999999997E-5</v>
+      </c>
+    </row>
+    <row r="36" spans="2:14">
+      <c r="B36">
+        <v>9.2840200000000005E-3</v>
+      </c>
+      <c r="C36">
+        <v>8.7737999999999998E-4</v>
+      </c>
+      <c r="H36">
+        <v>2.0849699999999998E-3</v>
+      </c>
+      <c r="N36" s="6">
+        <v>4.6968500000000003E-5</v>
+      </c>
+    </row>
+    <row r="37" spans="2:14">
+      <c r="H37">
+        <v>1.08211E-2</v>
+      </c>
+      <c r="N37" s="6">
+        <v>5.10216E-5</v>
+      </c>
+    </row>
+    <row r="38" spans="2:14">
+      <c r="B38">
+        <v>7.9748600000000003E-3</v>
+      </c>
+      <c r="C38">
+        <v>8.3804099999999998E-4</v>
+      </c>
+      <c r="H38">
+        <v>2.2940600000000001E-3</v>
+      </c>
+      <c r="N38" s="6">
+        <v>4.1007999999999998E-5</v>
+      </c>
+    </row>
+    <row r="39" spans="2:14">
+      <c r="B39">
+        <v>7.8949899999999993E-3</v>
+      </c>
+      <c r="C39">
+        <v>8.3780300000000003E-4</v>
+      </c>
+      <c r="H39">
+        <v>1.0643E-2</v>
+      </c>
+      <c r="N39" s="6">
+        <v>5.5074700000000003E-5</v>
+      </c>
+    </row>
+    <row r="40" spans="2:14">
+      <c r="B40">
+        <v>8.0170599999999995E-3</v>
+      </c>
+      <c r="C40">
+        <v>8.4209400000000005E-4</v>
+      </c>
+      <c r="H40">
+        <v>2.0790100000000001E-3</v>
+      </c>
+      <c r="N40" s="6">
+        <v>4.8160600000000001E-5</v>
+      </c>
+    </row>
+    <row r="41" spans="2:14">
+      <c r="B41">
+        <v>7.9710500000000004E-3</v>
+      </c>
+      <c r="C41">
+        <v>8.4400199999999995E-4</v>
+      </c>
+      <c r="H41">
+        <v>1.0730999999999999E-2</v>
+      </c>
+      <c r="N41" s="6">
+        <v>4.1007999999999998E-5</v>
+      </c>
+    </row>
+    <row r="42" spans="2:14">
+      <c r="B42">
+        <v>8.0151600000000003E-3</v>
+      </c>
+      <c r="C42">
+        <v>8.4805500000000001E-4</v>
+      </c>
+      <c r="H42">
+        <v>2.3260099999999999E-3</v>
+      </c>
+      <c r="N42" s="6">
+        <v>3.6001199999999997E-5</v>
+      </c>
+    </row>
+    <row r="43" spans="2:14">
+      <c r="H43">
+        <v>1.05541E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="2:14">
+      <c r="B44">
+        <v>0.12619900000000001</v>
+      </c>
+      <c r="C44">
+        <v>8.8906300000000005E-4</v>
+      </c>
+      <c r="H44">
+        <v>2.08807E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="2:14">
+      <c r="B45">
+        <v>0.124226</v>
+      </c>
+      <c r="C45">
+        <v>8.6402899999999999E-4</v>
+      </c>
+      <c r="H45">
+        <v>1.0726899999999999E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="2:14">
+      <c r="B46">
+        <v>0.123193</v>
+      </c>
+      <c r="C46">
+        <v>8.7308899999999996E-4</v>
+      </c>
+      <c r="H46">
+        <v>2.2809499999999999E-3</v>
+      </c>
+    </row>
+    <row r="47" spans="2:14">
+      <c r="B47">
+        <v>0.12363200000000001</v>
+      </c>
+      <c r="C47">
+        <v>9.17912E-4</v>
+      </c>
+      <c r="H47">
+        <v>1.0632000000000001E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="2:14">
+      <c r="B48">
+        <v>0.123808</v>
+      </c>
+      <c r="C48">
+        <v>8.9788400000000005E-4</v>
+      </c>
+      <c r="H48">
+        <v>2.08902E-3</v>
+      </c>
+    </row>
+    <row r="49" spans="8:8">
+      <c r="H49">
+        <v>1.0840900000000001E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="8:8">
+      <c r="H50">
+        <v>2.3000199999999998E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="8:8">
+      <c r="H51">
+        <v>1.0825899999999999E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="8:8">
+      <c r="H52">
+        <v>2.0811599999999999E-3</v>
+      </c>
+    </row>
+    <row r="53" spans="8:8">
+      <c r="H53">
+        <v>1.0726899999999999E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="8:8">
+      <c r="H54">
+        <v>2.4690599999999999E-3</v>
+      </c>
+    </row>
+    <row r="55" spans="8:8">
+      <c r="H55">
+        <v>1.0555999999999999E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="8:8">
+      <c r="H56">
+        <v>2.08092E-3</v>
+      </c>
+    </row>
+    <row r="57" spans="8:8">
+      <c r="H57">
+        <v>1.0655899999999999E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="8:8">
+      <c r="H58">
+        <v>2.2850000000000001E-3</v>
+      </c>
+    </row>
+    <row r="59" spans="8:8">
+      <c r="H59">
+        <v>1.05751E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="8:8">
+      <c r="H60">
+        <v>2.1579300000000002E-3</v>
+      </c>
+    </row>
+    <row r="61" spans="8:8">
+      <c r="H61">
+        <v>1.08171E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="8:8">
+      <c r="H62">
+        <v>2.3710699999999999E-3</v>
+      </c>
+    </row>
+    <row r="63" spans="8:8">
+      <c r="H63">
+        <v>1.0592900000000001E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="8:8">
+      <c r="H64">
+        <v>2.0739999999999999E-3</v>
+      </c>
+    </row>
+    <row r="65" spans="8:8">
+      <c r="H65">
+        <v>1.0721E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="8:8">
+      <c r="H66">
+        <v>2.2971599999999999E-3</v>
+      </c>
+    </row>
+    <row r="67" spans="8:8">
+      <c r="H67">
+        <v>1.05679E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="8:8">
+      <c r="H68">
+        <v>2.0749599999999998E-3</v>
+      </c>
+    </row>
+    <row r="69" spans="8:8">
+      <c r="H69">
+        <v>1.0819199999999999E-2</v>
+      </c>
+    </row>
+    <row r="70" spans="8:8">
+      <c r="H70">
+        <v>2.2997899999999999E-3</v>
+      </c>
+    </row>
+    <row r="71" spans="8:8">
+      <c r="H71">
+        <v>1.06239E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="8:8">
+      <c r="H72">
+        <v>2.07281E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="1" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated figures -- bigger font and markers.
git-svn-id: svn+ssh://software-srn.sandia.gov/svn/mapreduce/trunk@668 3fc257bb-8550-0410-81b3-a5c103da83f7
</commit_message>
<xml_diff>
--- a/paper/results.xlsx
+++ b/paper/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3660" yWindow="240" windowWidth="21600" windowHeight="13380" tabRatio="500" activeTab="7"/>
+    <workbookView xWindow="11380" yWindow="3020" windowWidth="21600" windowHeight="13380" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="CC" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <definedName name="jj_1" localSheetId="6">Sheet1!$N$41:$O$64</definedName>
     <definedName name="jjj" localSheetId="6">Sheet1!$BD$15:$BE$84</definedName>
   </definedNames>
-  <calcPr calcId="130406" concurrentCalc="0"/>
+  <calcPr calcId="130407" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
@@ -53,6 +53,78 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="92">
+  <si>
+    <t>R-MAT-20 (Original)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>RMAT-20 (Trilinos)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>RMAT-24 (Trilinos)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>RMAT-28 (Trilinos)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>R-MAT 20 (Old Cohen+Plimpton)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>R-MAT 20 (MR-MPI)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>New Cohen algorithm</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>R-MAT 24 (MR-MPI)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>R-MAT 28 (MR-MPI)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>R-MAT 20 (Trilinos+MR-MPI)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>R-MAT 24 (Trilinos+MR-MPI)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>R-MAT 28 (Trilinos+NR-MPI)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enhanced Algorithm</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>R-MAT 20 (MR-MPI)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>R-MAT 20 (MR-MPI)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>R-MAT 24 (MR-MPI)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>R-MAT 24 (Original)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>New Algorithm</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
   <si>
     <t>XMT</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -349,89 +421,11 @@
     <t>RMAT-28 (Original)</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
-  <si>
-    <t>R-MAT-20 (Original)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>RMAT-20 (Trilinos)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>RMAT-24 (Trilinos)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>RMAT-28 (Trilinos)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>R-MAT 20 (Old Cohen+Plimpton)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>R-MAT 20 (MR-MPI)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>New Cohen algorithm</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>R-MAT 24 (MR-MPI)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>R-MAT 28 (MR-MPI)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>R-MAT 20 (Trilinos+MR-MPI)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>R-MAT 24 (Trilinos+MR-MPI)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>R-MAT 28 (Trilinos+NR-MPI)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Enhanced Algorithm</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>R-MAT 20 (MR-MPI)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>R-MAT 20 (MR-MPI)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>R-MAT 24 (MR-MPI)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>R-MAT 24 (Original)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>New Algorithm</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
   <fonts count="5">
     <font>
       <sz val="10"/>
@@ -516,6 +510,33 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$AL$5:$AL$11</c:f>
@@ -579,6 +600,10 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="8"/>
+          </c:marker>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$AL$5:$AL$11</c:f>
@@ -654,6 +679,10 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="8"/>
+          </c:marker>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$AL$5:$AL$11</c:f>
@@ -729,6 +758,36 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="60000"/>
+                    <a:lumOff val="40000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$AL$5:$AL$11</c:f>
@@ -801,6 +860,36 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                    <a:lumOff val="40000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$AL$5:$AL$11</c:f>
@@ -862,11 +951,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="591489816"/>
-        <c:axId val="591476040"/>
+        <c:axId val="105452312"/>
+        <c:axId val="105461704"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="591489816"/>
+        <c:axId val="105452312"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -879,10 +968,10 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="1200"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1200"/>
                   <a:t>Number of Processors</a:t>
                 </a:r>
               </a:p>
@@ -893,12 +982,22 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="591476040"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="105461704"/>
         <c:crossesAt val="0.1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="591476040"/>
+        <c:axId val="105461704"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -912,10 +1011,10 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="1200"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1200"/>
                   <a:t>Time (seconds)</a:t>
                 </a:r>
               </a:p>
@@ -923,10 +1022,20 @@
           </c:tx>
           <c:layout/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.E+00" sourceLinked="0"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="591489816"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="105452312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -934,6 +1043,16 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -964,6 +1083,33 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$N$5:$N$11</c:f>
@@ -1030,6 +1176,10 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="8"/>
+          </c:marker>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$N$5:$N$11</c:f>
@@ -1105,6 +1255,10 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="8"/>
+          </c:marker>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$N$5:$N$11</c:f>
@@ -1180,6 +1334,33 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$N$5:$N$11</c:f>
@@ -1237,6 +1418,36 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="60000"/>
+                    <a:lumOff val="40000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$N$5:$N$11</c:f>
@@ -1309,6 +1520,36 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                    <a:lumOff val="40000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$N$5:$N$11</c:f>
@@ -1370,11 +1611,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="591680904"/>
-        <c:axId val="591686872"/>
+        <c:axId val="852103496"/>
+        <c:axId val="852095560"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="591680904"/>
+        <c:axId val="852103496"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1387,24 +1628,35 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="1200"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1200"/>
                   <a:t>Number of Processors</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="591686872"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="852095560"/>
         <c:crossesAt val="0.0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="591686872"/>
+        <c:axId val="852095560"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1418,26 +1670,48 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="1200"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1200"/>
                   <a:t>Time per PageRank Iteration (seconds)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="0.E+00" sourceLinked="0"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="591680904"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="852103496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -1469,6 +1743,33 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$BD$5:$BD$11</c:f>
@@ -1529,6 +1830,33 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$BD$5:$BD$11</c:f>
@@ -1592,6 +1920,36 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="60000"/>
+                    <a:lumOff val="40000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$BD$5:$BD$11</c:f>
@@ -1667,6 +2025,10 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+          </c:marker>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$BD$5:$BD$11</c:f>
@@ -1742,6 +2104,36 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                    <a:lumOff val="40000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$BD$5:$BD$11</c:f>
@@ -1817,6 +2209,10 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+          </c:marker>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$BD$5:$BD$11</c:f>
@@ -1878,11 +2274,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="591744104"/>
-        <c:axId val="591750104"/>
+        <c:axId val="852231944"/>
+        <c:axId val="852237944"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="591744104"/>
+        <c:axId val="852231944"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1895,25 +2291,36 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="1200"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1200"/>
                   <a:t>Number of Processors</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="591750104"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="852237944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="591750104"/>
+        <c:axId val="852237944"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1927,26 +2334,48 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="1200"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1200"/>
                   <a:t>Time (secs)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
-        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:numFmt formatCode="0.E+00" sourceLinked="0"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="591744104"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="852231944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -1978,6 +2407,26 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$A$5:$A$11</c:f>
@@ -2047,6 +2496,10 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+          </c:marker>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$A$5:$A$11</c:f>
@@ -2122,6 +2575,10 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="8"/>
+          </c:marker>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$A$5:$A$11</c:f>
@@ -2183,11 +2640,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="591790664"/>
-        <c:axId val="591800792"/>
+        <c:axId val="852277208"/>
+        <c:axId val="852287304"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="591790664"/>
+        <c:axId val="852277208"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2200,25 +2657,36 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="1200"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1200"/>
                   <a:t>Number of Processors</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="591800792"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="852287304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="591800792"/>
+        <c:axId val="852287304"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2232,26 +2700,48 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="1200"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1200"/>
                   <a:t>Time (secs)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
-        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:numFmt formatCode="0.E+00" sourceLinked="0"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="591790664"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="852277208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -2270,19 +2760,39 @@
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="2"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$AA$4</c:f>
+              <c:f>Sheet1!$AC$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>R-MAT 20 (MR-MPI)</c:v>
+                  <c:v>R-MAT 28 (MR-MPI)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$Z$5:$Z$11</c:f>
@@ -2315,30 +2825,21 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$AA$5:$AA$11</c:f>
+              <c:f>Sheet1!$AC$5:$AC$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>150.766</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>106.484</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>53.9303</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>18.2997</c:v>
+                  <c:v>23233.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.126341999999999</c:v>
+                  <c:v>11092.4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.11674</c:v>
+                  <c:v>5725.976000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.108394</c:v>
+                  <c:v>2827.016000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2358,6 +2859,10 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+          </c:marker>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$Z$5:$Z$11</c:f>
@@ -2420,19 +2925,23 @@
           </c:yVal>
         </c:ser>
         <c:ser>
-          <c:idx val="2"/>
+          <c:idx val="0"/>
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$AC$4</c:f>
+              <c:f>Sheet1!$AA$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>R-MAT 28 (MR-MPI)</c:v>
+                  <c:v>R-MAT 20 (MR-MPI)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="8"/>
+          </c:marker>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$Z$5:$Z$11</c:f>
@@ -2465,31 +2974,40 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$AC$5:$AC$11</c:f>
+              <c:f>Sheet1!$AA$5:$AA$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>150.766</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>106.484</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>53.9303</c:v>
+                </c:pt>
                 <c:pt idx="3">
-                  <c:v>23233.0</c:v>
+                  <c:v>18.2997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11092.4</c:v>
+                  <c:v>4.126341999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5725.976000000001</c:v>
+                  <c:v>2.11674</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2827.016000000001</c:v>
+                  <c:v>1.108394</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="591842952"/>
-        <c:axId val="591853048"/>
+        <c:axId val="852329656"/>
+        <c:axId val="852339752"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="591842952"/>
+        <c:axId val="852329656"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2502,25 +3020,36 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="1200"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1200"/>
                   <a:t>Number of Processors</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="591853048"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="852339752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="591853048"/>
+        <c:axId val="852339752"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2534,26 +3063,48 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="1200"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1200"/>
                   <a:t>Time (secs)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.E+00" sourceLinked="0"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="591842952"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="852329656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -2595,6 +3146,10 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+          </c:marker>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$AX$5:$AX$11</c:f>
@@ -2664,6 +3219,10 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="8"/>
+          </c:marker>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$AX$5:$AX$11</c:f>
@@ -2725,11 +3284,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="591889896"/>
-        <c:axId val="591902360"/>
+        <c:axId val="852376856"/>
+        <c:axId val="852389320"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="591889896"/>
+        <c:axId val="852376856"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2742,25 +3301,36 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="1200"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1200"/>
                   <a:t>Number of Processors</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="591902360"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="852389320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="591902360"/>
+        <c:axId val="852389320"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2774,26 +3344,48 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="1200"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1200"/>
                   <a:t>Time (secs)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.E+00" sourceLinked="0"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="591889896"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="852376856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -3330,11 +3922,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="592024216"/>
-        <c:axId val="592029992"/>
+        <c:axId val="865110152"/>
+        <c:axId val="865115928"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="592024216"/>
+        <c:axId val="865110152"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -3360,13 +3952,13 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="592029992"/>
+        <c:crossAx val="865115928"/>
         <c:crossesAt val="0.001"/>
         <c:crossBetween val="midCat"/>
         <c:minorUnit val="10.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="592029992"/>
+        <c:axId val="865115928"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -3393,7 +3985,7 @@
         <c:numFmt formatCode="0.E+00" sourceLinked="0"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="592024216"/>
+        <c:crossAx val="865110152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3861,11 +4453,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="592064312"/>
-        <c:axId val="592070312"/>
+        <c:axId val="865150808"/>
+        <c:axId val="865156808"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="592064312"/>
+        <c:axId val="865150808"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -3891,12 +4483,12 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="592070312"/>
+        <c:crossAx val="865156808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="592070312"/>
+        <c:axId val="865156808"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -3923,7 +4515,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="592064312"/>
+        <c:crossAx val="865150808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3943,7 +4535,7 @@
 
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr published="0"/>
+  <sheetPr/>
   <sheetViews>
     <sheetView zoomScale="97" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
@@ -3955,7 +4547,7 @@
 
 <file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr published="0"/>
+  <sheetPr/>
   <sheetViews>
     <sheetView zoomScale="97" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
@@ -3967,7 +4559,7 @@
 
 <file path=xl/chartsheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr published="0"/>
+  <sheetPr/>
   <sheetViews>
     <sheetView zoomScale="116" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
@@ -3979,7 +4571,7 @@
 
 <file path=xl/chartsheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr published="0"/>
+  <sheetPr/>
   <sheetViews>
     <sheetView zoomScale="116" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
@@ -3991,7 +4583,7 @@
 
 <file path=xl/chartsheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr published="0"/>
+  <sheetPr/>
   <sheetViews>
     <sheetView zoomScale="116" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
@@ -4003,9 +4595,9 @@
 
 <file path=xl/chartsheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr published="0"/>
+  <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="116" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="116" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -4241,11 +4833,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="jjj" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="jj_1" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="jj_1" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="jjj" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4568,7 +5160,6 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:BO85"/>
   <sheetViews>
     <sheetView view="pageLayout" topLeftCell="K1" workbookViewId="0">
@@ -4586,235 +5177,235 @@
   <sheetData>
     <row r="1" spans="1:67">
       <c r="A1" t="s">
+        <v>81</v>
+      </c>
+      <c r="N1" t="s">
+        <v>69</v>
+      </c>
+      <c r="T1" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>79</v>
+      </c>
+      <c r="BD1" t="s">
         <v>63</v>
-      </c>
-      <c r="N1" t="s">
-        <v>51</v>
-      </c>
-      <c r="T1" t="s">
-        <v>62</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>59</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>60</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>61</v>
-      </c>
-      <c r="BD1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:67">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="N2" t="s">
-        <v>48</v>
+        <v>66</v>
       </c>
       <c r="P2" t="s">
-        <v>54</v>
+        <v>72</v>
       </c>
       <c r="BD2" t="s">
-        <v>48</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:67">
       <c r="C3" t="s">
-        <v>91</v>
+        <v>17</v>
       </c>
       <c r="F3" t="s">
-        <v>53</v>
+        <v>71</v>
       </c>
       <c r="G3" t="s">
-        <v>55</v>
+        <v>73</v>
       </c>
       <c r="I3" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="O3" t="s">
+        <v>12</v>
+      </c>
+      <c r="S3" t="s">
+        <v>74</v>
+      </c>
+      <c r="U3" t="s">
+        <v>75</v>
+      </c>
+      <c r="V3" t="s">
+        <v>76</v>
+      </c>
+      <c r="W3" t="s">
+        <v>76</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>6</v>
+      </c>
+      <c r="AR3" t="s">
+        <v>85</v>
+      </c>
+      <c r="AU3" t="s">
         <v>86</v>
       </c>
-      <c r="S3" t="s">
-        <v>56</v>
-      </c>
-      <c r="U3" t="s">
-        <v>57</v>
-      </c>
-      <c r="V3" t="s">
-        <v>58</v>
-      </c>
-      <c r="W3" t="s">
-        <v>58</v>
-      </c>
-      <c r="AM3" t="s">
-        <v>80</v>
-      </c>
-      <c r="AR3" t="s">
-        <v>67</v>
-      </c>
-      <c r="AU3" t="s">
-        <v>68</v>
-      </c>
       <c r="BB3" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="BJ3" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="BK3" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="BL3" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:67">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>67</v>
       </c>
       <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" t="s">
+        <v>91</v>
+      </c>
+      <c r="I4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K4" t="s">
+        <v>60</v>
+      </c>
+      <c r="N4" t="s">
+        <v>67</v>
+      </c>
+      <c r="O4" t="s">
+        <v>13</v>
+      </c>
+      <c r="P4" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>62</v>
+      </c>
+      <c r="R4" t="s">
+        <v>68</v>
+      </c>
+      <c r="S4" t="s">
+        <v>90</v>
+      </c>
+      <c r="U4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" t="s">
+      <c r="V4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" t="s">
+      <c r="W4" t="s">
         <v>3</v>
       </c>
-      <c r="E4" t="s">
-        <v>50</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="Z4" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>68</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>67</v>
+      </c>
+      <c r="AM4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AN4" t="s">
+        <v>7</v>
+      </c>
+      <c r="AO4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AP4" t="s">
+        <v>68</v>
+      </c>
+      <c r="AR4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AS4" t="s">
+        <v>64</v>
+      </c>
+      <c r="AT4" t="s">
+        <v>65</v>
+      </c>
+      <c r="AU4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AV4" t="s">
+        <v>10</v>
+      </c>
+      <c r="AW4" t="s">
+        <v>11</v>
+      </c>
+      <c r="AX4" t="s">
+        <v>67</v>
+      </c>
+      <c r="AY4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AZ4" t="s">
+        <v>61</v>
+      </c>
+      <c r="BB4" t="s">
+        <v>23</v>
+      </c>
+      <c r="BC4" t="s">
+        <v>24</v>
+      </c>
+      <c r="BD4" t="s">
+        <v>67</v>
+      </c>
+      <c r="BE4" t="s">
+        <v>87</v>
+      </c>
+      <c r="BF4" t="s">
+        <v>88</v>
+      </c>
+      <c r="BG4" t="s">
+        <v>89</v>
+      </c>
+      <c r="BH4" t="s">
+        <v>68</v>
+      </c>
+      <c r="BJ4" t="s">
+        <v>0</v>
+      </c>
+      <c r="BK4" t="s">
         <v>90</v>
       </c>
-      <c r="G4" t="s">
-        <v>73</v>
-      </c>
-      <c r="I4" t="s">
-        <v>5</v>
-      </c>
-      <c r="J4" t="s">
-        <v>6</v>
-      </c>
-      <c r="K4" t="s">
-        <v>42</v>
-      </c>
-      <c r="N4" t="s">
-        <v>49</v>
-      </c>
-      <c r="O4" t="s">
-        <v>87</v>
-      </c>
-      <c r="P4" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>44</v>
-      </c>
-      <c r="R4" t="s">
-        <v>50</v>
-      </c>
-      <c r="S4" t="s">
-        <v>72</v>
-      </c>
-      <c r="U4" t="s">
-        <v>75</v>
-      </c>
-      <c r="V4" t="s">
-        <v>76</v>
-      </c>
-      <c r="W4" t="s">
-        <v>77</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>49</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>88</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>89</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>44</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>50</v>
-      </c>
-      <c r="AL4" t="s">
-        <v>49</v>
-      </c>
-      <c r="AM4" t="s">
-        <v>79</v>
-      </c>
-      <c r="AN4" t="s">
-        <v>81</v>
-      </c>
-      <c r="AO4" t="s">
-        <v>82</v>
-      </c>
-      <c r="AP4" t="s">
-        <v>50</v>
-      </c>
-      <c r="AR4" t="s">
-        <v>78</v>
-      </c>
-      <c r="AS4" t="s">
-        <v>46</v>
-      </c>
-      <c r="AT4" t="s">
-        <v>47</v>
-      </c>
-      <c r="AU4" t="s">
-        <v>83</v>
-      </c>
-      <c r="AV4" t="s">
-        <v>84</v>
-      </c>
-      <c r="AW4" t="s">
-        <v>85</v>
-      </c>
-      <c r="AX4" t="s">
-        <v>49</v>
-      </c>
-      <c r="AY4" t="s">
-        <v>79</v>
-      </c>
-      <c r="AZ4" t="s">
-        <v>43</v>
-      </c>
-      <c r="BB4" t="s">
-        <v>5</v>
-      </c>
-      <c r="BC4" t="s">
-        <v>6</v>
-      </c>
-      <c r="BD4" t="s">
-        <v>49</v>
-      </c>
-      <c r="BE4" t="s">
-        <v>69</v>
-      </c>
-      <c r="BF4" t="s">
-        <v>70</v>
-      </c>
-      <c r="BG4" t="s">
-        <v>71</v>
-      </c>
-      <c r="BH4" t="s">
-        <v>50</v>
-      </c>
-      <c r="BJ4" t="s">
-        <v>74</v>
-      </c>
-      <c r="BK4" t="s">
-        <v>72</v>
-      </c>
       <c r="BL4" t="s">
-        <v>73</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:67">
@@ -5957,7 +6548,7 @@
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3" t="s">
-        <v>52</v>
+        <v>70</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -5972,7 +6563,7 @@
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="1" t="s">
-        <v>52</v>
+        <v>70</v>
       </c>
       <c r="R12" s="1"/>
       <c r="BD12">
@@ -9945,6 +10536,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -9959,10 +10551,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:R72"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="M1" workbookViewId="0">
+    <sheetView view="pageLayout" topLeftCell="M1" workbookViewId="0">
       <selection activeCell="R4" sqref="R4:R7"/>
     </sheetView>
   </sheetViews>
@@ -9970,70 +10561,70 @@
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="G1" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="M1" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="N1" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:18">
       <c r="B2" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:18">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="H3" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="I3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L3" t="s">
+        <v>39</v>
+      </c>
+      <c r="N3" t="s">
         <v>26</v>
       </c>
-      <c r="K3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N3" t="s">
-        <v>8</v>
-      </c>
       <c r="Q3" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="R3" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:18">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="B4">
         <f>AVERAGE(B20:B24)</f>
@@ -10050,7 +10641,7 @@
         <v>0.41922300000000001</v>
       </c>
       <c r="G4" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="H4">
         <v>1.5562099999999999E-3</v>
@@ -10067,7 +10658,7 @@
         <v>0.36984467309977737</v>
       </c>
       <c r="M4" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="N4">
         <v>4.6457999999999997E-4</v>
@@ -10086,7 +10677,7 @@
     </row>
     <row r="5" spans="1:18">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="B5">
         <f>AVERAGE(B26:B30)</f>
@@ -10103,7 +10694,7 @@
         <v>14.619300000000001</v>
       </c>
       <c r="G5" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="H5">
         <v>4.0733200000000001E-3</v>
@@ -10120,7 +10711,7 @@
         <v>14.262968770746806</v>
       </c>
       <c r="M5" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="N5">
         <v>1.9678310000000001E-2</v>
@@ -10139,7 +10730,7 @@
     </row>
     <row r="6" spans="1:18">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="B6">
         <f>AVERAGE(B32:B36)</f>
@@ -10156,7 +10747,7 @@
         <v>0.24682000000000001</v>
       </c>
       <c r="G6" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="H6">
         <v>3.2574150000000003E-2</v>
@@ -10173,7 +10764,7 @@
         <v>43.650122067276612</v>
       </c>
       <c r="M6" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="N6">
         <v>5.31E-4</v>
@@ -10192,7 +10783,7 @@
     </row>
     <row r="7" spans="1:18">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="B7">
         <f>AVERAGE(B38:B42)</f>
@@ -10209,7 +10800,7 @@
         <v>0.179397</v>
       </c>
       <c r="G7" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="H7">
         <v>1.070432E-2</v>
@@ -10226,7 +10817,7 @@
         <v>5.7718544876048199</v>
       </c>
       <c r="M7" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="N7" s="6">
         <v>4.9336999999999999E-5</v>
@@ -10245,7 +10836,7 @@
     </row>
     <row r="8" spans="1:18">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="B8">
         <f>AVERAGE(B44:B48)</f>
@@ -10262,7 +10853,7 @@
         <v>0.22862499999999999</v>
       </c>
       <c r="G8" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="H8">
         <v>3.4496720000000002E-2</v>
@@ -10281,7 +10872,7 @@
     </row>
     <row r="9" spans="1:18">
       <c r="G9" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="H9">
         <v>5.296878E-2</v>
@@ -10300,13 +10891,13 @@
     </row>
     <row r="10" spans="1:18">
       <c r="B10" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="E10" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="G10" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="H10">
         <v>2.1985099999999999E-3</v>
@@ -10325,24 +10916,24 @@
     </row>
     <row r="11" spans="1:18">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="C11" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
       <c r="E11" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="F11" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:18">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="B12">
         <f>B4/6</f>
@@ -10353,20 +10944,20 @@
         <v>3.0359433333333334E-4</v>
       </c>
       <c r="E12">
-        <f>E4/5</f>
+        <f t="shared" ref="E12:F16" si="3">E4/5</f>
         <v>17.530059999999999</v>
       </c>
       <c r="F12">
-        <f>F4/5</f>
+        <f t="shared" si="3"/>
         <v>8.3844600000000005E-2</v>
       </c>
     </row>
     <row r="13" spans="1:18">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="B13">
-        <f t="shared" ref="B13" si="3">B5/6</f>
+        <f t="shared" ref="B13" si="4">B5/6</f>
         <v>0.13769920000000002</v>
       </c>
       <c r="C13">
@@ -10374,11 +10965,11 @@
         <v>4.5529666666666658E-3</v>
       </c>
       <c r="E13">
-        <f>E5/5</f>
+        <f t="shared" si="3"/>
         <v>341.26400000000001</v>
       </c>
       <c r="F13">
-        <f>F5/5</f>
+        <f t="shared" si="3"/>
         <v>2.9238600000000003</v>
       </c>
       <c r="H13">
@@ -10412,10 +11003,10 @@
     </row>
     <row r="14" spans="1:18">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="B14">
-        <f t="shared" ref="B14" si="4">B6/6</f>
+        <f t="shared" ref="B14" si="5">B6/6</f>
         <v>1.5439113333333334E-3</v>
       </c>
       <c r="C14">
@@ -10423,11 +11014,11 @@
         <v>1.5358139999999999E-4</v>
       </c>
       <c r="E14">
-        <f>E6/5</f>
+        <f t="shared" si="3"/>
         <v>2.1462599999999998</v>
       </c>
       <c r="F14">
-        <f>F6/5</f>
+        <f t="shared" si="3"/>
         <v>4.9364000000000005E-2</v>
       </c>
       <c r="H14">
@@ -10453,10 +11044,10 @@
     </row>
     <row r="15" spans="1:18">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="B15">
-        <f t="shared" ref="B15" si="5">B7/6</f>
+        <f t="shared" ref="B15" si="6">B7/6</f>
         <v>1.329104E-3</v>
       </c>
       <c r="C15">
@@ -10464,11 +11055,11 @@
         <v>1.4033316666666669E-4</v>
       </c>
       <c r="E15">
-        <f>E7/5</f>
+        <f t="shared" si="3"/>
         <v>1.7443040000000001</v>
       </c>
       <c r="F15">
-        <f>F7/5</f>
+        <f t="shared" si="3"/>
         <v>3.5879399999999999E-2</v>
       </c>
       <c r="H15">
@@ -10486,10 +11077,10 @@
     </row>
     <row r="16" spans="1:18">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="B16">
-        <f t="shared" ref="B16" si="6">B8/6</f>
+        <f t="shared" ref="B16" si="7">B8/6</f>
         <v>2.0701933333333335E-2</v>
       </c>
       <c r="C16">
@@ -10497,11 +11088,11 @@
         <v>1.4806589999999999E-4</v>
       </c>
       <c r="E16">
-        <f>E8/5</f>
+        <f t="shared" si="3"/>
         <v>21.2088</v>
       </c>
       <c r="F16">
-        <f>F8/5</f>
+        <f t="shared" si="3"/>
         <v>4.5725000000000002E-2</v>
       </c>
       <c r="H16">

</xml_diff>

<commit_message>
Many redone figures so they look better in B&W.
git-svn-id: svn+ssh://software-srn.sandia.gov/svn/mapreduce/trunk@817 3fc257bb-8550-0410-81b3-a5c103da83f7
</commit_message>
<xml_diff>
--- a/paper/results.xlsx
+++ b/paper/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="11380" yWindow="3020" windowWidth="21600" windowHeight="13380" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="460" yWindow="-420" windowWidth="25500" windowHeight="20680" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="CC" sheetId="2" r:id="rId1"/>
@@ -53,6 +53,98 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="92">
+  <si>
+    <t>PageRank</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>ORIG ALG</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Times per iteration</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>ORIG ALG</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>ORIG ALG</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Trilinos</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Trilinos</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Luby</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>CC</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tri</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pagerank</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>RMAT Generation</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>All runs on odin, pernode mode</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Old ALG</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Old ALG</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Old-Alg</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Trilinos+CC Hybrid</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>R-MAT 20 (Enhanced)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>R-MAT 24 (Enhanced)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>R-MAT 28 (Enhanced)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>R-MAT 24 (Original)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>RMAT-28 (Original)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
   <si>
     <t>R-MAT-20 (Original)</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -329,98 +421,6 @@
     <t>R-MAT 32</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
-  <si>
-    <t>PageRank</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>ORIG ALG</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Times per iteration</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>ORIG ALG</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>ORIG ALG</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Trilinos</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Trilinos</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Luby</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>CC</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Tri</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Pagerank</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>RMAT Generation</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>All runs on odin, pernode mode</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Old ALG</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Old ALG</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Old-Alg</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Trilinos+CC Hybrid</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>R-MAT 20 (Enhanced)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>R-MAT 24 (Enhanced)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>R-MAT 28 (Enhanced)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>R-MAT 24 (Original)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>RMAT-28 (Original)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
 </sst>
 </file>
 
@@ -521,7 +521,7 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="triangle"/>
-            <c:size val="8"/>
+            <c:size val="10"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent3">
@@ -601,8 +601,8 @@
             </c:strRef>
           </c:tx>
           <c:marker>
-            <c:symbol val="triangle"/>
-            <c:size val="8"/>
+            <c:symbol val="square"/>
+            <c:size val="10"/>
           </c:marker>
           <c:xVal>
             <c:numRef>
@@ -680,8 +680,17 @@
             </c:strRef>
           </c:tx>
           <c:marker>
-            <c:symbol val="triangle"/>
-            <c:size val="8"/>
+            <c:symbol val="circle"/>
+            <c:size val="10"/>
+            <c:spPr>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
           </c:marker>
           <c:xVal>
             <c:numRef>
@@ -761,29 +770,24 @@
           <c:spPr>
             <a:ln>
               <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
             </a:ln>
           </c:spPr>
           <c:marker>
             <c:symbol val="square"/>
-            <c:size val="8"/>
+            <c:size val="10"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2">
+                <a:srgbClr val="C0504D">
                   <a:lumMod val="60000"/>
                   <a:lumOff val="40000"/>
-                </a:schemeClr>
+                  <a:alpha val="0"/>
+                </a:srgbClr>
               </a:solidFill>
               <a:ln>
                 <a:solidFill>
-                  <a:schemeClr val="accent2">
-                    <a:lumMod val="60000"/>
-                    <a:lumOff val="40000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="accent2"/>
                 </a:solidFill>
               </a:ln>
             </c:spPr>
@@ -864,27 +868,26 @@
             <a:ln>
               <a:solidFill>
                 <a:schemeClr val="accent1">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
+                  <a:lumMod val="75000"/>
                 </a:schemeClr>
               </a:solidFill>
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:symbol val="square"/>
-            <c:size val="8"/>
+            <c:symbol val="circle"/>
+            <c:size val="10"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1">
+                <a:srgbClr val="4F81BD">
                   <a:lumMod val="60000"/>
                   <a:lumOff val="40000"/>
-                </a:schemeClr>
+                  <a:alpha val="0"/>
+                </a:srgbClr>
               </a:solidFill>
               <a:ln>
                 <a:solidFill>
                   <a:schemeClr val="accent1">
-                    <a:lumMod val="60000"/>
-                    <a:lumOff val="40000"/>
+                    <a:lumMod val="75000"/>
                   </a:schemeClr>
                 </a:solidFill>
               </a:ln>
@@ -951,11 +954,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="105452312"/>
-        <c:axId val="105461704"/>
+        <c:axId val="998455000"/>
+        <c:axId val="998462904"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="105452312"/>
+        <c:axId val="998455000"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -992,12 +995,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="105461704"/>
+        <c:crossAx val="998462904"/>
         <c:crossesAt val="0.1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="105461704"/>
+        <c:axId val="998462904"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1035,7 +1038,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="105452312"/>
+        <c:crossAx val="998455000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1094,7 +1097,7 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="triangle"/>
-            <c:size val="8"/>
+            <c:size val="10"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent3">
@@ -1177,8 +1180,8 @@
             </c:strRef>
           </c:tx>
           <c:marker>
-            <c:symbol val="triangle"/>
-            <c:size val="8"/>
+            <c:symbol val="square"/>
+            <c:size val="10"/>
           </c:marker>
           <c:xVal>
             <c:numRef>
@@ -1256,8 +1259,8 @@
             </c:strRef>
           </c:tx>
           <c:marker>
-            <c:symbol val="triangle"/>
-            <c:size val="8"/>
+            <c:symbol val="circle"/>
+            <c:size val="10"/>
           </c:marker>
           <c:xVal>
             <c:numRef>
@@ -1344,13 +1347,14 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:symbol val="square"/>
-            <c:size val="7"/>
+            <c:symbol val="triangle"/>
+            <c:size val="10"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent3">
+                <a:srgbClr val="9BBB59">
                   <a:lumMod val="75000"/>
-                </a:schemeClr>
+                  <a:alpha val="0"/>
+                </a:srgbClr>
               </a:solidFill>
               <a:ln>
                 <a:solidFill>
@@ -1421,29 +1425,24 @@
           <c:spPr>
             <a:ln>
               <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
             </a:ln>
           </c:spPr>
           <c:marker>
             <c:symbol val="square"/>
-            <c:size val="8"/>
+            <c:size val="10"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2">
+                <a:srgbClr val="C0504D">
                   <a:lumMod val="60000"/>
                   <a:lumOff val="40000"/>
-                </a:schemeClr>
+                  <a:alpha val="0"/>
+                </a:srgbClr>
               </a:solidFill>
               <a:ln>
                 <a:solidFill>
-                  <a:schemeClr val="accent2">
-                    <a:lumMod val="60000"/>
-                    <a:lumOff val="40000"/>
-                  </a:schemeClr>
+                  <a:srgbClr val="C0504D"/>
                 </a:solidFill>
               </a:ln>
             </c:spPr>
@@ -1523,29 +1522,22 @@
           <c:spPr>
             <a:ln>
               <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:symbol val="square"/>
-            <c:size val="8"/>
+            <c:symbol val="circle"/>
+            <c:size val="10"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent1">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
+                  <a:alpha val="0"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:ln>
                 <a:solidFill>
-                  <a:schemeClr val="accent1">
-                    <a:lumMod val="60000"/>
-                    <a:lumOff val="40000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="accent1"/>
                 </a:solidFill>
               </a:ln>
             </c:spPr>
@@ -1611,11 +1603,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="852103496"/>
-        <c:axId val="852095560"/>
+        <c:axId val="998526856"/>
+        <c:axId val="998534744"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="852103496"/>
+        <c:axId val="998526856"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1651,12 +1643,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="852095560"/>
+        <c:crossAx val="998534744"/>
         <c:crossesAt val="0.0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="852095560"/>
+        <c:axId val="998534744"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1694,7 +1686,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="852103496"/>
+        <c:crossAx val="998526856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1747,24 +1739,25 @@
             <a:ln>
               <a:solidFill>
                 <a:schemeClr val="accent3">
-                  <a:lumMod val="75000"/>
+                  <a:lumMod val="50000"/>
                 </a:schemeClr>
               </a:solidFill>
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="8"/>
+            <c:symbol val="triangle"/>
+            <c:size val="10"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent3">
+                <a:srgbClr val="9BBB59">
                   <a:lumMod val="75000"/>
-                </a:schemeClr>
+                  <a:alpha val="0"/>
+                </a:srgbClr>
               </a:solidFill>
               <a:ln>
                 <a:solidFill>
                   <a:schemeClr val="accent3">
-                    <a:lumMod val="75000"/>
+                    <a:lumMod val="50000"/>
                   </a:schemeClr>
                 </a:solidFill>
               </a:ln>
@@ -1840,8 +1833,8 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:symbol val="square"/>
-            <c:size val="8"/>
+            <c:symbol val="triangle"/>
+            <c:size val="10"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent3">
@@ -1923,29 +1916,24 @@
           <c:spPr>
             <a:ln>
               <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="8"/>
+            <c:symbol val="square"/>
+            <c:size val="10"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2">
+                <a:srgbClr val="C0504D">
                   <a:lumMod val="60000"/>
                   <a:lumOff val="40000"/>
-                </a:schemeClr>
+                  <a:alpha val="0"/>
+                </a:srgbClr>
               </a:solidFill>
               <a:ln>
                 <a:solidFill>
-                  <a:schemeClr val="accent2">
-                    <a:lumMod val="60000"/>
-                    <a:lumOff val="40000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="accent2"/>
                 </a:solidFill>
               </a:ln>
             </c:spPr>
@@ -2027,7 +2015,7 @@
           </c:tx>
           <c:marker>
             <c:symbol val="square"/>
-            <c:size val="8"/>
+            <c:size val="10"/>
           </c:marker>
           <c:xVal>
             <c:numRef>
@@ -2107,29 +2095,24 @@
           <c:spPr>
             <a:ln>
               <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
             </a:ln>
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="8"/>
+            <c:size val="10"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1">
+                <a:srgbClr val="4F81BD">
                   <a:lumMod val="60000"/>
                   <a:lumOff val="40000"/>
-                </a:schemeClr>
+                  <a:alpha val="0"/>
+                </a:srgbClr>
               </a:solidFill>
               <a:ln>
                 <a:solidFill>
-                  <a:schemeClr val="accent1">
-                    <a:lumMod val="60000"/>
-                    <a:lumOff val="40000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="accent1"/>
                 </a:solidFill>
               </a:ln>
             </c:spPr>
@@ -2210,8 +2193,8 @@
             </c:strRef>
           </c:tx>
           <c:marker>
-            <c:symbol val="square"/>
-            <c:size val="8"/>
+            <c:symbol val="circle"/>
+            <c:size val="10"/>
           </c:marker>
           <c:xVal>
             <c:numRef>
@@ -2274,11 +2257,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="852231944"/>
-        <c:axId val="852237944"/>
+        <c:axId val="998598552"/>
+        <c:axId val="998604680"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="852231944"/>
+        <c:axId val="998598552"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2315,12 +2298,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="852237944"/>
+        <c:crossAx val="998604680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="852237944"/>
+        <c:axId val="998604680"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2358,7 +2341,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="852231944"/>
+        <c:crossAx val="998598552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2418,7 +2401,7 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="triangle"/>
-            <c:size val="8"/>
+            <c:size val="10"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent3">
@@ -2498,7 +2481,7 @@
           </c:tx>
           <c:marker>
             <c:symbol val="square"/>
-            <c:size val="8"/>
+            <c:size val="10"/>
           </c:marker>
           <c:xVal>
             <c:numRef>
@@ -2577,7 +2560,7 @@
           </c:tx>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="8"/>
+            <c:size val="10"/>
           </c:marker>
           <c:xVal>
             <c:numRef>
@@ -2640,11 +2623,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="852277208"/>
-        <c:axId val="852287304"/>
+        <c:axId val="998633528"/>
+        <c:axId val="998653688"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="852277208"/>
+        <c:axId val="998633528"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2681,12 +2664,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="852287304"/>
+        <c:crossAx val="998653688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="852287304"/>
+        <c:axId val="998653688"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2724,7 +2707,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="852277208"/>
+        <c:crossAx val="998633528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2784,7 +2767,7 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="triangle"/>
-            <c:size val="8"/>
+            <c:size val="10"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent3">
@@ -2861,7 +2844,7 @@
           </c:tx>
           <c:marker>
             <c:symbol val="square"/>
-            <c:size val="8"/>
+            <c:size val="10"/>
           </c:marker>
           <c:xVal>
             <c:numRef>
@@ -2940,7 +2923,7 @@
           </c:tx>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="8"/>
+            <c:size val="10"/>
           </c:marker>
           <c:xVal>
             <c:numRef>
@@ -3003,11 +2986,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="852329656"/>
-        <c:axId val="852339752"/>
+        <c:axId val="998687992"/>
+        <c:axId val="998708296"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="852329656"/>
+        <c:axId val="998687992"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -3044,12 +3027,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="852339752"/>
+        <c:crossAx val="998708296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="852339752"/>
+        <c:axId val="998708296"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -3087,7 +3070,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="852329656"/>
+        <c:crossAx val="998687992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3148,7 +3131,7 @@
           </c:tx>
           <c:marker>
             <c:symbol val="square"/>
-            <c:size val="8"/>
+            <c:size val="10"/>
           </c:marker>
           <c:xVal>
             <c:numRef>
@@ -3221,7 +3204,7 @@
           </c:tx>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="8"/>
+            <c:size val="10"/>
           </c:marker>
           <c:xVal>
             <c:numRef>
@@ -3284,11 +3267,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="852376856"/>
-        <c:axId val="852389320"/>
+        <c:axId val="998736008"/>
+        <c:axId val="998744168"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="852376856"/>
+        <c:axId val="998736008"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -3325,12 +3308,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="852389320"/>
+        <c:crossAx val="998744168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="852389320"/>
+        <c:axId val="998744168"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -3368,7 +3351,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="852376856"/>
+        <c:crossAx val="998736008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3922,11 +3905,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="865110152"/>
-        <c:axId val="865115928"/>
+        <c:axId val="998849672"/>
+        <c:axId val="998855448"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="865110152"/>
+        <c:axId val="998849672"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -3952,13 +3935,13 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="865115928"/>
+        <c:crossAx val="998855448"/>
         <c:crossesAt val="0.001"/>
         <c:crossBetween val="midCat"/>
         <c:minorUnit val="10.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="865115928"/>
+        <c:axId val="998855448"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -3985,7 +3968,7 @@
         <c:numFmt formatCode="0.E+00" sourceLinked="0"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="865110152"/>
+        <c:crossAx val="998849672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4453,11 +4436,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="865150808"/>
-        <c:axId val="865156808"/>
+        <c:axId val="998890232"/>
+        <c:axId val="998896232"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="865150808"/>
+        <c:axId val="998890232"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -4483,12 +4466,12 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="865156808"/>
+        <c:crossAx val="998896232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="865156808"/>
+        <c:axId val="998896232"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -4515,7 +4498,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="865150808"/>
+        <c:crossAx val="998890232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4833,11 +4816,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="jj_1" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="jjj" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="jjj" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="jj_1" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5177,235 +5160,235 @@
   <sheetData>
     <row r="1" spans="1:67">
       <c r="A1" t="s">
-        <v>81</v>
+        <v>12</v>
       </c>
       <c r="N1" t="s">
-        <v>69</v>
+        <v>0</v>
       </c>
       <c r="T1" t="s">
-        <v>80</v>
+        <v>11</v>
       </c>
       <c r="Z1" t="s">
-        <v>77</v>
+        <v>8</v>
       </c>
       <c r="AL1" t="s">
-        <v>78</v>
+        <v>9</v>
       </c>
       <c r="AX1" t="s">
-        <v>79</v>
+        <v>10</v>
       </c>
       <c r="BD1" t="s">
-        <v>63</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:67">
       <c r="A2" t="s">
-        <v>82</v>
+        <v>13</v>
       </c>
       <c r="N2" t="s">
-        <v>66</v>
+        <v>89</v>
       </c>
       <c r="P2" t="s">
-        <v>72</v>
+        <v>3</v>
       </c>
       <c r="BD2" t="s">
-        <v>66</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:67">
       <c r="C3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" t="s">
+        <v>41</v>
+      </c>
+      <c r="O3" t="s">
+        <v>35</v>
+      </c>
+      <c r="S3" t="s">
+        <v>5</v>
+      </c>
+      <c r="U3" t="s">
+        <v>6</v>
+      </c>
+      <c r="V3" t="s">
+        <v>7</v>
+      </c>
+      <c r="W3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AR3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AU3" t="s">
         <v>17</v>
       </c>
-      <c r="F3" t="s">
-        <v>71</v>
-      </c>
-      <c r="G3" t="s">
-        <v>73</v>
-      </c>
-      <c r="I3" t="s">
-        <v>18</v>
-      </c>
-      <c r="O3" t="s">
-        <v>12</v>
-      </c>
-      <c r="S3" t="s">
-        <v>74</v>
-      </c>
-      <c r="U3" t="s">
-        <v>75</v>
-      </c>
-      <c r="V3" t="s">
-        <v>76</v>
-      </c>
-      <c r="W3" t="s">
-        <v>76</v>
-      </c>
-      <c r="AM3" t="s">
-        <v>6</v>
-      </c>
-      <c r="AR3" t="s">
-        <v>85</v>
-      </c>
-      <c r="AU3" t="s">
-        <v>86</v>
-      </c>
       <c r="BB3" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="BJ3" t="s">
-        <v>83</v>
+        <v>14</v>
       </c>
       <c r="BK3" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
       <c r="BL3" t="s">
-        <v>83</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:67">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="B4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" t="s">
+        <v>91</v>
+      </c>
+      <c r="F4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" t="s">
+        <v>46</v>
+      </c>
+      <c r="J4" t="s">
+        <v>47</v>
+      </c>
+      <c r="K4" t="s">
+        <v>83</v>
+      </c>
+      <c r="N4" t="s">
+        <v>90</v>
+      </c>
+      <c r="O4" t="s">
+        <v>36</v>
+      </c>
+      <c r="P4" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>85</v>
+      </c>
+      <c r="R4" t="s">
+        <v>91</v>
+      </c>
+      <c r="S4" t="s">
+        <v>21</v>
+      </c>
+      <c r="U4" t="s">
+        <v>24</v>
+      </c>
+      <c r="V4" t="s">
+        <v>25</v>
+      </c>
+      <c r="W4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>90</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>85</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>90</v>
+      </c>
+      <c r="AM4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AN4" t="s">
+        <v>30</v>
+      </c>
+      <c r="AO4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AP4" t="s">
+        <v>91</v>
+      </c>
+      <c r="AR4" t="s">
+        <v>27</v>
+      </c>
+      <c r="AS4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AT4" t="s">
+        <v>88</v>
+      </c>
+      <c r="AU4" t="s">
+        <v>32</v>
+      </c>
+      <c r="AV4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AW4" t="s">
+        <v>34</v>
+      </c>
+      <c r="AX4" t="s">
+        <v>90</v>
+      </c>
+      <c r="AY4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AZ4" t="s">
+        <v>84</v>
+      </c>
+      <c r="BB4" t="s">
+        <v>46</v>
+      </c>
+      <c r="BC4" t="s">
+        <v>47</v>
+      </c>
+      <c r="BD4" t="s">
+        <v>90</v>
+      </c>
+      <c r="BE4" t="s">
+        <v>18</v>
+      </c>
+      <c r="BF4" t="s">
         <v>19</v>
       </c>
-      <c r="C4" t="s">
+      <c r="BG4" t="s">
         <v>20</v>
       </c>
-      <c r="D4" t="s">
+      <c r="BH4" t="s">
+        <v>91</v>
+      </c>
+      <c r="BJ4" t="s">
+        <v>23</v>
+      </c>
+      <c r="BK4" t="s">
         <v>21</v>
       </c>
-      <c r="E4" t="s">
-        <v>68</v>
-      </c>
-      <c r="F4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" t="s">
-        <v>91</v>
-      </c>
-      <c r="I4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J4" t="s">
-        <v>24</v>
-      </c>
-      <c r="K4" t="s">
-        <v>60</v>
-      </c>
-      <c r="N4" t="s">
-        <v>67</v>
-      </c>
-      <c r="O4" t="s">
-        <v>13</v>
-      </c>
-      <c r="P4" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>62</v>
-      </c>
-      <c r="R4" t="s">
-        <v>68</v>
-      </c>
-      <c r="S4" t="s">
-        <v>90</v>
-      </c>
-      <c r="U4" t="s">
-        <v>1</v>
-      </c>
-      <c r="V4" t="s">
-        <v>2</v>
-      </c>
-      <c r="W4" t="s">
-        <v>3</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>67</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>14</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>15</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>62</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>68</v>
-      </c>
-      <c r="AL4" t="s">
-        <v>67</v>
-      </c>
-      <c r="AM4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AN4" t="s">
-        <v>7</v>
-      </c>
-      <c r="AO4" t="s">
-        <v>8</v>
-      </c>
-      <c r="AP4" t="s">
-        <v>68</v>
-      </c>
-      <c r="AR4" t="s">
-        <v>4</v>
-      </c>
-      <c r="AS4" t="s">
-        <v>64</v>
-      </c>
-      <c r="AT4" t="s">
-        <v>65</v>
-      </c>
-      <c r="AU4" t="s">
-        <v>9</v>
-      </c>
-      <c r="AV4" t="s">
-        <v>10</v>
-      </c>
-      <c r="AW4" t="s">
-        <v>11</v>
-      </c>
-      <c r="AX4" t="s">
-        <v>67</v>
-      </c>
-      <c r="AY4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AZ4" t="s">
-        <v>61</v>
-      </c>
-      <c r="BB4" t="s">
-        <v>23</v>
-      </c>
-      <c r="BC4" t="s">
-        <v>24</v>
-      </c>
-      <c r="BD4" t="s">
-        <v>67</v>
-      </c>
-      <c r="BE4" t="s">
-        <v>87</v>
-      </c>
-      <c r="BF4" t="s">
-        <v>88</v>
-      </c>
-      <c r="BG4" t="s">
-        <v>89</v>
-      </c>
-      <c r="BH4" t="s">
-        <v>68</v>
-      </c>
-      <c r="BJ4" t="s">
-        <v>0</v>
-      </c>
-      <c r="BK4" t="s">
-        <v>90</v>
-      </c>
       <c r="BL4" t="s">
-        <v>91</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:67">
@@ -6548,7 +6531,7 @@
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3" t="s">
-        <v>70</v>
+        <v>1</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -6563,7 +6546,7 @@
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="1" t="s">
-        <v>70</v>
+        <v>1</v>
       </c>
       <c r="R12" s="1"/>
       <c r="BD12">
@@ -10561,70 +10544,70 @@
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="G1" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="M1" t="s">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="N1" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:18">
       <c r="B2" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="E2" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:18">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H3" t="s">
         <v>75</v>
       </c>
-      <c r="D3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F3" t="s">
-        <v>36</v>
-      </c>
-      <c r="H3" t="s">
-        <v>52</v>
-      </c>
       <c r="I3" t="s">
-        <v>44</v>
+        <v>67</v>
       </c>
       <c r="K3" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="L3" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
       <c r="N3" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="Q3" t="s">
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="R3" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:18">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="B4">
         <f>AVERAGE(B20:B24)</f>
@@ -10641,7 +10624,7 @@
         <v>0.41922300000000001</v>
       </c>
       <c r="G4" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="H4">
         <v>1.5562099999999999E-3</v>
@@ -10658,7 +10641,7 @@
         <v>0.36984467309977737</v>
       </c>
       <c r="M4" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="N4">
         <v>4.6457999999999997E-4</v>
@@ -10677,7 +10660,7 @@
     </row>
     <row r="5" spans="1:18">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="B5">
         <f>AVERAGE(B26:B30)</f>
@@ -10694,7 +10677,7 @@
         <v>14.619300000000001</v>
       </c>
       <c r="G5" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="H5">
         <v>4.0733200000000001E-3</v>
@@ -10711,7 +10694,7 @@
         <v>14.262968770746806</v>
       </c>
       <c r="M5" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="N5">
         <v>1.9678310000000001E-2</v>
@@ -10730,7 +10713,7 @@
     </row>
     <row r="6" spans="1:18">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="B6">
         <f>AVERAGE(B32:B36)</f>
@@ -10747,7 +10730,7 @@
         <v>0.24682000000000001</v>
       </c>
       <c r="G6" t="s">
-        <v>55</v>
+        <v>78</v>
       </c>
       <c r="H6">
         <v>3.2574150000000003E-2</v>
@@ -10764,7 +10747,7 @@
         <v>43.650122067276612</v>
       </c>
       <c r="M6" t="s">
-        <v>42</v>
+        <v>65</v>
       </c>
       <c r="N6">
         <v>5.31E-4</v>
@@ -10783,7 +10766,7 @@
     </row>
     <row r="7" spans="1:18">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="B7">
         <f>AVERAGE(B38:B42)</f>
@@ -10800,7 +10783,7 @@
         <v>0.179397</v>
       </c>
       <c r="G7" t="s">
-        <v>56</v>
+        <v>79</v>
       </c>
       <c r="H7">
         <v>1.070432E-2</v>
@@ -10817,7 +10800,7 @@
         <v>5.7718544876048199</v>
       </c>
       <c r="M7" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="N7" s="6">
         <v>4.9336999999999999E-5</v>
@@ -10836,7 +10819,7 @@
     </row>
     <row r="8" spans="1:18">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>54</v>
       </c>
       <c r="B8">
         <f>AVERAGE(B44:B48)</f>
@@ -10853,7 +10836,7 @@
         <v>0.22862499999999999</v>
       </c>
       <c r="G8" t="s">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="H8">
         <v>3.4496720000000002E-2</v>
@@ -10872,7 +10855,7 @@
     </row>
     <row r="9" spans="1:18">
       <c r="G9" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="H9">
         <v>5.296878E-2</v>
@@ -10891,13 +10874,13 @@
     </row>
     <row r="10" spans="1:18">
       <c r="B10" t="s">
-        <v>50</v>
+        <v>73</v>
       </c>
       <c r="E10" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="G10" t="s">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="H10">
         <v>2.1985099999999999E-3</v>
@@ -10916,24 +10899,24 @@
     </row>
     <row r="11" spans="1:18">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="C11" t="s">
-        <v>75</v>
+        <v>6</v>
       </c>
       <c r="E11" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="F11" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:18">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="B12">
         <f>B4/6</f>
@@ -10954,7 +10937,7 @@
     </row>
     <row r="13" spans="1:18">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="B13">
         <f t="shared" ref="B13" si="4">B5/6</f>
@@ -11003,7 +10986,7 @@
     </row>
     <row r="14" spans="1:18">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="B14">
         <f t="shared" ref="B14" si="5">B6/6</f>
@@ -11044,7 +11027,7 @@
     </row>
     <row r="15" spans="1:18">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="B15">
         <f t="shared" ref="B15" si="6">B7/6</f>
@@ -11077,7 +11060,7 @@
     </row>
     <row r="16" spans="1:18">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>54</v>
       </c>
       <c r="B16">
         <f t="shared" ref="B16" si="7">B8/6</f>
@@ -11657,7 +11640,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>